<commit_message>
Add: statics, activators, sounds, unique containers
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D8BE7D-6A8E-497A-93AC-422F7E8E848B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26E87F5-EB37-428F-A532-3CF1DCE2D117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="7" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Door</t>
   </si>
   <si>
-    <t>tlvoat_secret_wall</t>
-  </si>
-  <si>
     <t>I met a woman, Aryasi Othral, outside her family tomb. She asked me to clear the spirits inside so that she can visit her ancesters. I turned her down.</t>
   </si>
   <si>
@@ -236,12 +233,6 @@
     <t>Let Aryasi know</t>
   </si>
   <si>
-    <t>tlvoat_relative_ashes1</t>
-  </si>
-  <si>
-    <t>tlvoat_relative_ashes2</t>
-  </si>
-  <si>
     <t>Misc</t>
   </si>
   <si>
@@ -275,21 +266,12 @@
     <t>tlvoat_skeleton_archer</t>
   </si>
   <si>
-    <t>tlvoat_shrine_unique</t>
-  </si>
-  <si>
     <t>tlvoat_load_door_unique</t>
   </si>
   <si>
     <t>CONT</t>
   </si>
   <si>
-    <t>tlvoat_urn_lletho_othral_unique</t>
-  </si>
-  <si>
-    <t>tlvoat_urn_jathys_othral_unique</t>
-  </si>
-  <si>
     <t>Urn Labelled "Jathys Othral"</t>
   </si>
   <si>
@@ -299,9 +281,6 @@
     <t>Urn Labelled "Uravasa Othral"</t>
   </si>
   <si>
-    <t>tlvoat_urn_uravasa_unique</t>
-  </si>
-  <si>
     <t>tlvoat_uravasa_ghost</t>
   </si>
   <si>
@@ -354,6 +333,39 @@
   </si>
   <si>
     <t>tlvoat_aryasi Othral</t>
+  </si>
+  <si>
+    <t>tlvoat_urn_lletho_uni</t>
+  </si>
+  <si>
+    <t>tlvoat_urn_jathys_uni</t>
+  </si>
+  <si>
+    <t>tlvoat_urn_uravasa_uni</t>
+  </si>
+  <si>
+    <t>Urn Labelled "Tandram Othral"</t>
+  </si>
+  <si>
+    <t>tlvoat_urn_tandram_uni</t>
+  </si>
+  <si>
+    <t>tlvoat_lletho_ashes_unique</t>
+  </si>
+  <si>
+    <t>tlvoat_jathys_ashes_unique</t>
+  </si>
+  <si>
+    <t>tlvoat_uravasa_ashes_unique</t>
+  </si>
+  <si>
+    <t>Ashes of Uravasa Othral</t>
+  </si>
+  <si>
+    <t>tlvoat_othral_secret_wall</t>
+  </si>
+  <si>
+    <t>tlvoat_othral_shrine_unique</t>
   </si>
 </sst>
 </file>
@@ -888,7 +900,7 @@
   <dimension ref="A2:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,7 +925,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -1095,13 +1107,13 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1112,13 +1124,13 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1129,13 +1141,13 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1146,13 +1158,13 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1163,13 +1175,13 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1180,13 +1192,13 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1197,13 +1209,13 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9">
         <v>60</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1214,16 +1226,16 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>70</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
         <v>48</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1234,16 +1246,16 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>71</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
         <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1254,16 +1266,16 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12">
         <v>200</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1274,16 +1286,16 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13">
         <v>300</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1321,7 +1333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
   <dimension ref="A2:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1358,10 +1370,10 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1369,13 +1381,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1447,11 +1459,11 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:D32 E3">
+  <conditionalFormatting sqref="E3 B3:D32">
     <cfRule type="expression" dxfId="10" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -1510,16 +1522,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1527,16 +1539,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1544,20 +1556,20 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:D32 E3:E5">
+  <conditionalFormatting sqref="E3:E5 B3:D32">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -1588,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65134921-D347-4BBE-A2AC-6E1606FA8DED}">
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,44 +1625,44 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1658,13 +1670,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1672,17 +1684,31 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:D33">
+  <conditionalFormatting sqref="B3:D34">
     <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -1691,7 +1717,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B1:B1048576" xr:uid="{6A29AA8E-4E7A-4B79-B0F8-675FB012FEDC}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B1:B3 B4:B1048576" xr:uid="{6A29AA8E-4E7A-4B79-B0F8-675FB012FEDC}">
       <formula1>31</formula1>
     </dataValidation>
   </dataValidations>
@@ -1703,7 +1729,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A1048576</xm:sqref>
+          <xm:sqref>A1:A3 A4:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1713,10 +1739,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F94C72C-6EBC-4A19-A0BC-385E0AA67890}">
-  <dimension ref="A2:E8"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1741,7 +1767,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -1752,10 +1778,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -1763,13 +1789,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -1777,57 +1803,74 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E6:E8 B3:D32">
+  <conditionalFormatting sqref="B3:D33 E6:E9">
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -1849,7 +1892,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D100</xm:sqref>
+          <xm:sqref>D3:D101</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1891,7 +1934,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1900,7 +1943,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1908,7 +1951,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1917,7 +1960,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1925,16 +1968,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1942,16 +1985,16 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: loot and unique items
* Update: replace area by secret entrance with preaching place
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26E87F5-EB37-428F-A532-3CF1DCE2D117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC986325-70B8-4B6C-88E4-4F3B502FE8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="7" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="5" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -287,30 +287,15 @@
     <t>Uravasa Othral's Ghost</t>
   </si>
   <si>
-    <t>tlvoat_gauntlet_r_bonemold</t>
-  </si>
-  <si>
-    <t>Othral Fine R. Bonemold Gauntlet</t>
-  </si>
-  <si>
     <t>Armour</t>
   </si>
   <si>
-    <t>tlvoat_chitin_sword</t>
-  </si>
-  <si>
     <t>Othral Family Blade</t>
   </si>
   <si>
     <t>Weapon</t>
   </si>
   <si>
-    <t>tlvoat_gauntlet_l_bonemold</t>
-  </si>
-  <si>
-    <t>Othral Fine L. Bonemold Gauntlet</t>
-  </si>
-  <si>
     <t>lvl 20</t>
   </si>
   <si>
@@ -366,6 +351,21 @@
   </si>
   <si>
     <t>tlvoat_othral_shrine_unique</t>
+  </si>
+  <si>
+    <t>tlvoat_chitin_sword_unique</t>
+  </si>
+  <si>
+    <t>tlvoat_gauntlet_r_bone_unique</t>
+  </si>
+  <si>
+    <t>tlvoat_gauntlet_l_bone_unique</t>
+  </si>
+  <si>
+    <t>Othral Family Right Bracer</t>
+  </si>
+  <si>
+    <t>Othral Family Left Bracer</t>
   </si>
 </sst>
 </file>
@@ -1370,10 +1370,10 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1381,13 +1381,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1459,7 +1459,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1496,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E963F2BA-EA95-4418-AB9C-44FAC2775617}">
   <dimension ref="A2:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1531,7 +1531,7 @@
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1548,7 +1548,7 @@
         <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1565,7 +1565,7 @@
         <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1603,7 +1603,7 @@
   <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1628,7 +1628,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>63</v>
@@ -1642,7 +1642,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -1656,10 +1656,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
         <v>62</v>
@@ -1667,44 +1667,44 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
         <v>80</v>
-      </c>
-      <c r="C6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1741,7 +1741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F94C72C-6EBC-4A19-A0BC-385E0AA67890}">
   <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1781,7 +1781,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -1792,7 +1792,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
         <v>59</v>
@@ -1806,7 +1806,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
         <v>76</v>
@@ -1823,7 +1823,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
         <v>75</v>
@@ -1840,10 +1840,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -1857,7 +1857,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
         <v>77</v>
@@ -1960,7 +1960,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update: defined initial dialogue lines
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDC8C67-5FD1-430A-902D-ECB7E3DF0312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CDFF2F-C252-4C01-85BC-C3E70B60597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" firstSheet="2" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="184">
   <si>
     <t>Name</t>
   </si>
@@ -303,9 +303,6 @@
     <t>lvl 5</t>
   </si>
   <si>
-    <t>Lvl 4</t>
-  </si>
-  <si>
     <t>OnActivate: ForceGreeting Aryasi if not yet spoken, aryasi.hasPCAttemptEnter to 1</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>Head inside, speak to Aryasi, help</t>
   </si>
   <si>
-    <t>ask for help, ask if PC changed mind, ask if PC cleared tomb anyway, malePC nude, femalePC nude</t>
-  </si>
-  <si>
     <t>Update Aryasi, is clear</t>
   </si>
   <si>
@@ -453,12 +447,6 @@
     <t>p2 2 greetings:</t>
   </si>
   <si>
-    <t>completed escort</t>
-  </si>
-  <si>
-    <t>asks if PC found secret area</t>
-  </si>
-  <si>
     <t>clear the tomb</t>
   </si>
   <si>
@@ -487,6 +475,129 @@
   </si>
   <si>
     <t>PC Clothes &lt;= 0, PC not Argonian, PC not Kajiit, PC isFemale = 1</t>
+  </si>
+  <si>
+    <t>Goodbye</t>
+  </si>
+  <si>
+    <t>Please cover up. I'm not talking unless you cover yourself.</t>
+  </si>
+  <si>
+    <t>Oh, oh please cover yourself! You're rather distracting!</t>
+  </si>
+  <si>
+    <t>Lvl 2</t>
+  </si>
+  <si>
+    <t>something about family</t>
+  </si>
+  <si>
+    <t>Oh, are you going in? Could you help to clear the tomb?</t>
+  </si>
+  <si>
+    <t>Oh hello there! Could I ask for help to clear the tomb?</t>
+  </si>
+  <si>
+    <t>ask for help, ask when PC attempted to go in, ask if PC changed mind, ask if PC cleared tomb anyway, malePC nude, femalePC nude</t>
+  </si>
+  <si>
+    <t>Talked to PC = 1</t>
+  </si>
+  <si>
+    <t>Hello again %PCName, are you able to help me to clear the tomb?</t>
+  </si>
+  <si>
+    <t>Ah, %PCName. Did you clear the tomb?</t>
+  </si>
+  <si>
+    <t>Talked to PC = 1, hasPCEnteredBefore = 1</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &lt; not updated</t>
+  </si>
+  <si>
+    <t>How is it going? Have you cleared the tomb?</t>
+  </si>
+  <si>
+    <t>Priest %PCName, I do not wish to trouble you, but have you been able to clear the tomb?</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &gt;= updated, unable to clear</t>
+  </si>
+  <si>
+    <t>I don't know what it is that I'm feeling. A loss that's deeper than what I felt many years ago.</t>
+  </si>
+  <si>
+    <t>It feels… colder in here than I remember. The spirits of my family are silent to me.</t>
+  </si>
+  <si>
+    <t>The spirits of my family remain silent.</t>
+  </si>
+  <si>
+    <t>I guess I was never really an Othral. I should stopped thinking of myself as one when I ran away.</t>
+  </si>
+  <si>
+    <t>Goodbye?</t>
+  </si>
+  <si>
+    <t>asks if PC found secret area, asks if PC found secret area (temple)</t>
+  </si>
+  <si>
+    <t>Hey %PCName, have you found anything?</t>
+  </si>
+  <si>
+    <t>%PCRank, I do not wish to get in your way, but if there's anything I can do to help please ask.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &gt;= updated</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &gt;= updated, refused to find secret</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &gt;= find secret</t>
+  </si>
+  <si>
+    <t>escorting, completed escort</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == escorting</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == escorting success</t>
+  </si>
+  <si>
+    <t>Don't worry, I'm keeping up!</t>
+  </si>
+  <si>
+    <t>Ah! This is her! Oh thank you, thank you so much for taking me to my grandmother. Please, leave me for a while so that I may speak with her spirit.</t>
+  </si>
+  <si>
+    <t>Yes, so that I may speak with the spirits of my family. I wish to settle some things. Would you be able to help with this?</t>
+  </si>
+  <si>
+    <t>Have you changed your mind?</t>
+  </si>
+  <si>
+    <t>Yes, I saw that you when in. Did you clear it anyway?</t>
+  </si>
+  <si>
+    <t>isCleared = 1</t>
+  </si>
+  <si>
+    <t>isCleared = 0</t>
+  </si>
+  <si>
+    <t>Choice</t>
+  </si>
+  <si>
+    <t>Ah, %PCName! Is it safe to go in?</t>
+  </si>
+  <si>
+    <t>Yes, I saw that you when in. Did you clear it anyway? You seem rather dirty compared to earlier.</t>
+  </si>
+  <si>
+    <t>Ah, %PCName! Is it safe to go in? You seem rather dirty compared to earlier.</t>
   </si>
 </sst>
 </file>
@@ -559,6 +670,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="8" tint="0.39994506668294322"/>
@@ -575,20 +700,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1157,7 +1268,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1196,13 +1307,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:E32">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$C3="Yes"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1227,7 +1338,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1579,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B243748A-4AED-4508-9429-6EAB26E82FD6}">
   <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,223 +1708,228 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
         <v>121</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" t="s">
         <v>123</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>124</v>
-      </c>
-      <c r="F7" t="s">
-        <v>125</v>
-      </c>
-      <c r="G7" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" t="s">
         <v>130</v>
-      </c>
-      <c r="C20" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>138</v>
+      <c r="C26" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>138</v>
+      <c r="C28" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1823,10 +1939,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F6"/>
+  <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1863,10 +1979,16 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" t="s">
         <v>143</v>
       </c>
       <c r="F3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1877,18 +1999,30 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" t="s">
         <v>143</v>
       </c>
       <c r="F4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>140</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="F5" t="s">
         <v>87</v>
@@ -1898,19 +2032,352 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>140</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" t="s">
+        <v>180</v>
+      </c>
+      <c r="F21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24" t="s">
+        <v>180</v>
+      </c>
+      <c r="F24" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:F32">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1940,7 +2407,7 @@
   <dimension ref="A2:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1974,15 +2441,15 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3 B3:D32">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2085,10 +2552,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E5 B3:D32">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2143,7 +2610,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
         <v>63</v>
@@ -2157,7 +2624,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -2171,10 +2638,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
         <v>96</v>
-      </c>
-      <c r="C5" t="s">
-        <v>97</v>
       </c>
       <c r="D5" t="s">
         <v>62</v>
@@ -2185,10 +2652,10 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
         <v>80</v>
@@ -2199,10 +2666,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
         <v>80</v>
@@ -2213,7 +2680,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>81</v>
@@ -2224,10 +2691,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D34">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2296,7 +2763,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -2307,7 +2774,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
         <v>59</v>
@@ -2321,7 +2788,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>76</v>
@@ -2338,7 +2805,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
         <v>75</v>
@@ -2355,10 +2822,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -2372,7 +2839,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
         <v>77</v>
@@ -2386,10 +2853,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D33 E6:E9">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add: cleaner journal entries and flow, end dialogue topic lines
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CDFF2F-C252-4C01-85BC-C3E70B60597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64536A98-8B1C-4924-88C5-DFC37E65FBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="3" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="2" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="198">
   <si>
     <t>Name</t>
   </si>
@@ -153,51 +153,18 @@
     <t>Door</t>
   </si>
   <si>
-    <t>I met a woman, Aryasi Othral, outside her family tomb. She asked me to clear the spirits inside so that she can visit her ancesters. I turned her down.</t>
-  </si>
-  <si>
-    <t>I met Aryasi Othral camped outside of her family's tomb. She wants to pay her respects, but estrangment in life has meant that the guardian spirits are hostile even to her. She asked me to clear them out so that she can enter.</t>
-  </si>
-  <si>
-    <t>Met Othral/attempted to enter tomb, turned her down</t>
-  </si>
-  <si>
-    <t>Met Othral/attempted to enter tomb, accepted</t>
-  </si>
-  <si>
-    <t>I returned to Othral to accept her offer to clear the hostile spirits in her family tomb.</t>
-  </si>
-  <si>
-    <t>Spoke prior, return to complete</t>
-  </si>
-  <si>
-    <t>Cleared the tomb</t>
-  </si>
-  <si>
-    <t>I have cleared the Othral Ancestral Tomb of hostile undead. I shall let Aryasi Othral that it's safe for her to enter.</t>
-  </si>
-  <si>
-    <t>I let Othral know it's safe for her to enter to pay her respects. She has gone in and should have had some time to herself. I should check up on her.</t>
-  </si>
-  <si>
     <t>Updated Othral, she's moved, fade in/out</t>
   </si>
   <si>
     <t>Met grandmother's spirit</t>
   </si>
   <si>
-    <t>I've let Aryasi Othral know that I met her grandmother's spirit and she expressed wanting to speak to her. She wants me to take her there.</t>
-  </si>
-  <si>
     <t>Lead Aryasi, they've spoken, she expressed her thanks</t>
   </si>
   <si>
     <t>FIN</t>
   </si>
   <si>
-    <t>Aryasi thanked me for giving her the opportunity to speak with her grandmother's spirit. She gave me a reward of X</t>
-  </si>
-  <si>
     <t>Aryasi thanked me for giving her the opportunity to speak with her grandmother's spirit. She offered a reward, but I turned her down.</t>
   </si>
   <si>
@@ -207,15 +174,6 @@
     <t>PC killed quest giver, at any point</t>
   </si>
   <si>
-    <t>I met grandmother in a secret section in Othral Ancestral Tomb. She senses her grandchild's presence and wants to speak to her. I should let Aryasi Othral know.</t>
-  </si>
-  <si>
-    <t>I banished Aryasi's grandmother's ghost. Aryasi is angry and distrought that she will never have the opportuntiy to speak with her ancester. She will no longer speak with me.</t>
-  </si>
-  <si>
-    <t>PC killed ghost, updated Aryasi</t>
-  </si>
-  <si>
     <t>tlvoat_aryasi_othral_script</t>
   </si>
   <si>
@@ -598,6 +556,90 @@
   </si>
   <si>
     <t>Ah, %PCName! Is it safe to go in? You seem rather dirty compared to earlier.</t>
+  </si>
+  <si>
+    <t>brief overview of family history, joyous she can reconnect</t>
+  </si>
+  <si>
+    <t>initial speculation (yet revealed), initial speculation (revealed), ask if found yet (acutal), ask if found yet (not yet)</t>
+  </si>
+  <si>
+    <t>(Yes, no), (already found, no), (Yes, (Lie) none), (There is none, not yet)</t>
+  </si>
+  <si>
+    <t>Thank you again for making it safe for me</t>
+  </si>
+  <si>
+    <t>Thank you again %PCName for allowing me to enter my family's tomb to speak with them. You are an exemplar for the Temple.</t>
+  </si>
+  <si>
+    <t>isPCInTemple = 1</t>
+  </si>
+  <si>
+    <t>I haven't spoken with them in so long, and I thought that they would want to speak with me given how long it's been and that I'm the last member of the family. But I thought wrong. The only one who I ever really got on with was my grandmother, but I can't find her. I used to suspect that there is a hidden section of the tomb.</t>
+  </si>
+  <si>
+    <t>Yes! I'm so happy that I've been able to reconnect with my grandmother.</t>
+  </si>
+  <si>
+    <t>Whenever I asked my parents they always denied it, but every time my mother expressed missing grandmother she would come to the tomb. Once I sneaked after her and she prayed at the shrine, but then I was caught and couldn't find anything else.</t>
+  </si>
+  <si>
+    <t>hasPCRevealedSecret = 0</t>
+  </si>
+  <si>
+    <t>hasPCRevealedSecret = 1</t>
+  </si>
+  <si>
+    <t>Have you found it yet?</t>
+  </si>
+  <si>
+    <t>hasPCRevealedSecret = 0, journal == offered to find</t>
+  </si>
+  <si>
+    <t>hasPCRevealedSecret = 1, journal == offered to find</t>
+  </si>
+  <si>
+    <t>Met Othral/attempted to enter tomb, accepted/accepted after initial decline</t>
+  </si>
+  <si>
+    <t>I met Aryasi Othral outside of her family's tomb, who can't enter because the tomb's guardians are hostile towards her. I accepted her request to clear the tomb so that she can enter.</t>
+  </si>
+  <si>
+    <t>All guardians in Othral Ancestral Tomb have been dispatched. I will let Aryasi Othral know that she can safely enter.</t>
+  </si>
+  <si>
+    <t>All tomb guardians dead, was previously accepted</t>
+  </si>
+  <si>
+    <t>I let Aryasi Othral know that her family's tomb is safe. She's gone inside to speak with the spirits. I should return to check on her.</t>
+  </si>
+  <si>
+    <t>Let Aryasi know it's safe, both accepted before &amp; not accepted. Starts quest if latter</t>
+  </si>
+  <si>
+    <t>I lied to Aryasi Othral that her family's tomb is safe. The tomb's guardian's might end her.</t>
+  </si>
+  <si>
+    <t>Aryasi Othral mentioned that there might be a hidden section of Othral Ancestral Tomb. I offered to help find it.</t>
+  </si>
+  <si>
+    <t>Aryasi Othral wants me to lead her to where her grandmother has been laid to rest.</t>
+  </si>
+  <si>
+    <t>Let Aryasi know it's safe, both accepted before &amp; not accepted. Starts quest if latter. Kills Aryasi</t>
+  </si>
+  <si>
+    <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that she's had an opportunity to reconnect. She gave me a ring that was her grandmother's.</t>
+  </si>
+  <si>
+    <t>BEGIN</t>
+  </si>
+  <si>
+    <t>LATTER BEGIN</t>
+  </si>
+  <si>
+    <t>Aryasi Othral was killed by her family's guardian spirits.</t>
   </si>
 </sst>
 </file>
@@ -654,21 +696,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill>
@@ -788,6 +816,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -796,6 +838,20 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1242,7 +1298,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1251,7 +1307,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1259,7 +1315,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1268,7 +1324,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1276,16 +1332,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1293,27 +1349,27 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:E32">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$C3="Yes"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1429,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
-  <dimension ref="A2:F13"/>
+  <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,7 +1512,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1464,13 +1520,16 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>185</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>184</v>
+      </c>
+      <c r="F3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1481,16 +1540,16 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>186</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1498,16 +1557,19 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>188</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="F5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1515,13 +1577,16 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>193</v>
+      </c>
+      <c r="F6" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1532,13 +1597,13 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1549,13 +1614,13 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>192</v>
       </c>
       <c r="D8">
         <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1566,13 +1631,16 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>194</v>
       </c>
       <c r="D9">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1583,19 +1651,19 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D10">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1603,19 +1671,16 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>197</v>
       </c>
       <c r="D11">
-        <v>71</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>47</v>
+        <v>200</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1623,40 +1688,20 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D12">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13">
-        <v>300</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:E32 F10 F12">
+  <conditionalFormatting sqref="F3 F5:F6 F9 B3:E31 F11">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -1690,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B243748A-4AED-4508-9429-6EAB26E82FD6}">
   <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1708,228 +1753,237 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="H4" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="G7" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C22" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C23" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>147</v>
+        <v>133</v>
+      </c>
+      <c r="C25" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>138</v>
+        <v>124</v>
+      </c>
+      <c r="C27" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
+      </c>
+      <c r="D28" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1939,10 +1993,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F24"/>
+  <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1979,16 +2033,16 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1999,16 +2053,16 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="F4" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2019,13 +2073,13 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2036,13 +2090,13 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2053,13 +2107,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="F7" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2070,13 +2124,13 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" t="s">
         <v>140</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2087,13 +2141,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F9" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2104,13 +2158,13 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="F10" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2121,16 +2175,16 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="F11" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2141,13 +2195,13 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="F12" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2158,13 +2212,13 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2175,16 +2229,16 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E14" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="F14" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2195,13 +2249,13 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="F15" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2212,13 +2266,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="F16" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2229,16 +2283,16 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="F17" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2249,13 +2303,13 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="F18" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2266,13 +2320,13 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E19" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2283,13 +2337,13 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2300,16 +2354,16 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="E21" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F21" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2320,16 +2374,16 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="E22" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F22" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2340,16 +2394,16 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="E23" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F23" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2360,24 +2414,163 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
         <v>133</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D27" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E29" t="s">
+        <v>166</v>
+      </c>
+      <c r="F29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" t="s">
+        <v>166</v>
+      </c>
+      <c r="F30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E24" t="s">
-        <v>180</v>
-      </c>
-      <c r="F24" t="s">
-        <v>179</v>
+      <c r="E31" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E32" t="s">
+        <v>166</v>
+      </c>
+      <c r="F32" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F32">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="B3:F64">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2441,15 +2634,15 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3 B3:D32">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2504,16 +2697,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2521,16 +2714,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
         <v>70</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2538,24 +2731,24 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
         <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E5 B3:D32">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2610,13 +2803,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2624,13 +2817,13 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2638,13 +2831,13 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2652,13 +2845,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2666,13 +2859,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2680,21 +2873,21 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D34">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2749,7 +2942,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -2763,7 +2956,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -2774,10 +2967,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -2788,16 +2981,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2805,16 +2998,16 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2822,16 +3015,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2839,24 +3032,24 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D33 E6:E9">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$A3="Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add: shrine script with skill/faction checks
Update: rotated first two doors, removed door leading into shrine room
Update: Added column to far room
Update: adjusted lights in secret antechamber
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64536A98-8B1C-4924-88C5-DFC37E65FBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64ACDD-6914-480D-B3D9-E3969118459A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="2" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="200">
   <si>
     <t>Name</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Shrine of the Tribunal</t>
   </si>
   <si>
-    <t>OnActivate: if index &gt;= 30 or Wisdom(?) &gt;= 50 then MsgBox to pray, check it over, do nothing ELSE MsgBox to pray, do nothing</t>
-  </si>
-  <si>
     <t>Let Aryasi know</t>
   </si>
   <si>
@@ -640,6 +637,15 @@
   </si>
   <si>
     <t>Aryasi Othral was killed by her family's guardian spirits.</t>
+  </si>
+  <si>
+    <t>OnActivate: if index &gt;= 30 or Security &gt;= 60 or PCInTemple then MsgBox to pray, check it over, do nothing ELSE MsgBox to pray, do nothing</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits</t>
+  </si>
+  <si>
+    <t>tlvoat_othral_shrine_unique_scr</t>
   </si>
 </sst>
 </file>
@@ -696,7 +702,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="19">
     <dxf>
       <fill>
         <patternFill>
@@ -838,20 +844,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1268,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
   <dimension ref="A2:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1307,7 +1299,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1324,15 +1316,15 @@
         <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -1341,7 +1333,7 @@
         <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1349,16 +1341,16 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1449,10 +1441,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1487,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1520,16 +1512,16 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1540,13 +1532,13 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1557,16 +1549,16 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D5">
         <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1577,16 +1569,16 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D6">
         <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1597,7 +1589,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D7">
         <v>40</v>
@@ -1614,7 +1606,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -1631,13 +1623,13 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
@@ -1671,7 +1663,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -1701,7 +1693,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F3 F5:F6 F9 B3:E31 F11">
+  <conditionalFormatting sqref="F3 B3:E31 F5:F6 F9 F11">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -1753,237 +1745,237 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" t="s">
         <v>107</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>108</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>109</v>
-      </c>
-      <c r="G7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2033,16 +2025,16 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2053,16 +2045,16 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2073,13 +2065,13 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2090,13 +2082,13 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2107,13 +2099,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2124,13 +2116,13 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" t="s">
         <v>139</v>
-      </c>
-      <c r="F8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2141,13 +2133,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2158,13 +2150,13 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2175,16 +2167,16 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2195,13 +2187,13 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2212,13 +2204,13 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2229,16 +2221,16 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" t="s">
         <v>148</v>
       </c>
-      <c r="E14" t="s">
-        <v>149</v>
-      </c>
       <c r="F14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2249,13 +2241,13 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2266,13 +2258,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2283,16 +2275,16 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2303,13 +2295,13 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2320,13 +2312,13 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2337,13 +2329,13 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2354,16 +2346,16 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2374,16 +2366,16 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2394,16 +2386,16 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2414,16 +2406,16 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2434,13 +2426,13 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F25" t="s">
         <v>174</v>
-      </c>
-      <c r="F25" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2451,10 +2443,10 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2465,10 +2457,10 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2479,10 +2471,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2493,16 +2485,16 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E29" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" t="s">
         <v>178</v>
-      </c>
-      <c r="E29" t="s">
-        <v>166</v>
-      </c>
-      <c r="F29" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2513,16 +2505,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2533,16 +2525,16 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" t="s">
+        <v>165</v>
+      </c>
+      <c r="F31" t="s">
         <v>181</v>
-      </c>
-      <c r="E31" t="s">
-        <v>166</v>
-      </c>
-      <c r="F31" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2553,16 +2545,16 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2634,7 +2626,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2697,16 +2689,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2714,16 +2706,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2731,16 +2723,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2803,13 +2795,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2817,13 +2809,13 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2831,13 +2823,13 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
         <v>81</v>
       </c>
-      <c r="C5" t="s">
-        <v>82</v>
-      </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2845,13 +2837,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2859,13 +2851,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2873,13 +2865,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
         <v>67</v>
-      </c>
-      <c r="D8" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2917,7 +2909,7 @@
   <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2942,7 +2934,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -2956,7 +2948,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -2967,7 +2959,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
@@ -2981,16 +2973,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2998,16 +2990,16 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3015,16 +3007,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3032,16 +3024,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: exterior tomb to 2, -18
Add: Aryasi Othral
Add: tomb guardians
Fix: shrine script's poor flow
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64ACDD-6914-480D-B3D9-E3969118459A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F04D4B1-D2F6-4BE4-AFCB-F37555646280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="202">
   <si>
     <t>Name</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Let Aryasi know</t>
   </si>
   <si>
-    <t>Misc</t>
-  </si>
-  <si>
     <t>Ashes of Lletho Othral</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>tlvoat_skeleton_archer</t>
   </si>
   <si>
-    <t>tlvoat_load_door_unique</t>
-  </si>
-  <si>
     <t>CONT</t>
   </si>
   <si>
@@ -646,6 +640,18 @@
   </si>
   <si>
     <t>tlvoat_othral_shrine_unique_scr</t>
+  </si>
+  <si>
+    <t>Ingred</t>
+  </si>
+  <si>
+    <t>all tlvoat skeletons</t>
+  </si>
+  <si>
+    <t>tlvoat_skeleton_script</t>
+  </si>
+  <si>
+    <t>tlvoat_ex_othral_door_unique</t>
   </si>
 </sst>
 </file>
@@ -1258,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
-  <dimension ref="A2:E6"/>
+  <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1299,7 +1305,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1316,7 +1322,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1324,7 +1330,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -1333,7 +1339,7 @@
         <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1341,16 +1347,30 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>52</v>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1444,7 +1464,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1480,7 +1500,7 @@
   <dimension ref="A2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1506,90 +1526,90 @@
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D6">
         <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D7">
         <v>40</v>
@@ -1600,13 +1620,13 @@
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -1617,13 +1637,13 @@
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9">
         <v>100</v>
@@ -1637,7 +1657,7 @@
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -1657,13 +1677,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -1674,7 +1694,7 @@
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
@@ -1745,237 +1765,237 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
         <v>104</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" t="s">
         <v>106</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>107</v>
-      </c>
-      <c r="F7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
         <v>113</v>
-      </c>
-      <c r="C20" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" t="s">
         <v>118</v>
-      </c>
-      <c r="C23" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2025,16 +2045,16 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" t="s">
         <v>124</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2045,16 +2065,16 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2065,13 +2085,13 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2082,13 +2102,13 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2099,13 +2119,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2116,13 +2136,13 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2133,13 +2153,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2150,13 +2170,13 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2167,16 +2187,16 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2187,13 +2207,13 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2204,13 +2224,13 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2221,16 +2241,16 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2241,13 +2261,13 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2258,13 +2278,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2275,16 +2295,16 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2295,13 +2315,13 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2312,13 +2332,13 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2329,13 +2349,13 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2346,16 +2366,16 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2366,16 +2386,16 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F22" t="s">
         <v>162</v>
-      </c>
-      <c r="E22" t="s">
-        <v>165</v>
-      </c>
-      <c r="F22" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2386,16 +2406,16 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2406,16 +2426,16 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2426,13 +2446,13 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2443,10 +2463,10 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2457,10 +2477,10 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2471,10 +2491,10 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2485,16 +2505,16 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2505,16 +2525,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30" t="s">
+        <v>163</v>
+      </c>
+      <c r="F30" t="s">
         <v>177</v>
-      </c>
-      <c r="E30" t="s">
-        <v>165</v>
-      </c>
-      <c r="F30" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2525,16 +2545,16 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2545,16 +2565,16 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" t="s">
+        <v>163</v>
+      </c>
+      <c r="F32" t="s">
         <v>180</v>
-      </c>
-      <c r="E32" t="s">
-        <v>165</v>
-      </c>
-      <c r="F32" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2626,7 +2646,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2664,7 +2684,7 @@
   <dimension ref="A2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2689,50 +2709,50 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" t="s">
-        <v>55</v>
-      </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2770,7 +2790,7 @@
   <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2792,44 +2812,44 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2837,13 +2857,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
         <v>85</v>
       </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2851,13 +2871,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
-        <v>88</v>
-      </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2865,13 +2885,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2909,7 +2929,7 @@
   <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2931,10 +2951,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>201</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -2948,7 +2968,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -2959,7 +2979,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
@@ -2973,16 +2993,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2990,16 +3010,16 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3007,16 +3027,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3024,16 +3044,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: pre-quest and part 1 of quest dialogue and scripting
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F04D4B1-D2F6-4BE4-AFCB-F37555646280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5776B7A-EA06-4B6F-B5D8-8110FCC74408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="235">
   <si>
     <t>Name</t>
   </si>
@@ -255,12 +255,6 @@
     <t>OnActivate: ForceGreeting Aryasi if not yet spoken, aryasi.hasPCAttemptEnter to 1</t>
   </si>
   <si>
-    <t>Talked to PC = 0, hasPCAttemptEnter = 1</t>
-  </si>
-  <si>
-    <t>Talked to PC = 0, hasPCAttemptEnter = 0</t>
-  </si>
-  <si>
     <t>tlvoat_urn_lletho_uni</t>
   </si>
   <si>
@@ -429,54 +423,18 @@
     <t>Goodbye</t>
   </si>
   <si>
-    <t>Please cover up. I'm not talking unless you cover yourself.</t>
-  </si>
-  <si>
-    <t>Oh, oh please cover yourself! You're rather distracting!</t>
-  </si>
-  <si>
     <t>Lvl 2</t>
   </si>
   <si>
     <t>something about family</t>
   </si>
   <si>
-    <t>Oh, are you going in? Could you help to clear the tomb?</t>
-  </si>
-  <si>
-    <t>Oh hello there! Could I ask for help to clear the tomb?</t>
-  </si>
-  <si>
     <t>ask for help, ask when PC attempted to go in, ask if PC changed mind, ask if PC cleared tomb anyway, malePC nude, femalePC nude</t>
   </si>
   <si>
-    <t>Talked to PC = 1</t>
-  </si>
-  <si>
-    <t>Hello again %PCName, are you able to help me to clear the tomb?</t>
-  </si>
-  <si>
-    <t>Ah, %PCName. Did you clear the tomb?</t>
-  </si>
-  <si>
-    <t>Talked to PC = 1, hasPCEnteredBefore = 1</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal &lt; not updated</t>
-  </si>
-  <si>
-    <t>How is it going? Have you cleared the tomb?</t>
-  </si>
-  <si>
-    <t>Priest %PCName, I do not wish to trouble you, but have you been able to clear the tomb?</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal &gt;= updated, unable to clear</t>
   </si>
   <si>
-    <t>I don't know what it is that I'm feeling. A loss that's deeper than what I felt many years ago.</t>
-  </si>
-  <si>
     <t>It feels… colder in here than I remember. The spirits of my family are silent to me.</t>
   </si>
   <si>
@@ -528,24 +486,12 @@
     <t>Have you changed your mind?</t>
   </si>
   <si>
-    <t>Yes, I saw that you when in. Did you clear it anyway?</t>
-  </si>
-  <si>
-    <t>isCleared = 1</t>
-  </si>
-  <si>
-    <t>isCleared = 0</t>
-  </si>
-  <si>
     <t>Choice</t>
   </si>
   <si>
     <t>Ah, %PCName! Is it safe to go in?</t>
   </si>
   <si>
-    <t>Yes, I saw that you when in. Did you clear it anyway? You seem rather dirty compared to earlier.</t>
-  </si>
-  <si>
     <t>Ah, %PCName! Is it safe to go in? You seem rather dirty compared to earlier.</t>
   </si>
   <si>
@@ -561,9 +507,6 @@
     <t>Thank you again for making it safe for me</t>
   </si>
   <si>
-    <t>Thank you again %PCName for allowing me to enter my family's tomb to speak with them. You are an exemplar for the Temple.</t>
-  </si>
-  <si>
     <t>isPCInTemple = 1</t>
   </si>
   <si>
@@ -652,6 +595,162 @@
   </si>
   <si>
     <t>tlvoat_ex_othral_door_unique</t>
+  </si>
+  <si>
+    <t>Please put something on. I'm not talking unless you cover yourself.</t>
+  </si>
+  <si>
+    <t>Oh, oh please cover yourself! Y-you're rather distracting!</t>
+  </si>
+  <si>
+    <t>Are you going in? I need someone to clear the tomb, would you be willing to help me? Though if you don't want to I can't stop such a powerful %PCClass such as yourself.</t>
+  </si>
+  <si>
+    <t>Hello again %PCName, are you free to clear the tomb?</t>
+  </si>
+  <si>
+    <t>%PCName I saw that you went into my family's tomb. Did you happen to clear the tomb anyway?</t>
+  </si>
+  <si>
+    <t>Sera %PCName, I do not wish to trouble you, but have you been able to clear the tomb?</t>
+  </si>
+  <si>
+    <t>How is the tomb? Is it safe for me to go in?</t>
+  </si>
+  <si>
+    <t>Please %PCName I need time to myself. I don't know what it is that I'm feeling, and I need to sort myself out.</t>
+  </si>
+  <si>
+    <t>Hello %PCClass, I'm just working up the courage to end my family's tomb. The guardians are hostile even to me, it would be most helpful if someone could clear the tomb for me.</t>
+  </si>
+  <si>
+    <t>Talked to PC = 0, tlvoat_hasPCAttemptEnter = 0, tlvoat_hasPCEnteredTomb = 0</t>
+  </si>
+  <si>
+    <t>Talked to PC = 0, tlvoat_hasPCAttemptEnter = 1</t>
+  </si>
+  <si>
+    <t>Talked to PC = 1, tlvoat_hasPCEnteredTomb = 0</t>
+  </si>
+  <si>
+    <t>Talked to PC = 1, tlvoat_hasPCEnteredTomb = 1</t>
+  </si>
+  <si>
+    <t>Choice = 1</t>
+  </si>
+  <si>
+    <t>Choice "Yes, I can clear your family's tomb.", 1, "As a member of the Temple I'd be happy to.", 2, "I'm too busy right now.", 3, "No I will not.", 4</t>
+  </si>
+  <si>
+    <t>Choice "Yes, I can clear your family's tomb.", 1, "I'm too busy right now.", 3, "No I will not.", 4</t>
+  </si>
+  <si>
+    <t>PCFaction Temple, tlvoat_estranged_spirits.Journal &lt;= 0</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &lt;= 0</t>
+  </si>
+  <si>
+    <t>Oh that's wonderful, thank you %PCName! Let me know when you've cleared it. I'll be waiting here.</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 10</t>
+  </si>
+  <si>
+    <t>Choice = 2</t>
+  </si>
+  <si>
+    <t>Choice = 3</t>
+  </si>
+  <si>
+    <t>Choice = 4</t>
+  </si>
+  <si>
+    <t>Oh of course! I might be here for some time yet, so if you change your mind you know where to find me.</t>
+  </si>
+  <si>
+    <t>Ah, I'm sorry for bothering you.</t>
+  </si>
+  <si>
+    <t>PCFaction Temple, tlvoat_estranged_spirits.Journal &lt;= 5</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &lt;= 5</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 5</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 4</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &lt;= 5, tlvoat_hasPCEnteredTomb = 1, tlvoat_tombClearCount &gt;= 5</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &lt;= 5, tlvoat_hasPCEnteredTomb = 1, tlvoat_tombClearCount &lt; 5</t>
+  </si>
+  <si>
+    <t>I saw that you went into my family's tomb. Did you happen to clear it anyway? You seem rather dirty compared to earlier.</t>
+  </si>
+  <si>
+    <t>I saw that you went into my family's tomb. Did you happen to clear it anyway?</t>
+  </si>
+  <si>
+    <t>Choice "Yes, the tomb is now safe.", 5, "No, it's not safe for you to enter.", 6</t>
+  </si>
+  <si>
+    <t>Choice = 5</t>
+  </si>
+  <si>
+    <t>Choice = 7</t>
+  </si>
+  <si>
+    <t>Choice "(Lie) Yes, the tomb is now safe.", 7, "No, it's not safe for you to enter.", 6</t>
+  </si>
+  <si>
+    <t>Choice = 6</t>
+  </si>
+  <si>
+    <t>It is? Thank you for putting yourself in danger for me. Give me a little while so that I may converse with my family's spirits.</t>
+  </si>
+  <si>
+    <t>Ok, I'll just keep waiting here.</t>
+  </si>
+  <si>
+    <t>It is? You seem rather unbothered after defeating the tomb's guardians. Well, I trust you %PCName, thank you for putting yourself in danger for me. Give me a little while so that I may converse with my family's spirits.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 20, tlvoat_skeleton Dead &gt;= 5, tlvoat_skeleton_archer &gt;= 1</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 10, tlvoat_skeleton Dead &lt; 5, tlvoat_skeleton_archer &lt; 1</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &lt;= 20</t>
+  </si>
+  <si>
+    <t>PCFaction Temple, tlvoat_estranged_spirits.Journal &lt;= 20</t>
+  </si>
+  <si>
+    <t>OnDeath: increments global tlvoat_Othral_Skeletons_Counter, if &gt;= 6 set journal to 20</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 30</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 30, FadeOut 0.3 PositionCell, FadeIn 1.0 Goodbye</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 31, FadeOut 0.3 PositionCell, SetHealth 0, FadeIn 1.0 Goodbye</t>
+  </si>
+  <si>
+    <t>I'm terribly sorry sera %PCName, I did not realise that you are a priest. Thank you for granting me some of your time in helping me to connect with my family's spirits.</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 10, set tlvoat_hasPCSaidInTemple to 1</t>
+  </si>
+  <si>
+    <t>Thank you again sera %PCName for making my family's tomb safe enough for me to speak with them. I've never met a priest like you before.</t>
   </si>
 </sst>
 </file>
@@ -1266,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
   <dimension ref="A2:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1330,7 +1429,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -1339,7 +1438,7 @@
         <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1359,18 +1458,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>180</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1566,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1500,7 +1602,7 @@
   <dimension ref="A2:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1532,16 +1634,16 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="F3" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1552,13 +1654,13 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1569,16 +1671,16 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="D5">
         <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="F5" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1589,16 +1691,16 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="D6">
         <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1609,7 +1711,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="D7">
         <v>40</v>
@@ -1626,7 +1728,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -1643,7 +1745,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="D9">
         <v>100</v>
@@ -1683,7 +1785,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -1748,7 +1850,7 @@
   <dimension ref="A2:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1765,237 +1867,237 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
         <v>102</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" t="s">
         <v>104</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>105</v>
-      </c>
-      <c r="F7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
         <v>111</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" t="s">
         <v>116</v>
-      </c>
-      <c r="C23" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2005,10 +2107,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F32"/>
+  <dimension ref="A2:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2016,7 +2118,7 @@
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
     <col min="3" max="3" width="20.77734375" customWidth="1"/>
     <col min="4" max="4" width="66.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.109375" customWidth="1"/>
+    <col min="5" max="5" width="34.109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="50.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2030,7 +2132,7 @@
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -2039,144 +2141,144 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" t="s">
         <v>122</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3" t="s">
-        <v>126</v>
-      </c>
-      <c r="F3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" t="s">
-        <v>126</v>
+        <v>184</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>132</v>
+        <v>191</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>131</v>
+        <v>185</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>135</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>136</v>
+        <v>187</v>
       </c>
       <c r="F8" t="s">
-        <v>137</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>139</v>
+        <v>189</v>
       </c>
       <c r="F9" t="s">
-        <v>138</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>140</v>
+        <v>188</v>
       </c>
       <c r="F10" t="s">
-        <v>138</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2187,16 +2289,16 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" t="s">
-        <v>126</v>
+        <v>190</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="F11" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2207,13 +2309,13 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="F12" t="s">
-        <v>150</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2224,13 +2326,13 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2241,16 +2343,16 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" t="s">
-        <v>146</v>
+        <v>131</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="F14" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2261,13 +2363,13 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="F15" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2278,13 +2380,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="F16" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2295,16 +2397,16 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E17" t="s">
-        <v>126</v>
+        <v>142</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="F17" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2315,270 +2417,453 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="F18" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E20" t="s">
-        <v>163</v>
+        <v>232</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F20" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E21" t="s">
-        <v>163</v>
+        <v>206</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="F21" t="s">
-        <v>161</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E22" t="s">
-        <v>163</v>
+        <v>207</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="F22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E23" t="s">
-        <v>163</v>
+        <v>221</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="F23" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F24" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F25" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F30" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>13</v>
       </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E24" t="s">
-        <v>163</v>
-      </c>
-      <c r="F24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>13</v>
       </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" t="s">
-        <v>116</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F25" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>13</v>
       </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" t="s">
-        <v>130</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>13</v>
       </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s">
-        <v>130</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>13</v>
       </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E29" t="s">
-        <v>163</v>
-      </c>
-      <c r="F29" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E30" t="s">
-        <v>163</v>
-      </c>
-      <c r="F30" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E31" t="s">
-        <v>163</v>
-      </c>
-      <c r="F31" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E32" t="s">
-        <v>163</v>
-      </c>
-      <c r="F32" t="s">
-        <v>180</v>
+      <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F64">
+  <conditionalFormatting sqref="B3:F73">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2612,7 +2897,7 @@
   <dimension ref="A2:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2634,7 +2919,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -2646,7 +2931,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2815,13 +3100,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2829,13 +3114,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2843,13 +3128,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2857,10 +3142,10 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
         <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>85</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
@@ -2871,10 +3156,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
         <v>84</v>
-      </c>
-      <c r="C7" t="s">
-        <v>86</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
@@ -2885,7 +3170,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
@@ -2954,7 +3239,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -2968,7 +3253,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -2979,7 +3264,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
@@ -2993,7 +3278,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
         <v>59</v>
@@ -3010,7 +3295,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>58</v>
@@ -3027,10 +3312,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -3044,7 +3329,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Add: Uravasa's ghost to tomb, dialogue for middle of the quest
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5776B7A-EA06-4B6F-B5D8-8110FCC74408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7297DF42-E1B8-4CD6-A322-A339DE2C1182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="262">
   <si>
     <t>Name</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Aryasi thanked me for giving her the opportunity to speak with her grandmother's spirit. She offered a reward, but I turned her down.</t>
   </si>
   <si>
-    <t>I killed Aryasi Othral. She should now have the opportunity to speak with her ancesters.</t>
-  </si>
-  <si>
     <t>PC killed quest giver, at any point</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>Urn Labelled "Uravasa Othral"</t>
   </si>
   <si>
-    <t>tlvoat_uravasa_ghost</t>
-  </si>
-  <si>
     <t>Uravasa Othral's Ghost</t>
   </si>
   <si>
@@ -435,36 +429,9 @@
     <t>tlvoat_estranged_spirits.Journal &gt;= updated, unable to clear</t>
   </si>
   <si>
-    <t>It feels… colder in here than I remember. The spirits of my family are silent to me.</t>
-  </si>
-  <si>
-    <t>The spirits of my family remain silent.</t>
-  </si>
-  <si>
-    <t>I guess I was never really an Othral. I should stopped thinking of myself as one when I ran away.</t>
-  </si>
-  <si>
-    <t>Goodbye?</t>
-  </si>
-  <si>
     <t>asks if PC found secret area, asks if PC found secret area (temple)</t>
   </si>
   <si>
-    <t>Hey %PCName, have you found anything?</t>
-  </si>
-  <si>
-    <t>%PCRank, I do not wish to get in your way, but if there's anything I can do to help please ask.</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal &gt;= updated</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal &gt;= updated, refused to find secret</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal &gt;= find secret</t>
-  </si>
-  <si>
     <t>escorting, completed escort</t>
   </si>
   <si>
@@ -510,30 +477,12 @@
     <t>isPCInTemple = 1</t>
   </si>
   <si>
-    <t>I haven't spoken with them in so long, and I thought that they would want to speak with me given how long it's been and that I'm the last member of the family. But I thought wrong. The only one who I ever really got on with was my grandmother, but I can't find her. I used to suspect that there is a hidden section of the tomb.</t>
-  </si>
-  <si>
     <t>Yes! I'm so happy that I've been able to reconnect with my grandmother.</t>
   </si>
   <si>
-    <t>Whenever I asked my parents they always denied it, but every time my mother expressed missing grandmother she would come to the tomb. Once I sneaked after her and she prayed at the shrine, but then I was caught and couldn't find anything else.</t>
-  </si>
-  <si>
-    <t>hasPCRevealedSecret = 0</t>
-  </si>
-  <si>
-    <t>hasPCRevealedSecret = 1</t>
-  </si>
-  <si>
     <t>Have you found it yet?</t>
   </si>
   <si>
-    <t>hasPCRevealedSecret = 0, journal == offered to find</t>
-  </si>
-  <si>
-    <t>hasPCRevealedSecret = 1, journal == offered to find</t>
-  </si>
-  <si>
     <t>Met Othral/attempted to enter tomb, accepted/accepted after initial decline</t>
   </si>
   <si>
@@ -621,9 +570,6 @@
     <t>Please %PCName I need time to myself. I don't know what it is that I'm feeling, and I need to sort myself out.</t>
   </si>
   <si>
-    <t>Hello %PCClass, I'm just working up the courage to end my family's tomb. The guardians are hostile even to me, it would be most helpful if someone could clear the tomb for me.</t>
-  </si>
-  <si>
     <t>Talked to PC = 0, tlvoat_hasPCAttemptEnter = 0, tlvoat_hasPCEnteredTomb = 0</t>
   </si>
   <si>
@@ -751,6 +697,141 @@
   </si>
   <si>
     <t>Thank you again sera %PCName for making my family's tomb safe enough for me to speak with them. I've never met a priest like you before.</t>
+  </si>
+  <si>
+    <t>spirits of my family</t>
+  </si>
+  <si>
+    <t>Hello %PCClass, I was just working up the courage to enter my family's tomb. Unfortunately the guardian spirits are hostile even to me. I just need to find a way to clear the tomb so that I can speak to the spirits of my family. Well, only if their feelings have change.</t>
+  </si>
+  <si>
+    <t>It feels… colder in here than I remember. I spent some time reaching out, but the spirits of my family are silent to me.</t>
+  </si>
+  <si>
+    <t>I haven't spoken with them in so long. I thought, foolishly, foolishly, they would want to speak with me given how long it has been and that I'm the last one of the family alive. But I thought wrong, even in death they want nothing to do with me. Nothing! They can't see past who they think I am, so they don't see the woman that I am and always have been. Aren't families supposed to love each other unconditionally?</t>
+  </si>
+  <si>
+    <t>Ever since I… better understood who I am they pressured me to be who they wanted me to be. When that didn't work they turned to shame and mockery. Then it was denying what was promised to me as the firstborn, giving to my younger brothers Lletho and Jathys the family blade and armor. Eventually I took what I could and ran away. That was many years ago, and it was only recently that I received a letter from an old friend letting me know the fate of my family.</t>
+  </si>
+  <si>
+    <t>if PC in Temple: Choice "I'm sorry to hear that your family pushed you away.", 2, "Was there anyone in your family who you had a good relationship with?", 3, "Just as Ghostfence is a monument to Dunmer pride in overcoming our enemies, so too should you in standing up for yourself against a family that should know better.", 4 ELSE Choice "I'm sorry to hear that your family pushed you away.", 2, "Was there anyone in your family who you had a good relationship with?", 3</t>
+  </si>
+  <si>
+    <t>Thank you %PCName. Coming here has brought up so many old feelings that I've kept so very deeply buried. It hurts all the more that I don't even hear my grandmother's spirit, as she was the only one I ever had a good relationship with. I used to suspect that there is a hidden section of the tomb, and I am once again hoping there is one and that she was laid to rest there.</t>
+  </si>
+  <si>
+    <t>Yes, there was: my grandmother. I can't hear her either, which makes everything hurt all the more. I find myself hoping that there's a hidden section of the tomb, just as I once did.</t>
+  </si>
+  <si>
+    <t>tlvoat_hasAskedAboutSpirits = 0</t>
+  </si>
+  <si>
+    <t>Choice "Continue", 1, set tlvoat_hasAskedAboutSpirits to 1</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 30, tlvoat_hasAskedAboutSpirits = 1</t>
+  </si>
+  <si>
+    <t>They are remaining silent. I can't help but hope that my grandmother is in a hidden section.</t>
+  </si>
+  <si>
+    <t>I… Thank you %PCName… That means a lot to me. [she is silent for a minute] I've always felt like a coward or that I'm weak for running away. Everything that I've done has been to be someone not like my family at all. I think I've been hurting myself. I had hoped to speak to my grandmother, but she too is silent. I once suspected that there is a hidden section in this tomb, and I can feel hope rising that this is the case.</t>
+  </si>
+  <si>
+    <t>Whenever I asked my parents they always denied it, but every time my mother expressed missing grandmother she would come to the tomb. On one of these times I followed her and watched as she prayed at the shrine, then after a while, she reached out to it and I heard something heavy move elsewhere in the tomb. But that was when she caught me and I dragged me out. I investigated the shrine a few other times when I was alone, but found nothing. Maybe some fresh hands could reveal something?</t>
+  </si>
+  <si>
+    <t>If PCFoundSecret: Choice "I found a button hidden on the shrine and pressed it.", 4 ELSE Choice "I could take a look for you.", 1, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3</t>
+  </si>
+  <si>
+    <t>You will? Thank you! I'll be waiting right here.</t>
+  </si>
+  <si>
+    <t>Of course, you have done a lot for me already. I'll take a look, and if you change your mind I'll be right here.</t>
+  </si>
+  <si>
+    <t>PC lied that the tomb was safe</t>
+  </si>
+  <si>
+    <t>PC refused to help find hidden section</t>
+  </si>
+  <si>
+    <t>Aryasi wanted further help in finding a hidden section in Othral Ancestral tomb, I told her to search for it herself.</t>
+  </si>
+  <si>
+    <t>I see. I understand %PCName. You have already gone so far as to put yourself in danger for me, a stranger. Thank you for all that you've done up to this point, including listening to me vent my heart out about my family.</t>
+  </si>
+  <si>
+    <t>set tlvoat_Estranged_Spirits to 40</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 30</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 40</t>
+  </si>
+  <si>
+    <t>I have killed Aryasi Othral. Her death should give her the opportunity to speak with her ancesters.</t>
+  </si>
+  <si>
+    <t>I met Aryasi Othral who needed help with clearing her family's tomb. I turned her down for now.</t>
+  </si>
+  <si>
+    <t>Met Othral/attempted to enter tomb, declined</t>
+  </si>
+  <si>
+    <t>Met Othral/attempted to enter tomb, said no</t>
+  </si>
+  <si>
+    <t>set tlvoat_Estranged_Spirits to 200, Goodbye</t>
+  </si>
+  <si>
+    <t>Thank you again for clearing my family's tomb %PCClass, but right now I'd prefer to be alone.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &gt;= 200</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal = 40</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal = 40, tlvoat_hasPCSaidInTemple == 1</t>
+  </si>
+  <si>
+    <t>Sera, I hope searching for this hidden section isn't too much trouble for you.</t>
+  </si>
+  <si>
+    <t>Hey %PCName, have you found any hidden section of the tomb? Has the shrine been keeping a secret all these years?</t>
+  </si>
+  <si>
+    <t>tlvoat_uravasa_ghost_u</t>
+  </si>
+  <si>
+    <t>tlvoat_uravasa_ghost_u_script</t>
+  </si>
+  <si>
+    <t>If Distance Player &lt;= 512: ForceGreeting</t>
+  </si>
+  <si>
+    <t>You’re the new presence that I felt in the resting place of myself and the spirits of my family. Leave now, or I will make this tomb your resting place too.</t>
+  </si>
+  <si>
+    <t>Talked to PC = 1</t>
+  </si>
+  <si>
+    <t>Why are you continuing to linger in this sacred place?</t>
+  </si>
+  <si>
+    <t>Talked to PC = 0, tlvoat_Estranged_Spirits.Journal &gt;= 30</t>
+  </si>
+  <si>
+    <t>Talked to PC = 0, tlvoat_Estranged_Spirits.Journal &lt; 30</t>
+  </si>
+  <si>
+    <t>You are one of the new presences that I can feel in this resting place of the spirits of my family, but the other is strangely familier. Bring them to me so I can see who they are.</t>
+  </si>
+  <si>
+    <t>set tlvoat_uravasaMetPC to 1, Goodbye</t>
   </si>
 </sst>
 </file>
@@ -1363,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
-  <dimension ref="A2:E7"/>
+  <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1404,79 +1485,96 @@
         <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>253</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>252</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>68</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>180</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>228</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:E32">
+  <conditionalFormatting sqref="B3:E33">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$C3="Yes"</formula>
     </cfRule>
@@ -1495,7 +1593,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A1048576 C3:C60</xm:sqref>
+          <xm:sqref>A1:A1048576 C3:C61</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1566,7 +1664,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1599,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
-  <dimension ref="A2:F12"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1626,24 +1724,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="D3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F3" t="s">
-        <v>173</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1654,16 +1746,16 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>164</v>
+        <v>242</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1671,19 +1763,19 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="F5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1691,16 +1783,13 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="D6">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1711,16 +1800,19 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="F7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1728,13 +1820,16 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="D8">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>154</v>
+      </c>
+      <c r="F8" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1745,16 +1840,13 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1765,19 +1857,16 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>153</v>
       </c>
       <c r="D10">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1785,10 +1874,13 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="D11">
-        <v>200</v>
+        <v>100</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="F11" t="s">
         <v>38</v>
@@ -1802,20 +1894,80 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12">
-        <v>300</v>
+        <v>101</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
         <v>38</v>
       </c>
     </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13">
+        <v>200</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14">
+        <v>300</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D15">
+        <v>400</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F3 B3:E31 F5:F6 F9 F11">
+  <conditionalFormatting sqref="F7:F8 F11 F13:F14 B3:F5 B6:E34">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -1867,237 +2019,237 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
         <v>100</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" t="s">
         <v>102</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>103</v>
-      </c>
-      <c r="F7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
         <v>109</v>
-      </c>
-      <c r="C20" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" t="s">
         <v>114</v>
-      </c>
-      <c r="C23" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2107,10 +2259,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F41"/>
+  <dimension ref="A2:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2147,16 +2299,16 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" t="s">
         <v>120</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2167,19 +2319,19 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2187,13 +2339,13 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="F5" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2204,13 +2356,13 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2221,13 +2373,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="F7" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2238,13 +2390,13 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="F8" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2255,13 +2407,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="F9" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2272,13 +2424,13 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="F10" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2289,90 +2441,90 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>129</v>
+        <v>219</v>
       </c>
       <c r="F12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>130</v>
+        <v>246</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>132</v>
+        <v>251</v>
       </c>
       <c r="F14" t="s">
-        <v>137</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="F15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2380,16 +2532,19 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2397,33 +2552,33 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="F18" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2434,16 +2589,16 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="F19" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2454,96 +2609,96 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>232</v>
+        <v>188</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>233</v>
+        <v>192</v>
       </c>
       <c r="F20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E22" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="F23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>222</v>
+      <c r="E24" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="F24" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2551,19 +2706,19 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>223</v>
+        <v>133</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>231</v>
+        <v>179</v>
       </c>
       <c r="F25" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2571,19 +2726,19 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="F26" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2591,19 +2746,19 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="F27" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2611,19 +2766,19 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="F28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2631,16 +2786,16 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>145</v>
+        <v>196</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>198</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2651,16 +2806,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="F30" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2671,16 +2826,16 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>215</v>
+        <v>137</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="F31" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2691,16 +2846,16 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="F32" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2711,135 +2866,135 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>217</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>217</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>217</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" t="s">
+        <v>217</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F39" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" t="s">
-        <v>114</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F34" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" t="s">
-        <v>126</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" t="s">
-        <v>126</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F38" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F39" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
         <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>217</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="F40" t="s">
-        <v>160</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2850,20 +3005,171 @@
         <v>29</v>
       </c>
       <c r="C41" t="s">
+        <v>217</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F43" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F44" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F46" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>252</v>
+      </c>
+      <c r="C47" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F41" t="s">
-        <v>161</v>
+      <c r="D47" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F47" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>252</v>
+      </c>
+      <c r="C48" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F48" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>252</v>
+      </c>
+      <c r="C49" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F49" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F73">
+  <conditionalFormatting sqref="B3:F76">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2931,7 +3237,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2969,7 +3275,7 @@
   <dimension ref="A2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2991,19 +3297,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>252</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3011,16 +3317,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3028,16 +3334,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3100,13 +3406,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3114,13 +3420,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3128,13 +3434,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3142,13 +3448,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
         <v>81</v>
       </c>
-      <c r="C6" t="s">
-        <v>83</v>
-      </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3156,13 +3462,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
         <v>82</v>
       </c>
-      <c r="C7" t="s">
-        <v>84</v>
-      </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3170,13 +3476,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3239,7 +3545,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -3253,7 +3559,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -3264,10 +3570,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -3278,16 +3584,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3295,16 +3601,16 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3312,16 +3618,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3329,16 +3635,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: pre-quest & early quest dialogue to better account for PC's actions
Add: script to tomb ex door to have Aryasi call out to the PC
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7297DF42-E1B8-4CD6-A322-A339DE2C1182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DD00E6-4D55-4B43-861F-DB3BFB70968C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="265">
   <si>
     <t>Name</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Ancester Ghost</t>
   </si>
   <si>
-    <t>tlvoat_load_door</t>
-  </si>
-  <si>
     <t>Door</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>tlvoat_aryasi_othral_script</t>
   </si>
   <si>
-    <t>tlvoat_load_door_script</t>
-  </si>
-  <si>
     <t>tlvoat_shrine</t>
   </si>
   <si>
@@ -246,9 +240,6 @@
     <t>lvl 5</t>
   </si>
   <si>
-    <t>OnActivate: ForceGreeting Aryasi if not yet spoken, aryasi.hasPCAttemptEnter to 1</t>
-  </si>
-  <si>
     <t>tlvoat_urn_lletho_uni</t>
   </si>
   <si>
@@ -435,9 +426,6 @@
     <t>escorting, completed escort</t>
   </si>
   <si>
-    <t>tlvoat_estranged_spirits.Journal == escorting</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal == escorting success</t>
   </si>
   <si>
@@ -447,9 +435,6 @@
     <t>Ah! This is her! Oh thank you, thank you so much for taking me to my grandmother. Please, leave me for a while so that I may speak with her spirit.</t>
   </si>
   <si>
-    <t>Yes, so that I may speak with the spirits of my family. I wish to settle some things. Would you be able to help with this?</t>
-  </si>
-  <si>
     <t>Have you changed your mind?</t>
   </si>
   <si>
@@ -474,9 +459,6 @@
     <t>Thank you again for making it safe for me</t>
   </si>
   <si>
-    <t>isPCInTemple = 1</t>
-  </si>
-  <si>
     <t>Yes! I'm so happy that I've been able to reconnect with my grandmother.</t>
   </si>
   <si>
@@ -552,15 +534,6 @@
     <t>Oh, oh please cover yourself! Y-you're rather distracting!</t>
   </si>
   <si>
-    <t>Are you going in? I need someone to clear the tomb, would you be willing to help me? Though if you don't want to I can't stop such a powerful %PCClass such as yourself.</t>
-  </si>
-  <si>
-    <t>Hello again %PCName, are you free to clear the tomb?</t>
-  </si>
-  <si>
-    <t>%PCName I saw that you went into my family's tomb. Did you happen to clear the tomb anyway?</t>
-  </si>
-  <si>
     <t>Sera %PCName, I do not wish to trouble you, but have you been able to clear the tomb?</t>
   </si>
   <si>
@@ -585,21 +558,9 @@
     <t>Choice = 1</t>
   </si>
   <si>
-    <t>Choice "Yes, I can clear your family's tomb.", 1, "As a member of the Temple I'd be happy to.", 2, "I'm too busy right now.", 3, "No I will not.", 4</t>
-  </si>
-  <si>
-    <t>Choice "Yes, I can clear your family's tomb.", 1, "I'm too busy right now.", 3, "No I will not.", 4</t>
-  </si>
-  <si>
-    <t>PCFaction Temple, tlvoat_estranged_spirits.Journal &lt;= 0</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal &lt;= 0</t>
   </si>
   <si>
-    <t>Oh that's wonderful, thank you %PCName! Let me know when you've cleared it. I'll be waiting here.</t>
-  </si>
-  <si>
     <t>Journal "tlvoat_Estranged_Spirits", 10</t>
   </si>
   <si>
@@ -615,12 +576,6 @@
     <t>Oh of course! I might be here for some time yet, so if you change your mind you know where to find me.</t>
   </si>
   <si>
-    <t>Ah, I'm sorry for bothering you.</t>
-  </si>
-  <si>
-    <t>PCFaction Temple, tlvoat_estranged_spirits.Journal &lt;= 5</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal &lt;= 5</t>
   </si>
   <si>
@@ -663,9 +618,6 @@
     <t>Ok, I'll just keep waiting here.</t>
   </si>
   <si>
-    <t>It is? You seem rather unbothered after defeating the tomb's guardians. Well, I trust you %PCName, thank you for putting yourself in danger for me. Give me a little while so that I may converse with my family's spirits.</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal == 20, tlvoat_skeleton Dead &gt;= 5, tlvoat_skeleton_archer &gt;= 1</t>
   </si>
   <si>
@@ -675,24 +627,12 @@
     <t>tlvoat_estranged_spirits.Journal &lt;= 20</t>
   </si>
   <si>
-    <t>PCFaction Temple, tlvoat_estranged_spirits.Journal &lt;= 20</t>
-  </si>
-  <si>
     <t>OnDeath: increments global tlvoat_Othral_Skeletons_Counter, if &gt;= 6 set journal to 20</t>
   </si>
   <si>
     <t>tlvoat_estranged_spirits.Journal == 30</t>
   </si>
   <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 30, FadeOut 0.3 PositionCell, FadeIn 1.0 Goodbye</t>
-  </si>
-  <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 31, FadeOut 0.3 PositionCell, SetHealth 0, FadeIn 1.0 Goodbye</t>
-  </si>
-  <si>
-    <t>I'm terribly sorry sera %PCName, I did not realise that you are a priest. Thank you for granting me some of your time in helping me to connect with my family's spirits.</t>
-  </si>
-  <si>
     <t>Journal "tlvoat_Estranged_Spirits", 10, set tlvoat_hasPCSaidInTemple to 1</t>
   </si>
   <si>
@@ -702,15 +642,9 @@
     <t>spirits of my family</t>
   </si>
   <si>
-    <t>Hello %PCClass, I was just working up the courage to enter my family's tomb. Unfortunately the guardian spirits are hostile even to me. I just need to find a way to clear the tomb so that I can speak to the spirits of my family. Well, only if their feelings have change.</t>
-  </si>
-  <si>
     <t>It feels… colder in here than I remember. I spent some time reaching out, but the spirits of my family are silent to me.</t>
   </si>
   <si>
-    <t>I haven't spoken with them in so long. I thought, foolishly, foolishly, they would want to speak with me given how long it has been and that I'm the last one of the family alive. But I thought wrong, even in death they want nothing to do with me. Nothing! They can't see past who they think I am, so they don't see the woman that I am and always have been. Aren't families supposed to love each other unconditionally?</t>
-  </si>
-  <si>
     <t>Ever since I… better understood who I am they pressured me to be who they wanted me to be. When that didn't work they turned to shame and mockery. Then it was denying what was promised to me as the firstborn, giving to my younger brothers Lletho and Jathys the family blade and armor. Eventually I took what I could and ran away. That was many years ago, and it was only recently that I received a letter from an old friend letting me know the fate of my family.</t>
   </si>
   <si>
@@ -832,6 +766,81 @@
   </si>
   <si>
     <t>set tlvoat_uravasaMetPC to 1, Goodbye</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &lt;= 20, tlvoat_hasPCSaidInTemple = 1</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 50</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 30, FadeOut 0.1 PositionCell, FadeIn 1.0 Goodbye</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 31, FadeOut 0.1 PositionCell, SetHealth 0, FadeIn 1.0 Goodbye</t>
+  </si>
+  <si>
+    <t>I haven't spoken with them in so long. I thought, foolishly, that they would want to speak with me given how long it has been and that I'm the last one of the family alive. But I thought wrong, even in death they want nothing to do with me. Nothing! They can't see past who they think I am, so they don't see the woman that I am and always have been. Aren't families supposed to love each other unconditionally?</t>
+  </si>
+  <si>
+    <t>OnActivate: ForceGreeting Aryasi if not yet spoken, aryasi.hasPCAttemptEnter to 1; set hasPCEntered to 1</t>
+  </si>
+  <si>
+    <t>tlvoat_ex_othral_door_script</t>
+  </si>
+  <si>
+    <t>I saw that you went into my family's tomb, and did you happen to clear the tomb so that it's safe for me to go in?</t>
+  </si>
+  <si>
+    <t>Hello %PCClass, I'm trying to work up the courage to enter my family's resting place, as the guardian spirits are hostile even to me. Meaning I can't get in without them killing me. So I need to find a way to clear the tomb so that I can speak to the spirits of my family.</t>
+  </si>
+  <si>
+    <t>Hey, excuse me, are you going in? I need to clear the tomb, would you be willing to help by doing this for me? Though if you don't want to I can't stop such a powerful %PCClass such as yourself.</t>
+  </si>
+  <si>
+    <t>Hello again %PCName, as you can see I'm still here waiting for help to clear the tomb or to work up the courage.</t>
+  </si>
+  <si>
+    <t>Ordinarially the guardians would leave me alone, but they aren't. Perhaps because I ran away from my family or they no longer recognise me. I can cast some simple spells but they are too numerous and powerful for me, and so I'm left with risking near certain death or help from someone else. Would you be willing to do this for me?</t>
+  </si>
+  <si>
+    <t>You will? Thank you %PCName! When you think it's safe for me, let me know. I'll be waiting here. Before you go in, please respect my family's spirits. Meaning don't disturb their remains! I don't have much to reward you with, so while I'd prefer that you didn't, you can take the objects that they once valued in life including the offerings left by those paying their respects.</t>
+  </si>
+  <si>
+    <t>I'm terribly sorry sera %PCName, I did not realise that you are a priest. Thank you for granting me some of your time in helping me to connect with my family's spirits. When you think it's safe for me, let me know. I'll be waiting here.</t>
+  </si>
+  <si>
+    <t>Ah, well I'm sorry for bothering you.</t>
+  </si>
+  <si>
+    <t>Choice = 8</t>
+  </si>
+  <si>
+    <t>Choice = 9</t>
+  </si>
+  <si>
+    <t>[She enters the tomb.]</t>
+  </si>
+  <si>
+    <t>Choice = 10</t>
+  </si>
+  <si>
+    <t>Oh! Right. It's a good thing to be thorough. I'll keep waiting right here.</t>
+  </si>
+  <si>
+    <t>It is? You seem rather untouched after dealing the tomb's guardians. Well, I trust you %PCName, thank you for putting yourself in danger for me. Give me a little while so that I may converse with my family's spirits.</t>
+  </si>
+  <si>
+    <t>Choice "[Let her enter]", 10, "[Stop her] Wait, I think I may have missed a section.", 8</t>
+  </si>
+  <si>
+    <t>Choice "[Let her enter]", 9, "[Stop her] Wait, I think I may have missed a section.", 8</t>
+  </si>
+  <si>
+    <t>if PCRank Temple &gt;= 0: Choice "Yes, I can clear your family's tomb.", 1, "As a priest of the Temple I'd be happy to.", 2, "I'm too busy right now.", 3, "No I will not.", 4 ELSE Choice "Yes, I can clear your family's tomb.", 1, "I'm too busy right now.", 3, "No I will not.", 4</t>
+  </si>
+  <si>
+    <t>tlvoat_PCMentionInTemple = 1</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1456,7 @@
   <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,7 +1485,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1485,24 +1494,24 @@
         <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1510,16 +1519,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>66</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1527,16 +1536,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1544,16 +1553,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1561,16 +1570,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1664,7 +1673,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1700,7 +1709,7 @@
   <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1735,7 +1744,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1746,13 +1755,13 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1763,16 +1772,16 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1783,13 +1792,13 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D6">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1800,16 +1809,16 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D7">
         <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1820,16 +1829,16 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D8">
         <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1840,13 +1849,13 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D9">
         <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1857,13 +1866,13 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D10">
         <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1874,16 +1883,16 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D11">
         <v>100</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1894,16 +1903,16 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>101</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
         <v>37</v>
-      </c>
-      <c r="F12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1914,16 +1923,16 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="D13">
         <v>200</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1934,16 +1943,16 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D14">
         <v>300</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1954,20 +1963,20 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="D15">
         <v>400</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F7:F8 F11 F13:F14 B3:F5 B6:E34">
+  <conditionalFormatting sqref="B3:F5 B6:E34 F7:F8 F11 F13:F14">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2019,237 +2028,237 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
         <v>98</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" t="s">
         <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" t="s">
         <v>113</v>
-      </c>
-      <c r="D24" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2259,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F49"/>
+  <dimension ref="A2:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2299,16 +2308,16 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2319,16 +2328,16 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" t="s">
         <v>118</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2339,13 +2348,13 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>218</v>
+        <v>248</v>
       </c>
       <c r="F5" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2356,16 +2365,16 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>168</v>
+        <v>249</v>
       </c>
       <c r="F6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2373,13 +2382,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>169</v>
+        <v>250</v>
       </c>
       <c r="F7" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2390,16 +2399,16 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>170</v>
+        <v>247</v>
       </c>
       <c r="F8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2407,16 +2416,16 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F9" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2424,13 +2433,13 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F10" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2441,16 +2450,16 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="F11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2461,13 +2470,13 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="F12" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2478,16 +2487,16 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="F13" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2498,13 +2507,13 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="F14" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2515,13 +2524,13 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="F15" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2532,16 +2541,16 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2552,16 +2561,16 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2569,19 +2578,19 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>183</v>
+        <v>252</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2589,16 +2598,16 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="F19" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2609,16 +2618,16 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="F20" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2629,16 +2638,16 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>189</v>
+        <v>254</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="F21" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2649,16 +2658,16 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>212</v>
+        <v>262</v>
       </c>
       <c r="F22" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2669,13 +2678,13 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="F23" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2686,19 +2695,19 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>205</v>
+        <v>260</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>213</v>
+        <v>261</v>
       </c>
       <c r="F24" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2706,16 +2715,13 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>179</v>
+        <v>259</v>
       </c>
       <c r="F25" t="s">
-        <v>181</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2726,19 +2732,19 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>133</v>
+        <v>257</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
       <c r="F26" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2746,19 +2752,19 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>134</v>
+        <v>257</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>179</v>
+        <v>243</v>
       </c>
       <c r="F27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2766,19 +2772,19 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>134</v>
+        <v>251</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>180</v>
+        <v>263</v>
       </c>
       <c r="F28" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2786,16 +2792,16 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>196</v>
+        <v>129</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>198</v>
+        <v>263</v>
       </c>
       <c r="F29" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2806,16 +2812,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="F30" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2826,16 +2832,16 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="F31" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2846,16 +2852,16 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="F32" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2866,16 +2872,19 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>216</v>
+        <v>131</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="F33" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2883,13 +2892,16 @@
         <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+      <c r="F34" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2897,19 +2909,13 @@
         <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>109</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F35" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2917,16 +2923,19 @@
         <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>223</v>
+        <v>199</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="F36" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2934,16 +2943,16 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="F37" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -2951,13 +2960,13 @@
         <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>229</v>
+        <v>202</v>
       </c>
       <c r="F38" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -2968,19 +2977,16 @@
         <v>29</v>
       </c>
       <c r="C39" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="F39" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2988,188 +2994,208 @@
         <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>228</v>
+        <v>244</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="F40" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
         <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>143</v>
+        <v>206</v>
+      </c>
+      <c r="F41" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E42" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F44" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F46" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F47" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>230</v>
+      </c>
+      <c r="C48" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>230</v>
+      </c>
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F42" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="F43" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" t="s">
-        <v>117</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="F44" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" t="s">
-        <v>117</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F49" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
         <v>230</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F45" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" t="s">
-        <v>117</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F46" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" t="s">
-        <v>252</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="C50" t="s">
+        <v>116</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F47" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" t="s">
-        <v>252</v>
-      </c>
-      <c r="C48" t="s">
-        <v>119</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F48" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" t="s">
-        <v>252</v>
-      </c>
-      <c r="C49" t="s">
-        <v>119</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F49" t="s">
-        <v>256</v>
+      <c r="F50" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F76">
+  <conditionalFormatting sqref="B3:F77">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -3237,7 +3263,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3300,16 +3326,16 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3317,16 +3343,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3334,16 +3360,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3406,13 +3432,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3420,13 +3446,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3434,13 +3460,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3448,13 +3474,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3462,13 +3488,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3476,13 +3502,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3520,7 +3546,7 @@
   <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3545,10 +3571,10 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -3559,7 +3585,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -3570,10 +3596,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -3584,16 +3610,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3601,16 +3627,16 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3618,16 +3644,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3635,16 +3661,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: FadeOut/In sequences not correctly masking PositionCell calls
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DD00E6-4D55-4B43-861F-DB3BFB70968C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B571C1BC-5773-446F-B6C2-237967145BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="271">
   <si>
     <t>Name</t>
   </si>
@@ -156,15 +156,9 @@
     <t>Met grandmother's spirit</t>
   </si>
   <si>
-    <t>Lead Aryasi, they've spoken, she expressed her thanks</t>
-  </si>
-  <si>
     <t>FIN</t>
   </si>
   <si>
-    <t>Aryasi thanked me for giving her the opportunity to speak with her grandmother's spirit. She offered a reward, but I turned her down.</t>
-  </si>
-  <si>
     <t>PC killed quest giver, at any point</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>Shrine of the Tribunal</t>
   </si>
   <si>
-    <t>Let Aryasi know</t>
-  </si>
-  <si>
     <t>Ashes of Lletho Othral</t>
   </si>
   <si>
@@ -426,21 +417,12 @@
     <t>escorting, completed escort</t>
   </si>
   <si>
-    <t>tlvoat_estranged_spirits.Journal == escorting success</t>
-  </si>
-  <si>
-    <t>Don't worry, I'm keeping up!</t>
-  </si>
-  <si>
     <t>Ah! This is her! Oh thank you, thank you so much for taking me to my grandmother. Please, leave me for a while so that I may speak with her spirit.</t>
   </si>
   <si>
     <t>Have you changed your mind?</t>
   </si>
   <si>
-    <t>Choice</t>
-  </si>
-  <si>
     <t>Ah, %PCName! Is it safe to go in?</t>
   </si>
   <si>
@@ -462,42 +444,21 @@
     <t>Yes! I'm so happy that I've been able to reconnect with my grandmother.</t>
   </si>
   <si>
-    <t>Have you found it yet?</t>
-  </si>
-  <si>
     <t>Met Othral/attempted to enter tomb, accepted/accepted after initial decline</t>
   </si>
   <si>
-    <t>I met Aryasi Othral outside of her family's tomb, who can't enter because the tomb's guardians are hostile towards her. I accepted her request to clear the tomb so that she can enter.</t>
-  </si>
-  <si>
-    <t>All guardians in Othral Ancestral Tomb have been dispatched. I will let Aryasi Othral know that she can safely enter.</t>
-  </si>
-  <si>
     <t>All tomb guardians dead, was previously accepted</t>
   </si>
   <si>
-    <t>I let Aryasi Othral know that her family's tomb is safe. She's gone inside to speak with the spirits. I should return to check on her.</t>
-  </si>
-  <si>
     <t>Let Aryasi know it's safe, both accepted before &amp; not accepted. Starts quest if latter</t>
   </si>
   <si>
-    <t>I lied to Aryasi Othral that her family's tomb is safe. The tomb's guardian's might end her.</t>
-  </si>
-  <si>
-    <t>Aryasi Othral mentioned that there might be a hidden section of Othral Ancestral Tomb. I offered to help find it.</t>
-  </si>
-  <si>
     <t>Aryasi Othral wants me to lead her to where her grandmother has been laid to rest.</t>
   </si>
   <si>
     <t>Let Aryasi know it's safe, both accepted before &amp; not accepted. Starts quest if latter. Kills Aryasi</t>
   </si>
   <si>
-    <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that she's had an opportunity to reconnect. She gave me a ring that was her grandmother's.</t>
-  </si>
-  <si>
     <t>BEGIN</t>
   </si>
   <si>
@@ -708,12 +669,6 @@
     <t>I have killed Aryasi Othral. Her death should give her the opportunity to speak with her ancesters.</t>
   </si>
   <si>
-    <t>I met Aryasi Othral who needed help with clearing her family's tomb. I turned her down for now.</t>
-  </si>
-  <si>
-    <t>Met Othral/attempted to enter tomb, declined</t>
-  </si>
-  <si>
     <t>Met Othral/attempted to enter tomb, said no</t>
   </si>
   <si>
@@ -762,9 +717,6 @@
     <t>Talked to PC = 0, tlvoat_Estranged_Spirits.Journal &lt; 30</t>
   </si>
   <si>
-    <t>You are one of the new presences that I can feel in this resting place of the spirits of my family, but the other is strangely familier. Bring them to me so I can see who they are.</t>
-  </si>
-  <si>
     <t>set tlvoat_uravasaMetPC to 1, Goodbye</t>
   </si>
   <si>
@@ -774,12 +726,6 @@
     <t>tlvoat_estranged_spirits.Journal == 50</t>
   </si>
   <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 30, FadeOut 0.1 PositionCell, FadeIn 1.0 Goodbye</t>
-  </si>
-  <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 31, FadeOut 0.1 PositionCell, SetHealth 0, FadeIn 1.0 Goodbye</t>
-  </si>
-  <si>
     <t>I haven't spoken with them in so long. I thought, foolishly, that they would want to speak with me given how long it has been and that I'm the last one of the family alive. But I thought wrong, even in death they want nothing to do with me. Nothing! They can't see past who they think I am, so they don't see the woman that I am and always have been. Aren't families supposed to love each other unconditionally?</t>
   </si>
   <si>
@@ -841,6 +787,78 @@
   </si>
   <si>
     <t>tlvoat_PCMentionInTemple = 1</t>
+  </si>
+  <si>
+    <t>Did you find the time to clear the tomb for me?</t>
+  </si>
+  <si>
+    <t>You are one of the new presences that I can feel in this resting place. You are a stranger, yet the other feels strangely familier. Bring them to me so I can see who they are.</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 30, FadeOut 0.1, ModDisposition 5, PositionCell, FadeIn 1.0 Goodbye</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 31, FadeOut 0.1, ModDisposition 5, PositionCell, SetHealth 0, FadeIn 1.0 Goodbye</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.journal &lt;= 50</t>
+  </si>
+  <si>
+    <t>While most of my family continue to push me away, I hope my grandmother does not react in the same way.</t>
+  </si>
+  <si>
+    <t>Any luck with the shrine?</t>
+  </si>
+  <si>
+    <t>if tlvoat_uravasaMetPC == 1: Choice "Not only have I found a hidden section, but your grandmother spoke to me.", 4 ELSE Choice "Not yet.", 5</t>
+  </si>
+  <si>
+    <t>What? That's incredible! Please lead me to her.</t>
+  </si>
+  <si>
+    <t>Ah, ok. I'll continue waiting here.</t>
+  </si>
+  <si>
+    <t>set tlvoat_Estranged_Spirits to 50, AiFollow 0 0 0 0, Goodbye</t>
+  </si>
+  <si>
+    <t>Let's get to this secret part of the tomb as quickly as we can.</t>
+  </si>
+  <si>
+    <t>FadeOut 1.0 Player-&gt;PositionCell Goodbye FadeIn 1.0</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 60</t>
+  </si>
+  <si>
+    <t>All guardians in Othral Ancestral Tomb have been dispatched.</t>
+  </si>
+  <si>
+    <t>I have let Aryasi Othral know that her family's tomb is safe for her to enter.</t>
+  </si>
+  <si>
+    <t>I lied to Aryasi Othral that her family's tomb has been cleared of its guardians.</t>
+  </si>
+  <si>
+    <t>I have met a woman named Aryasi Othral who wants to enter her family's tomb, but cant't as it's unsafe even for her as the tomb's guardians will kill her. She wants me to clear the tomb so that it's safe for her.</t>
+  </si>
+  <si>
+    <t>Aryasi Othral wants to speak to her grandmother's spirit, but can't reach her. She mentioned that there might be a hidden section of Othral Ancestral Tomb. I offered to help find it.</t>
+  </si>
+  <si>
+    <t>I have lead Aryasi Othral to her grandmother's spirit.</t>
+  </si>
+  <si>
+    <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. She gave me a ring that was her mother's.</t>
+  </si>
+  <si>
+    <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. I turned down her reward.</t>
+  </si>
+  <si>
+    <t>tlvoat_othral_quest_glb_script</t>
+  </si>
+  <si>
+    <t>Handles timer &amp; Aryasi PositionCell</t>
   </si>
 </sst>
 </file>
@@ -1453,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
-  <dimension ref="A2:E8"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1482,10 +1500,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1494,7 +1512,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1502,33 +1520,33 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1536,16 +1554,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1553,16 +1571,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1570,16 +1588,30 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>193</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1673,7 +1705,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1708,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
   <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1744,10 +1776,10 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1755,16 +1787,19 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>220</v>
+        <v>264</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+      <c r="F4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1772,16 +1807,13 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>140</v>
+        <v>261</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1792,16 +1824,19 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>141</v>
+        <v>262</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="F6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1809,16 +1844,16 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>143</v>
+        <v>263</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1829,16 +1864,13 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>145</v>
+        <v>265</v>
       </c>
       <c r="D8">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F8" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1849,16 +1881,16 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D9">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1866,16 +1898,13 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>147</v>
+        <v>266</v>
       </c>
       <c r="D10">
-        <v>50</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1883,16 +1912,13 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>149</v>
+        <v>267</v>
       </c>
       <c r="D11">
         <v>100</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1903,16 +1929,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="D12">
         <v>101</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" t="s">
         <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1923,16 +1946,16 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="D13">
         <v>200</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1943,16 +1966,16 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D14">
         <v>300</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1963,20 +1986,20 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="D15">
         <v>400</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F5 B6:E34 F7:F8 F11 F13:F14">
+  <conditionalFormatting sqref="F6:F7 F11 F13:F14 B5:E34 B3:F4">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2028,237 +2051,237 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
         <v>95</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" t="s">
         <v>97</v>
-      </c>
-      <c r="D7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" t="s">
         <v>110</v>
-      </c>
-      <c r="D24" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2268,10 +2291,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F50"/>
+  <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2308,16 +2331,16 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2328,16 +2351,16 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" t="s">
         <v>115</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2348,13 +2371,13 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="F5" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2365,13 +2388,13 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="F6" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2382,13 +2405,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="F7" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2399,33 +2422,33 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="F9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2433,50 +2456,50 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="F10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="F11" t="s">
-        <v>123</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
       <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2487,16 +2510,13 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>119</v>
+        <v>185</v>
       </c>
       <c r="F13" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2507,16 +2527,19 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="F14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2524,224 +2547,224 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="F15" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
       <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F20" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F21" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="F22" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F23" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F24" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F25" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="F26" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2752,19 +2775,19 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="F27" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2772,16 +2795,16 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="F28" t="s">
-        <v>170</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2792,19 +2815,19 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>129</v>
+        <v>233</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="F29" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2812,16 +2835,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>181</v>
+        <v>124</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>183</v>
+        <v>245</v>
       </c>
       <c r="F30" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2832,16 +2855,16 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="F31" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2852,16 +2875,16 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="F32" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2872,16 +2895,16 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="F33" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2892,16 +2915,19 @@
         <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>196</v>
+        <v>125</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="F34" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2909,13 +2935,16 @@
         <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+      <c r="F35" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2923,215 +2952,206 @@
         <v>29</v>
       </c>
       <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>184</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F38" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>184</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" t="s">
+        <v>184</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F41" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" t="s">
+        <v>184</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F42" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" t="s">
+        <v>184</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F43" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F36" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" t="s">
-        <v>197</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F37" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" t="s">
-        <v>197</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="E45" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F38" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" t="s">
-        <v>197</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F39" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" t="s">
-        <v>197</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F40" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" t="s">
-        <v>197</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F41" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" t="s">
-        <v>197</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F43" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F44" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" t="s">
-        <v>114</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F45" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" t="s">
-        <v>114</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F46" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" t="s">
-        <v>114</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F47" t="s">
-        <v>218</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3139,63 +3159,140 @@
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>230</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F48" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F50" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F51" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>215</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F52" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>215</v>
+      </c>
+      <c r="C53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F53" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>215</v>
+      </c>
+      <c r="C54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F48" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" t="s">
-        <v>230</v>
-      </c>
-      <c r="C49" t="s">
-        <v>116</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F49" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" t="s">
-        <v>230</v>
-      </c>
-      <c r="C50" t="s">
-        <v>116</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F50" t="s">
-        <v>234</v>
+      <c r="F54" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F77">
+  <conditionalFormatting sqref="B3:F81">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -3204,7 +3301,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D1:D1048576" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D1:D50 D51:D1048576" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
       <formula1>512</formula1>
     </dataValidation>
   </dataValidations>
@@ -3216,7 +3313,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A1048576</xm:sqref>
+          <xm:sqref>A1:A50 A51:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3263,7 +3360,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3326,16 +3423,16 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3343,16 +3440,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3360,16 +3457,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3432,13 +3529,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3446,13 +3543,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3460,13 +3557,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3474,13 +3571,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3488,13 +3585,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3502,13 +3599,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3571,7 +3668,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
@@ -3585,7 +3682,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -3596,10 +3693,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -3610,16 +3707,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3627,16 +3724,16 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3644,16 +3741,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3661,16 +3758,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: second FadeOut/In at end of quest to be an hour long wait
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B571C1BC-5773-446F-B6C2-237967145BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C73D8E9-6F0D-465F-B4A5-1D91E75182D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="277">
   <si>
     <t>Name</t>
   </si>
@@ -417,9 +417,6 @@
     <t>escorting, completed escort</t>
   </si>
   <si>
-    <t>Ah! This is her! Oh thank you, thank you so much for taking me to my grandmother. Please, leave me for a while so that I may speak with her spirit.</t>
-  </si>
-  <si>
     <t>Have you changed your mind?</t>
   </si>
   <si>
@@ -453,9 +450,6 @@
     <t>Let Aryasi know it's safe, both accepted before &amp; not accepted. Starts quest if latter</t>
   </si>
   <si>
-    <t>Aryasi Othral wants me to lead her to where her grandmother has been laid to rest.</t>
-  </si>
-  <si>
     <t>Let Aryasi know it's safe, both accepted before &amp; not accepted. Starts quest if latter. Kills Aryasi</t>
   </si>
   <si>
@@ -795,12 +789,6 @@
     <t>You are one of the new presences that I can feel in this resting place. You are a stranger, yet the other feels strangely familier. Bring them to me so I can see who they are.</t>
   </si>
   <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 30, FadeOut 0.1, ModDisposition 5, PositionCell, FadeIn 1.0 Goodbye</t>
-  </si>
-  <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 31, FadeOut 0.1, ModDisposition 5, PositionCell, SetHealth 0, FadeIn 1.0 Goodbye</t>
-  </si>
-  <si>
     <t>tlvoat_Estranged_Spirits.journal &lt;= 50</t>
   </si>
   <si>
@@ -825,30 +813,12 @@
     <t>Let's get to this secret part of the tomb as quickly as we can.</t>
   </si>
   <si>
-    <t>FadeOut 1.0 Player-&gt;PositionCell Goodbye FadeIn 1.0</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal == 60</t>
-  </si>
-  <si>
     <t>All guardians in Othral Ancestral Tomb have been dispatched.</t>
   </si>
   <si>
-    <t>I have let Aryasi Othral know that her family's tomb is safe for her to enter.</t>
-  </si>
-  <si>
-    <t>I lied to Aryasi Othral that her family's tomb has been cleared of its guardians.</t>
-  </si>
-  <si>
     <t>I have met a woman named Aryasi Othral who wants to enter her family's tomb, but cant't as it's unsafe even for her as the tomb's guardians will kill her. She wants me to clear the tomb so that it's safe for her.</t>
   </si>
   <si>
-    <t>Aryasi Othral wants to speak to her grandmother's spirit, but can't reach her. She mentioned that there might be a hidden section of Othral Ancestral Tomb. I offered to help find it.</t>
-  </si>
-  <si>
-    <t>I have lead Aryasi Othral to her grandmother's spirit.</t>
-  </si>
-  <si>
     <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. She gave me a ring that was her mother's.</t>
   </si>
   <si>
@@ -859,6 +829,54 @@
   </si>
   <si>
     <t>Handles timer &amp; Aryasi PositionCell</t>
+  </si>
+  <si>
+    <t>StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 30, ModDisposition 5, StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 31, ModDisposition 5, StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
+  </si>
+  <si>
+    <t>%PCName! Thank you for waiting, my grandmother and I have been talking things over and things are awkward, but progressing well. My hopes that she would be accepting have been true.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 70</t>
+  </si>
+  <si>
+    <t>I should speak with Aryasi now that she's had time to speak to her grandmother's spirit.</t>
+  </si>
+  <si>
+    <t>I have lead Aryasi to her grandmother's spirit.</t>
+  </si>
+  <si>
+    <t>Aryasi wants me to lead her to where her grandmother has been laid to rest.</t>
+  </si>
+  <si>
+    <t>I have let Aryasi know that her family's tomb is safe for her to enter.</t>
+  </si>
+  <si>
+    <t>I lied to Aryasi  that her family's tomb has been cleared of its guardians.</t>
+  </si>
+  <si>
+    <t>Aryasi wants to speak to her grandmother's spirit, but can't reach her. She mentioned that there might be a hidden section of Othral Ancestral Tomb. I offered to help find it.</t>
+  </si>
+  <si>
+    <t>Finished waiting</t>
+  </si>
+  <si>
+    <t>Ah! This is her! Oh thank you, thank you so much for taking me to my grandmother. Please, leave us for an hour so that we talk things over.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 60, tlvoat_isTalkingToUravasa = 1</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 60, tlvoat_isTalkingToUravasa = 0</t>
+  </si>
+  <si>
+    <t>Please give us some time to speak.</t>
   </si>
 </sst>
 </file>
@@ -1473,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
   <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1520,16 +1538,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1537,16 +1555,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1554,7 +1572,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1563,7 +1581,7 @@
         <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1588,16 +1606,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1605,13 +1623,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1723,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1738,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
-  <dimension ref="A2:F15"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1776,7 +1794,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1787,16 +1805,16 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1807,13 +1825,13 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1824,16 +1842,16 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1844,16 +1862,16 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D7">
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" t="s">
         <v>136</v>
-      </c>
-      <c r="F7" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1864,7 +1882,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D8">
         <v>40</v>
@@ -1873,7 +1891,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1881,7 +1899,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>135</v>
+        <v>268</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -1898,13 +1916,13 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D10">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1912,16 +1930,16 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D11">
-        <v>100</v>
-      </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1929,10 +1947,10 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="D12">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
         <v>36</v>
@@ -1946,19 +1964,16 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>201</v>
+        <v>258</v>
       </c>
       <c r="D13">
-        <v>200</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>200</v>
+        <v>101</v>
       </c>
       <c r="F13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1966,19 +1981,19 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>139</v>
+        <v>199</v>
       </c>
       <c r="D14">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1986,20 +2001,40 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>206</v>
+        <v>137</v>
       </c>
       <c r="D15">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>37</v>
+        <v>197</v>
       </c>
       <c r="F15" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16">
+        <v>400</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F6:F7 F11 F13:F14 B5:E34 B3:F4">
+  <conditionalFormatting sqref="B3:F4 F6:F7 F12 F14:F15 B5:E35">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2260,7 +2295,7 @@
         <v>118</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -2273,7 +2308,7 @@
         <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -2281,7 +2316,7 @@
         <v>107</v>
       </c>
       <c r="D28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2291,10 +2326,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F54"/>
+  <dimension ref="A2:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2334,7 +2369,7 @@
         <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>116</v>
@@ -2354,7 +2389,7 @@
         <v>112</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>116</v>
@@ -2374,10 +2409,10 @@
         <v>113</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2391,10 +2426,10 @@
         <v>113</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2408,10 +2443,10 @@
         <v>113</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2425,10 +2460,10 @@
         <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2442,10 +2477,10 @@
         <v>113</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2459,10 +2494,10 @@
         <v>113</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2476,10 +2511,10 @@
         <v>113</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2493,7 +2528,7 @@
         <v>113</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>116</v>
@@ -2513,10 +2548,10 @@
         <v>113</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2530,13 +2565,13 @@
         <v>113</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2550,10 +2585,10 @@
         <v>113</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2567,10 +2602,10 @@
         <v>113</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2584,13 +2619,13 @@
         <v>113</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>116</v>
       </c>
       <c r="F17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2604,16 +2639,16 @@
         <v>113</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>123</v>
+        <v>273</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F18" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2621,16 +2656,16 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>234</v>
+        <v>276</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="F19" t="s">
-        <v>156</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2641,19 +2676,16 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>182</v>
+        <v>264</v>
       </c>
       <c r="F20" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2664,16 +2696,16 @@
         <v>106</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>162</v>
+        <v>232</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F21" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2684,16 +2716,16 @@
         <v>106</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="F22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -2704,13 +2736,13 @@
         <v>106</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>244</v>
+        <v>162</v>
       </c>
       <c r="F23" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2724,10 +2756,13 @@
         <v>106</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>176</v>
+        <v>234</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="F24" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2741,13 +2776,13 @@
         <v>106</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="F25" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2761,10 +2796,10 @@
         <v>106</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>241</v>
+        <v>174</v>
       </c>
       <c r="F26" t="s">
-        <v>237</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2778,16 +2813,16 @@
         <v>106</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F27" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2800,14 +2835,11 @@
       <c r="D28" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="F28" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2818,16 +2850,16 @@
         <v>106</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="F29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2838,16 +2870,16 @@
         <v>106</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="F30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2858,16 +2890,16 @@
         <v>106</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>168</v>
+        <v>231</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
       <c r="F31" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -2878,13 +2910,13 @@
         <v>106</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>173</v>
+        <v>243</v>
       </c>
       <c r="F32" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2898,13 +2930,13 @@
         <v>106</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>126</v>
+        <v>166</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F33" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2918,13 +2950,13 @@
         <v>106</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>125</v>
+        <v>167</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F34" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2938,13 +2970,16 @@
         <v>106</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>183</v>
+        <v>125</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="F35" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2955,186 +2990,186 @@
         <v>106</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F36" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>182</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>182</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" t="s">
+        <v>182</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F43" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
+        <v>182</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F44" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" t="s">
+        <v>182</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F45" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>182</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" t="s">
-        <v>184</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F37" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" t="s">
-        <v>184</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F38" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" t="s">
-        <v>184</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F39" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" t="s">
-        <v>184</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F40" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" t="s">
-        <v>184</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F41" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" t="s">
-        <v>184</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F42" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" t="s">
-        <v>184</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="F43" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" t="s">
-        <v>184</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" t="s">
-        <v>111</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F45" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F46" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3145,13 +3180,13 @@
         <v>111</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F47" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3165,16 +3200,13 @@
         <v>111</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>257</v>
+        <v>196</v>
       </c>
       <c r="F48" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -3185,13 +3217,16 @@
         <v>111</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>256</v>
+        <v>200</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="F49" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3202,16 +3237,16 @@
         <v>111</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="F50" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -3222,77 +3257,114 @@
         <v>111</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F51" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>215</v>
+        <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="F52" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>215</v>
+        <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>223</v>
+        <v>250</v>
       </c>
       <c r="F53" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C54" t="s">
         <v>113</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F54" t="s">
         <v>220</v>
       </c>
-      <c r="E54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>213</v>
+      </c>
+      <c r="C55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F55" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>213</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F54" t="s">
-        <v>219</v>
+      <c r="F56" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F81">
+  <conditionalFormatting sqref="B3:F83">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -3301,7 +3373,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D1:D50 D51:D1048576" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D1:D1048576" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
       <formula1>512</formula1>
     </dataValidation>
   </dataValidations>
@@ -3313,7 +3385,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A50 A51:A1048576</xm:sqref>
+          <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3423,7 +3495,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
         <v>55</v>
@@ -3535,7 +3607,7 @@
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3549,7 +3621,7 @@
         <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3563,7 +3635,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3668,7 +3740,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Add: end of the quest
Update: removed ghost, replaced with quest/story focus on the urn
Add: TODO list
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C73D8E9-6F0D-465F-B4A5-1D91E75182D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFEF1B2-83D3-4394-8296-767699D67FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="283">
   <si>
     <t>Name</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Dark Elf</t>
   </si>
   <si>
-    <t>Ancester Ghost</t>
-  </si>
-  <si>
     <t>Door</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>Urn Labelled "Uravasa Othral"</t>
   </si>
   <si>
-    <t>Uravasa Othral's Ghost</t>
-  </si>
-  <si>
     <t>Armour</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>Weapon</t>
   </si>
   <si>
-    <t>lvl 20</t>
-  </si>
-  <si>
     <t>lvl 5</t>
   </si>
   <si>
@@ -696,24 +687,6 @@
     <t>If Distance Player &lt;= 512: ForceGreeting</t>
   </si>
   <si>
-    <t>You’re the new presence that I felt in the resting place of myself and the spirits of my family. Leave now, or I will make this tomb your resting place too.</t>
-  </si>
-  <si>
-    <t>Talked to PC = 1</t>
-  </si>
-  <si>
-    <t>Why are you continuing to linger in this sacred place?</t>
-  </si>
-  <si>
-    <t>Talked to PC = 0, tlvoat_Estranged_Spirits.Journal &gt;= 30</t>
-  </si>
-  <si>
-    <t>Talked to PC = 0, tlvoat_Estranged_Spirits.Journal &lt; 30</t>
-  </si>
-  <si>
-    <t>set tlvoat_uravasaMetPC to 1, Goodbye</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal &lt;= 20, tlvoat_hasPCSaidInTemple = 1</t>
   </si>
   <si>
@@ -786,9 +759,6 @@
     <t>Did you find the time to clear the tomb for me?</t>
   </si>
   <si>
-    <t>You are one of the new presences that I can feel in this resting place. You are a stranger, yet the other feels strangely familier. Bring them to me so I can see who they are.</t>
-  </si>
-  <si>
     <t>tlvoat_Estranged_Spirits.journal &lt;= 50</t>
   </si>
   <si>
@@ -798,9 +768,6 @@
     <t>Any luck with the shrine?</t>
   </si>
   <si>
-    <t>if tlvoat_uravasaMetPC == 1: Choice "Not only have I found a hidden section, but your grandmother spoke to me.", 4 ELSE Choice "Not yet.", 5</t>
-  </si>
-  <si>
     <t>What? That's incredible! Please lead me to her.</t>
   </si>
   <si>
@@ -819,9 +786,6 @@
     <t>I have met a woman named Aryasi Othral who wants to enter her family's tomb, but cant't as it's unsafe even for her as the tomb's guardians will kill her. She wants me to clear the tomb so that it's safe for her.</t>
   </si>
   <si>
-    <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. She gave me a ring that was her mother's.</t>
-  </si>
-  <si>
     <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. I turned down her reward.</t>
   </si>
   <si>
@@ -877,6 +841,60 @@
   </si>
   <si>
     <t>Please give us some time to speak.</t>
+  </si>
+  <si>
+    <t>grandmother's ring</t>
+  </si>
+  <si>
+    <t>Here I want you to have my grandmother's ring. It was one of the things that I took when I ran away. I thought my grandmother would be angry when I spoke to her, but it turns out she always wanted me to have it. My parents twisted things to deny even this. And yes she is happy with me rewarding this to you, as it's basically mine now to do with as I please.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 70</t>
+  </si>
+  <si>
+    <t>tlvoat_ring_matriarch_unique</t>
+  </si>
+  <si>
+    <t>Ring of the Matriarch</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Choice "[Take the ring] Thank you.", 1, "[Refuse the ring] No reward is necessary.", 2</t>
+  </si>
+  <si>
+    <t>I'm sure that you can put this to good use. I hope that we can meet again someday.</t>
+  </si>
+  <si>
+    <t>Oh! Of course, you are humble. I hope that we can meet again someday.</t>
+  </si>
+  <si>
+    <t>Choice = 2, tlvoat_PCMentionInTemple = 1</t>
+  </si>
+  <si>
+    <t>My apologies sera %PCName, I forgot that priests do not usually accept gifts and rewards for acts of service. Well, I hope that we can meet again someday.</t>
+  </si>
+  <si>
+    <t>Player-&gt;AddItem "tlvoat_ring_matriarch_unique", 1; Journal "tlvoat_Estranged_Spirits", 100</t>
+  </si>
+  <si>
+    <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. She gave me a ring that was her grandmother's.</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 101</t>
+  </si>
+  <si>
+    <t>tlvoat_urn_uravasa_uni_script</t>
+  </si>
+  <si>
+    <t>Handles distance check with PC</t>
+  </si>
+  <si>
+    <t>I have found Uravasa Othral's resting place.</t>
+  </si>
+  <si>
+    <t>if GetJournalIndex == 45: Choice "Not only have I found a hidden section, but your grandmother has been laid to rest there.", 4 ELSE Choice "Not yet.", 5</t>
   </si>
 </sst>
 </file>
@@ -1489,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1521,7 +1539,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1530,7 +1548,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1538,16 +1556,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1555,16 +1573,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1572,16 +1590,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1589,16 +1607,16 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1606,16 +1624,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1623,13 +1641,30 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>260</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1723,7 +1758,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1756,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1794,7 +1829,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1805,16 +1840,16 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1825,13 +1860,13 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1842,16 +1877,16 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
         <v>133</v>
-      </c>
-      <c r="F6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1862,16 +1897,16 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="D7">
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1882,30 +1917,27 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="D8">
         <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="D9">
-        <v>50</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1916,13 +1948,16 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D10">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1930,16 +1965,13 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="D11">
-        <v>70</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1947,16 +1979,16 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D12">
-        <v>100</v>
-      </c>
-      <c r="F12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1964,13 +1996,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="D13">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1981,19 +2013,16 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>199</v>
+        <v>246</v>
       </c>
       <c r="D14">
-        <v>200</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>198</v>
+        <v>101</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2001,19 +2030,19 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="D15">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2021,20 +2050,40 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>204</v>
+        <v>134</v>
       </c>
       <c r="D16">
+        <v>300</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17">
         <v>400</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E17" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F4 F6:F7 F12 F14:F15 B5:E35">
+  <conditionalFormatting sqref="B3:F4 F6:F7 F13 F15:F16 B5:E36">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2086,237 +2135,237 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
         <v>92</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" t="s">
         <v>94</v>
-      </c>
-      <c r="D7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" t="s">
         <v>107</v>
-      </c>
-      <c r="D24" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D28" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2326,10 +2375,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F56"/>
+  <dimension ref="A2:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2366,16 +2415,16 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2386,16 +2435,16 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" t="s">
         <v>112</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2406,13 +2455,13 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="F5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2423,13 +2472,13 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2440,13 +2489,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="F7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2457,13 +2506,13 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="F8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2474,13 +2523,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="F9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2491,13 +2540,13 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2508,13 +2557,13 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2525,16 +2574,16 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="F12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2545,13 +2594,13 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2562,16 +2611,16 @@
         <v>29</v>
       </c>
       <c r="C14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="F14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2582,13 +2631,13 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2599,13 +2648,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2616,16 +2665,16 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="F17" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2636,16 +2685,16 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="F18" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2656,16 +2705,16 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="F19" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2676,13 +2725,13 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="F20" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -2693,16 +2742,16 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2713,16 +2762,16 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2733,16 +2782,16 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2753,16 +2802,16 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F24" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2773,16 +2822,16 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="F25" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2793,13 +2842,13 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F26" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2810,16 +2859,16 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="F27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,13 +2879,13 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F28" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2847,16 +2896,16 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="F29" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2867,16 +2916,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="F30" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2887,16 +2936,16 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="F31" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2907,16 +2956,16 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="F32" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2927,16 +2976,16 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F33" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2947,16 +2996,16 @@
         <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F34" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2967,16 +3016,16 @@
         <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F35" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2987,16 +3036,16 @@
         <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F36" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3007,13 +3056,13 @@
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F37" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3024,10 +3073,10 @@
         <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
@@ -3038,16 +3087,16 @@
         <v>29</v>
       </c>
       <c r="C39" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="F39" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3058,13 +3107,13 @@
         <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F40" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3075,13 +3124,13 @@
         <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F41" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -3092,13 +3141,13 @@
         <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F42" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3109,16 +3158,16 @@
         <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F43" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3129,13 +3178,13 @@
         <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F44" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3146,13 +3195,13 @@
         <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="F45" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -3163,10 +3212,10 @@
         <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -3177,16 +3226,16 @@
         <v>29</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F47" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3197,13 +3246,13 @@
         <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F48" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3214,16 +3263,16 @@
         <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F49" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3234,16 +3283,16 @@
         <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="F50" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -3254,13 +3303,13 @@
         <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="F51" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -3271,16 +3320,16 @@
         <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F52" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3291,56 +3340,56 @@
         <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="F53" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>213</v>
+        <v>29</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>265</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>216</v>
+        <v>272</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>221</v>
+        <v>276</v>
       </c>
       <c r="F54" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>213</v>
+        <v>29</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>265</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>221</v>
+        <v>278</v>
       </c>
       <c r="F55" t="s">
-        <v>219</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -3348,23 +3397,43 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>213</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
-        <v>113</v>
+        <v>265</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>218</v>
+        <v>273</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>116</v>
+        <v>278</v>
       </c>
       <c r="F56" t="s">
-        <v>217</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" t="s">
+        <v>265</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F57" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F83">
+  <conditionalFormatting sqref="B3:F84">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -3432,7 +3501,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3467,10 +3536,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E963F2BA-EA95-4418-AB9C-44FAC2775617}">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A2:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3495,16 +3564,16 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3512,37 +3581,20 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3:E5 B3:D32">
+  <conditionalFormatting sqref="E3:E4 B3:D31">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -3573,10 +3625,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65134921-D347-4BBE-A2AC-6E1606FA8DED}">
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3601,13 +3653,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3615,13 +3667,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3629,13 +3681,13 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3643,13 +3695,13 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3657,13 +3709,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3671,13 +3723,27 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D9" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3715,7 +3781,7 @@
   <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3740,10 +3806,10 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -3754,7 +3820,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -3765,10 +3831,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -3779,16 +3845,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3796,16 +3862,16 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3813,16 +3879,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3830,16 +3896,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: many many more dialogue lines and journal entries to accomodate PC choice in progressing the quest
* Update: most dialogue lines to fix typos, and to sound more natural and convey needed info to PC
* Fix: "spirits of my family" topic being added too early
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFEF1B2-83D3-4394-8296-767699D67FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84300DBF-DADF-46ED-8FEC-DC58B70C00AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="328">
   <si>
     <t>Name</t>
   </si>
@@ -399,9 +399,6 @@
     <t>ask for help, ask when PC attempted to go in, ask if PC changed mind, ask if PC cleared tomb anyway, malePC nude, femalePC nude</t>
   </si>
   <si>
-    <t>tlvoat_estranged_spirits.Journal &gt;= updated, unable to clear</t>
-  </si>
-  <si>
     <t>asks if PC found secret area, asks if PC found secret area (temple)</t>
   </si>
   <si>
@@ -411,12 +408,6 @@
     <t>Have you changed your mind?</t>
   </si>
   <si>
-    <t>Ah, %PCName! Is it safe to go in?</t>
-  </si>
-  <si>
-    <t>Ah, %PCName! Is it safe to go in? You seem rather dirty compared to earlier.</t>
-  </si>
-  <si>
     <t>brief overview of family history, joyous she can reconnect</t>
   </si>
   <si>
@@ -429,9 +420,6 @@
     <t>Thank you again for making it safe for me</t>
   </si>
   <si>
-    <t>Yes! I'm so happy that I've been able to reconnect with my grandmother.</t>
-  </si>
-  <si>
     <t>Met Othral/attempted to enter tomb, accepted/accepted after initial decline</t>
   </si>
   <si>
@@ -486,9 +474,6 @@
     <t>How is the tomb? Is it safe for me to go in?</t>
   </si>
   <si>
-    <t>Please %PCName I need time to myself. I don't know what it is that I'm feeling, and I need to sort myself out.</t>
-  </si>
-  <si>
     <t>Talked to PC = 0, tlvoat_hasPCAttemptEnter = 0, tlvoat_hasPCEnteredTomb = 0</t>
   </si>
   <si>
@@ -528,33 +513,12 @@
     <t>Journal "tlvoat_Estranged_Spirits", 5</t>
   </si>
   <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 4</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal &lt;= 5, tlvoat_hasPCEnteredTomb = 1, tlvoat_tombClearCount &gt;= 5</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal &lt;= 5, tlvoat_hasPCEnteredTomb = 1, tlvoat_tombClearCount &lt; 5</t>
-  </si>
-  <si>
-    <t>I saw that you went into my family's tomb. Did you happen to clear it anyway? You seem rather dirty compared to earlier.</t>
-  </si>
-  <si>
-    <t>I saw that you went into my family's tomb. Did you happen to clear it anyway?</t>
-  </si>
-  <si>
-    <t>Choice "Yes, the tomb is now safe.", 5, "No, it's not safe for you to enter.", 6</t>
-  </si>
-  <si>
     <t>Choice = 5</t>
   </si>
   <si>
     <t>Choice = 7</t>
   </si>
   <si>
-    <t>Choice "(Lie) Yes, the tomb is now safe.", 7, "No, it's not safe for you to enter.", 6</t>
-  </si>
-  <si>
     <t>Choice = 6</t>
   </si>
   <si>
@@ -564,12 +528,6 @@
     <t>Ok, I'll just keep waiting here.</t>
   </si>
   <si>
-    <t>tlvoat_estranged_spirits.Journal == 20, tlvoat_skeleton Dead &gt;= 5, tlvoat_skeleton_archer &gt;= 1</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal == 10, tlvoat_skeleton Dead &lt; 5, tlvoat_skeleton_archer &lt; 1</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal &lt;= 20</t>
   </si>
   <si>
@@ -582,9 +540,6 @@
     <t>Journal "tlvoat_Estranged_Spirits", 10, set tlvoat_hasPCSaidInTemple to 1</t>
   </si>
   <si>
-    <t>Thank you again sera %PCName for making my family's tomb safe enough for me to speak with them. I've never met a priest like you before.</t>
-  </si>
-  <si>
     <t>spirits of my family</t>
   </si>
   <si>
@@ -597,36 +552,12 @@
     <t>if PC in Temple: Choice "I'm sorry to hear that your family pushed you away.", 2, "Was there anyone in your family who you had a good relationship with?", 3, "Just as Ghostfence is a monument to Dunmer pride in overcoming our enemies, so too should you in standing up for yourself against a family that should know better.", 4 ELSE Choice "I'm sorry to hear that your family pushed you away.", 2, "Was there anyone in your family who you had a good relationship with?", 3</t>
   </si>
   <si>
-    <t>Thank you %PCName. Coming here has brought up so many old feelings that I've kept so very deeply buried. It hurts all the more that I don't even hear my grandmother's spirit, as she was the only one I ever had a good relationship with. I used to suspect that there is a hidden section of the tomb, and I am once again hoping there is one and that she was laid to rest there.</t>
-  </si>
-  <si>
-    <t>Yes, there was: my grandmother. I can't hear her either, which makes everything hurt all the more. I find myself hoping that there's a hidden section of the tomb, just as I once did.</t>
-  </si>
-  <si>
-    <t>tlvoat_hasAskedAboutSpirits = 0</t>
-  </si>
-  <si>
     <t>Choice "Continue", 1, set tlvoat_hasAskedAboutSpirits to 1</t>
   </si>
   <si>
     <t>tlvoat_estranged_spirits.Journal == 30, tlvoat_hasAskedAboutSpirits = 1</t>
   </si>
   <si>
-    <t>They are remaining silent. I can't help but hope that my grandmother is in a hidden section.</t>
-  </si>
-  <si>
-    <t>I… Thank you %PCName… That means a lot to me. [she is silent for a minute] I've always felt like a coward or that I'm weak for running away. Everything that I've done has been to be someone not like my family at all. I think I've been hurting myself. I had hoped to speak to my grandmother, but she too is silent. I once suspected that there is a hidden section in this tomb, and I can feel hope rising that this is the case.</t>
-  </si>
-  <si>
-    <t>Whenever I asked my parents they always denied it, but every time my mother expressed missing grandmother she would come to the tomb. On one of these times I followed her and watched as she prayed at the shrine, then after a while, she reached out to it and I heard something heavy move elsewhere in the tomb. But that was when she caught me and I dragged me out. I investigated the shrine a few other times when I was alone, but found nothing. Maybe some fresh hands could reveal something?</t>
-  </si>
-  <si>
-    <t>If PCFoundSecret: Choice "I found a button hidden on the shrine and pressed it.", 4 ELSE Choice "I could take a look for you.", 1, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3</t>
-  </si>
-  <si>
-    <t>You will? Thank you! I'll be waiting right here.</t>
-  </si>
-  <si>
     <t>Of course, you have done a lot for me already. I'll take a look, and if you change your mind I'll be right here.</t>
   </si>
   <si>
@@ -648,9 +579,6 @@
     <t>tlvoat_Estranged_Spirits.Journal == 30</t>
   </si>
   <si>
-    <t>tlvoat_Estranged_Spirits.Journal == 40</t>
-  </si>
-  <si>
     <t>I have killed Aryasi Othral. Her death should give her the opportunity to speak with her ancesters.</t>
   </si>
   <si>
@@ -663,21 +591,9 @@
     <t>Thank you again for clearing my family's tomb %PCClass, but right now I'd prefer to be alone.</t>
   </si>
   <si>
-    <t>tlvoat_Estranged_Spirits.Journal &gt;= 200</t>
-  </si>
-  <si>
-    <t>tlvoat_Estranged_Spirits.Journal = 40</t>
-  </si>
-  <si>
-    <t>tlvoat_Estranged_Spirits.Journal = 40, tlvoat_hasPCSaidInTemple == 1</t>
-  </si>
-  <si>
     <t>Sera, I hope searching for this hidden section isn't too much trouble for you.</t>
   </si>
   <si>
-    <t>Hey %PCName, have you found any hidden section of the tomb? Has the shrine been keeping a secret all these years?</t>
-  </si>
-  <si>
     <t>tlvoat_uravasa_ghost_u</t>
   </si>
   <si>
@@ -693,33 +609,12 @@
     <t>tlvoat_estranged_spirits.Journal == 50</t>
   </si>
   <si>
-    <t>I haven't spoken with them in so long. I thought, foolishly, that they would want to speak with me given how long it has been and that I'm the last one of the family alive. But I thought wrong, even in death they want nothing to do with me. Nothing! They can't see past who they think I am, so they don't see the woman that I am and always have been. Aren't families supposed to love each other unconditionally?</t>
-  </si>
-  <si>
     <t>OnActivate: ForceGreeting Aryasi if not yet spoken, aryasi.hasPCAttemptEnter to 1; set hasPCEntered to 1</t>
   </si>
   <si>
     <t>tlvoat_ex_othral_door_script</t>
   </si>
   <si>
-    <t>I saw that you went into my family's tomb, and did you happen to clear the tomb so that it's safe for me to go in?</t>
-  </si>
-  <si>
-    <t>Hello %PCClass, I'm trying to work up the courage to enter my family's resting place, as the guardian spirits are hostile even to me. Meaning I can't get in without them killing me. So I need to find a way to clear the tomb so that I can speak to the spirits of my family.</t>
-  </si>
-  <si>
-    <t>Hey, excuse me, are you going in? I need to clear the tomb, would you be willing to help by doing this for me? Though if you don't want to I can't stop such a powerful %PCClass such as yourself.</t>
-  </si>
-  <si>
-    <t>Hello again %PCName, as you can see I'm still here waiting for help to clear the tomb or to work up the courage.</t>
-  </si>
-  <si>
-    <t>Ordinarially the guardians would leave me alone, but they aren't. Perhaps because I ran away from my family or they no longer recognise me. I can cast some simple spells but they are too numerous and powerful for me, and so I'm left with risking near certain death or help from someone else. Would you be willing to do this for me?</t>
-  </si>
-  <si>
-    <t>You will? Thank you %PCName! When you think it's safe for me, let me know. I'll be waiting here. Before you go in, please respect my family's spirits. Meaning don't disturb their remains! I don't have much to reward you with, so while I'd prefer that you didn't, you can take the objects that they once valued in life including the offerings left by those paying their respects.</t>
-  </si>
-  <si>
     <t>I'm terribly sorry sera %PCName, I did not realise that you are a priest. Thank you for granting me some of your time in helping me to connect with my family's spirits. When you think it's safe for me, let me know. I'll be waiting here.</t>
   </si>
   <si>
@@ -741,9 +636,6 @@
     <t>Oh! Right. It's a good thing to be thorough. I'll keep waiting right here.</t>
   </si>
   <si>
-    <t>It is? You seem rather untouched after dealing the tomb's guardians. Well, I trust you %PCName, thank you for putting yourself in danger for me. Give me a little while so that I may converse with my family's spirits.</t>
-  </si>
-  <si>
     <t>Choice "[Let her enter]", 10, "[Stop her] Wait, I think I may have missed a section.", 8</t>
   </si>
   <si>
@@ -756,9 +648,6 @@
     <t>tlvoat_PCMentionInTemple = 1</t>
   </si>
   <si>
-    <t>Did you find the time to clear the tomb for me?</t>
-  </si>
-  <si>
     <t>tlvoat_Estranged_Spirits.journal &lt;= 50</t>
   </si>
   <si>
@@ -777,9 +666,6 @@
     <t>set tlvoat_Estranged_Spirits to 50, AiFollow 0 0 0 0, Goodbye</t>
   </si>
   <si>
-    <t>Let's get to this secret part of the tomb as quickly as we can.</t>
-  </si>
-  <si>
     <t>All guardians in Othral Ancestral Tomb have been dispatched.</t>
   </si>
   <si>
@@ -804,9 +690,6 @@
     <t>Journal "tlvoat_Estranged_Spirits", 31, ModDisposition 5, StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
   </si>
   <si>
-    <t>%PCName! Thank you for waiting, my grandmother and I have been talking things over and things are awkward, but progressing well. My hopes that she would be accepting have been true.</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal == 70</t>
   </si>
   <si>
@@ -831,24 +714,15 @@
     <t>Finished waiting</t>
   </si>
   <si>
-    <t>Ah! This is her! Oh thank you, thank you so much for taking me to my grandmother. Please, leave us for an hour so that we talk things over.</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal == 60, tlvoat_isTalkingToUravasa = 1</t>
   </si>
   <si>
     <t>tlvoat_estranged_spirits.Journal == 60, tlvoat_isTalkingToUravasa = 0</t>
   </si>
   <si>
-    <t>Please give us some time to speak.</t>
-  </si>
-  <si>
     <t>grandmother's ring</t>
   </si>
   <si>
-    <t>Here I want you to have my grandmother's ring. It was one of the things that I took when I ran away. I thought my grandmother would be angry when I spoke to her, but it turns out she always wanted me to have it. My parents twisted things to deny even this. And yes she is happy with me rewarding this to you, as it's basically mine now to do with as I please.</t>
-  </si>
-  <si>
     <t>tlvoat_Estranged_Spirits.Journal == 70</t>
   </si>
   <si>
@@ -867,18 +741,12 @@
     <t>I'm sure that you can put this to good use. I hope that we can meet again someday.</t>
   </si>
   <si>
-    <t>Oh! Of course, you are humble. I hope that we can meet again someday.</t>
-  </si>
-  <si>
     <t>Choice = 2, tlvoat_PCMentionInTemple = 1</t>
   </si>
   <si>
     <t>My apologies sera %PCName, I forgot that priests do not usually accept gifts and rewards for acts of service. Well, I hope that we can meet again someday.</t>
   </si>
   <si>
-    <t>Player-&gt;AddItem "tlvoat_ring_matriarch_unique", 1; Journal "tlvoat_Estranged_Spirits", 100</t>
-  </si>
-  <si>
     <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. She gave me a ring that was her grandmother's.</t>
   </si>
   <si>
@@ -894,7 +762,274 @@
     <t>I have found Uravasa Othral's resting place.</t>
   </si>
   <si>
-    <t>if GetJournalIndex == 45: Choice "Not only have I found a hidden section, but your grandmother has been laid to rest there.", 4 ELSE Choice "Not yet.", 5</t>
+    <t>Hello %PCClass, I'm here to speak to my family's spirits, but the tomb is too dangerous for me. I was just considering whether to risk death, leave, or ask someone to clear the tomb for me.</t>
+  </si>
+  <si>
+    <t>Hello again %PCName, as you can see I'm still here waiting for help to clear the tomb or to work up the courage to go in alone.</t>
+  </si>
+  <si>
+    <t>%PCName it's good to see you again. Have you found some time to help me clear the tomb?</t>
+  </si>
+  <si>
+    <t>Hey, excuse me, are you going in? I need to clear the tomb, would you be willing to help me out? Though if you don't want to I can't stop a powerful %PCClass such as yourself from going in anyway.</t>
+  </si>
+  <si>
+    <t>I saw that you went in. Did you happen to clear the tomb so that it's safe even for me?</t>
+  </si>
+  <si>
+    <t>I told Aryasi that I was unable to clear her family's tomb.</t>
+  </si>
+  <si>
+    <t>Good luck in there! I hope I haven't just asked you to go to your death.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &lt;= 20, tlvoat_hasPCEnteredTomb = 0</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &lt;= 20, tlvoat_hasPCEnteredTomb = 0, tlvoat_hasPCSaidInTemple = 1</t>
+  </si>
+  <si>
+    <t>Good luck sera! I hope ALMSIVI has blessed you in helping me.</t>
+  </si>
+  <si>
+    <t>Please %PCClass I need time to myself. I don't know what it is that I'm feeling right now, and I need to sort myself out.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 200, tlvoat_hasPCSaidInTemple = 1</t>
+  </si>
+  <si>
+    <t>Thank you sera for making my family's tomb safe for me, the Temple has my gratitude. Right now though I'd prefer to be alone.</t>
+  </si>
+  <si>
+    <t>Hey %PCName, have you found any hidden section of the tomb? Was I right about the shrine?</t>
+  </si>
+  <si>
+    <t>Less talk more hurrying to my grandmother!</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &lt;= 45</t>
+  </si>
+  <si>
+    <t>Oh my! This really is her urn! Thank you so much for taking me to my grandmother. Please, leave me for an hour so that I can have some time to speak with her spirit.</t>
+  </si>
+  <si>
+    <t>Please come back to me in an hour.</t>
+  </si>
+  <si>
+    <t>Ah %PCName! Thank you for waiting, I have been able to speak with my grandmother! I never thought I'd ever be able to communicate with her again, and yet here I am. We were mere strangers, and yet, you have gone above and beyond in helping me. I don't think I'll ever be able to properly repay you, but I would like to give you my grandmother's ring.</t>
+  </si>
+  <si>
+    <t>Hello again %PCName. I'm doing very well, how are you?</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &gt;= 100</t>
+  </si>
+  <si>
+    <t>Normally the guardians would leave me alone, but it has been many years since I last visited. While I can cast some simple spells to defend myself, they are too numerous and powerful for me, and so I'm left with risking near certain death or help from someone else. Would you be willing to do this for me? I don't have much, but I can spare 50 gold.</t>
+  </si>
+  <si>
+    <t>You will? Thank you %PCName! When you think it's safe for me, let me know. I'll be waiting here. Before you go in, please respect my family's spirits. Meaning don't disturb their remains! I don't have much to reward you with, so while I'd prefer that you didn't, you can take the objects that they once valued in life. And the offerings left by those paying their respects are also yours to take.</t>
+  </si>
+  <si>
+    <t>There's a lot of guardians across all of the main rooms, so you'll need to be thorough.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &lt;= 10, tlvoat_hasPCEnteredTomb = 0</t>
+  </si>
+  <si>
+    <t>Is it safe to go in?</t>
+  </si>
+  <si>
+    <t>Choice "Yes, the tomb is now safe.", 5, "No, it's not yet safe for you to enter.", 6</t>
+  </si>
+  <si>
+    <t>Choice "(Lie) Yes, the tomb is now safe.", 7, "No, it's not yet safe for you to enter.", 6</t>
+  </si>
+  <si>
+    <t>Is it safe to go in? You do look like you've seen some scrapes.</t>
+  </si>
+  <si>
+    <t>Is it safe? You do look like you've seen some scrapes. I don't have much, but 50 gold is yours if it is.</t>
+  </si>
+  <si>
+    <t>Did you happen to clear it? I don't have much, but 50 gold is yours if it is.</t>
+  </si>
+  <si>
+    <t>It is? You seem rather untouched after dealing with the tomb's guardians. Well, I trust you %PCName, thank you for putting yourself in danger for me. Give me a little while so that I may converse with my family's spirits.</t>
+  </si>
+  <si>
+    <t>Thank you again sera %PCName for making my family's tomb safe enough for me to speak with my family. I've never met a priest like you before.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits &gt;= 30, tlvoat_hasPCReceivedReward1 = 0</t>
+  </si>
+  <si>
+    <t>Oh right I had completely forgotten that I need to give you a reward. Here's the gold that I promised you as thanks.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 30, tlvoat_hasAskedAboutSpirits = 0</t>
+  </si>
+  <si>
+    <t>I haven't spoken with them in so long. I thought, foolishly, that they would want to speak with me given how long it has been and that I'm now the last of the family still alive. But I thought wrong, even in death they want nothing to do with me. Nothing! They can't see past who they think I am, so they don't see the woman that I am and always have been. Aren't families supposed to love each other unconditionally?</t>
+  </si>
+  <si>
+    <t>Yes, there was: my grandmother. I can't hear her either, which makes everything hurt all the more. I find myself hoping that there's a hidden section of the tomb, just as I once did, and that she's there. And that's why I can't hear her, but I'm probably just letting myself be fooled by hope once again.</t>
+  </si>
+  <si>
+    <t>set tlvoat_PCMentionInTemple to 1</t>
+  </si>
+  <si>
+    <t>They are remaining silent. I can't help but hope that my grandmother is in some hidden section.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.journal &gt;= 70</t>
+  </si>
+  <si>
+    <t>I'm so happy that I've been able to reconnect with my grandmother. Thank you %PCName.</t>
+  </si>
+  <si>
+    <t>Whenever I asked my parents they always denied it, but every time my mother expressed missing grandmother she would come to the tomb. Once, I followed her and watched as she prayed at the shrine, then after a while, she reached out to it and I heard something heavy move elsewhere in the tomb. But that was when she caught me and dragged me out. I investigated the shrine a few other times when I was alone, but found nothing. Maybe some fresh hands and eyes could reveal something?</t>
+  </si>
+  <si>
+    <t>If PCFoundSecret: Choice "I have already found a switch hidden on the shrine and pressed it.", 4, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3 ELSE Choice "I could take a look for you.", 1, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3</t>
+  </si>
+  <si>
+    <t>set tlvoat_hasPCMentionSecret to 1</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &lt;= 45, tlvoat_hasPCMentionSecret = 1</t>
+  </si>
+  <si>
+    <t>set tlvoat_Estranged_Spirits to 35</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 35</t>
+  </si>
+  <si>
+    <t>If PCFoundSecret: Choice "I have already found a switch hidden on the shrine and pressed it.", 4, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3 ELSE Choice "Yes, I could take a look for you.", 1, "I still don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3</t>
+  </si>
+  <si>
+    <t>Do you now have the time to help search for it?</t>
+  </si>
+  <si>
+    <t>What's in there? Have you found my grandmother's resting place?</t>
+  </si>
+  <si>
+    <t>So I was right! I really don't want to get my hopes up too much, but please take a look. You're looking for an urn labelled "Uravasa Othral". There might also be more guardians in there so be careful.</t>
+  </si>
+  <si>
+    <t>You will? Thank you! I honestly wasn't expecting you to offer to help again. I recommend investigating the shrine first, but the switch might actually be elsewhere. If there is a hidden area then you're looking for an urn labelled "Uravasa Othral".</t>
+  </si>
+  <si>
+    <t>I told Aryasi that I could not find her grandmother's resting place in the hidden section of Othral Ancestral Tomb.</t>
+  </si>
+  <si>
+    <t>I lied to Aryasi that I could not find her grandmother's resting place in the hidden section of Othral Ancestral Tomb.</t>
+  </si>
+  <si>
+    <t>if tlvoat_hasPCFoundUrn == 1: Choice "I've found your grandmother's urn.", 5, "(Lie) I'm sorry, but there's nothing in there.", 8, "I haven't found anything yet.", 6 ELSE Choice "I'm sorry, but there's nothing in there.", 7, "I haven't found anything yet.", 6</t>
+  </si>
+  <si>
+    <t>Oh, I… thank you %PCName for looking. I'm going to need to be alone for a while.</t>
+  </si>
+  <si>
+    <t>I told Aryasi that I could not find any hidden section in Othral Ancestral Tomb.</t>
+  </si>
+  <si>
+    <t>if GetJournalIndex == 45: Choice "Not only have I found a hidden section, but your grandmother has been laid to rest there.", 5 ELSE Choice "There isn't anythig special with the shrine.", 9, "Not yet.", 5</t>
+  </si>
+  <si>
+    <t>set tlvoat_Estranged_Spirits to 700, Goodbye</t>
+  </si>
+  <si>
+    <t>set tlvoat_Estranged_Spirits to 701, Goodbye</t>
+  </si>
+  <si>
+    <t>set tlvoat_Estranged_Spirits to 600, Goodbye</t>
+  </si>
+  <si>
+    <t>Thank you for helping to find it.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &gt;= 50</t>
+  </si>
+  <si>
+    <t>It was one of the things that I took when I ran away. Something to remember her by. I thought my grandmother would be angry when I spoke to her, but it turns out she always wanted me to have it. Another thing my parents denied to me.</t>
+  </si>
+  <si>
+    <t>RemoveItem "tlvoat_ring_matriarch_unique", 1; Player-&gt;AddItem "tlvoat_ring_matriarch_unique", 1; Journal "tlvoat_Estranged_Spirits", 100</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 100</t>
+  </si>
+  <si>
+    <t>I hope it's helping you on your adventures.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 101</t>
+  </si>
+  <si>
+    <t>I still have it here. I think my grandmother suspected that I lent towards magic, like her, and that's why she wanted me to have it. And why my father didn't, as he wanted me to take after him as a warrior.</t>
+  </si>
+  <si>
+    <t>Choice = 2, PC isFemale = 1</t>
+  </si>
+  <si>
+    <t>Choice = 2, PC isFemale = 0</t>
+  </si>
+  <si>
+    <t>Of course you are humble too. Well, I hope that we can meet again someday.</t>
+  </si>
+  <si>
+    <t>Oh! Of course, you are humble to go with being brave and strong. I would like to be like you one day. I truly hope that we can meet again someday.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 500</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 200</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &lt;= 45, tlvoat_hasPCSaidInTemple == 1</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &lt;= 5, tlvoat_hasPCEnteredTomb = 1, tlvoat_tombClearCount &gt;= 6</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &lt;= 5, tlvoat_hasPCEnteredTomb = 1, tlvoat_tombClearCount &lt; 6</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 10</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 20</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 50; Player-&gt;AddItem Gold_001, 50; set tlvoat_hasPCReceivedReward1</t>
+  </si>
+  <si>
+    <t>Thank you %PCName. Coming here has brought up so many old feelings that I've kept so very deeply buried. It hurts all the more that I don't even hear my grandmother's spirit, as she was the only one I ever had a good relationship with. I used to suspect that there is a hidden section of the tomb, and I am once again hoping there is one and that she was laid to rest there. Though I might just be letting myself be fooled by hope once again.</t>
+  </si>
+  <si>
+    <t>I… Thank you %PCName… That means a lot to me. [She is silent for a minute.] I've always felt like a coward or that I was weak for running away, rather than sticking with it. Everything that I've done has been to get as far away from my family. I think I've been hurting myself. I had hoped to speak to my grandmother, but she too is silent. I once suspected that there is a hidden section in this tomb, and she's in there and that's why I can't hear her.</t>
+  </si>
+  <si>
+    <t>Aryasi wants further help with speaking with her family's spirits. I have turned her down for now.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.journal &gt;= 600</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.journal == 200</t>
+  </si>
+  <si>
+    <t>Still silent. I'll linger a while longer in the hope that I can reach my grandmother's spirit.</t>
+  </si>
+  <si>
+    <t>I think I'm going to have to get used to never connecting with any of my family's spirits. The thought is a lonely one.</t>
+  </si>
+  <si>
+    <t>No luck so far. I understand why you don't want to help any further, you've done so much for me already.</t>
   </si>
 </sst>
 </file>
@@ -1556,16 +1691,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1573,16 +1708,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1590,7 +1725,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1599,7 +1734,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1624,16 +1759,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1641,13 +1776,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1655,7 +1790,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>279</v>
+        <v>235</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1664,7 +1799,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>280</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -1758,7 +1893,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1791,10 +1926,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
-  <dimension ref="A2:F17"/>
+  <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1829,7 +1964,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1840,16 +1975,16 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" t="s">
         <v>128</v>
-      </c>
-      <c r="F4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1860,13 +1995,13 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1877,16 +2012,16 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>257</v>
+        <v>218</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1897,19 +2032,19 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>258</v>
+        <v>219</v>
       </c>
       <c r="D7">
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1917,27 +2052,27 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>259</v>
+        <v>322</v>
       </c>
       <c r="D8">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>281</v>
+        <v>220</v>
       </c>
       <c r="D9">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1948,13 +2083,10 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="D10">
-        <v>50</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1965,13 +2097,16 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
       <c r="D11">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1979,16 +2114,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="D12">
-        <v>70</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1996,16 +2128,16 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>277</v>
+        <v>215</v>
       </c>
       <c r="D13">
-        <v>100</v>
-      </c>
-      <c r="F13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2013,10 +2145,10 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="D14">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F14" t="s">
         <v>35</v>
@@ -2030,19 +2162,16 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="D15">
-        <v>200</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>195</v>
+        <v>101</v>
       </c>
       <c r="F15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2050,19 +2179,19 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
       <c r="D16">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="F16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2070,20 +2199,108 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>201</v>
+        <v>130</v>
       </c>
       <c r="D17">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>36</v>
+        <v>171</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18">
+        <v>400</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D19">
+        <v>500</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D20">
+        <v>600</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D21">
+        <v>700</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D22">
+        <v>701</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F4 F6:F7 F13 F15:F16 B5:E36">
+  <conditionalFormatting sqref="B3:F4 F6:F8 F14 F16:F17 F19:F22 B5:E38">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2312,7 +2529,7 @@
         <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -2320,7 +2537,7 @@
         <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -2344,7 +2561,7 @@
         <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -2357,7 +2574,7 @@
         <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -2365,7 +2582,7 @@
         <v>104</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2375,10 +2592,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F57"/>
+  <dimension ref="A2:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2418,7 +2635,7 @@
         <v>109</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>113</v>
@@ -2438,7 +2655,7 @@
         <v>109</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>113</v>
@@ -2447,7 +2664,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2458,10 +2675,10 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="F5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2475,10 +2692,10 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2492,10 +2709,10 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="F7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2509,13 +2726,13 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="F8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2526,13 +2743,13 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2543,10 +2760,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>144</v>
+        <v>247</v>
       </c>
       <c r="F10" t="s">
-        <v>213</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2560,15 +2777,15 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>145</v>
+        <v>244</v>
       </c>
       <c r="F11" t="s">
-        <v>174</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -2577,16 +2794,13 @@
         <v>110</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="F12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2597,10 +2811,10 @@
         <v>110</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="F13" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2614,13 +2828,13 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>204</v>
+        <v>248</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>205</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2634,13 +2848,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>209</v>
+        <v>165</v>
       </c>
       <c r="F15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2651,13 +2865,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>208</v>
+        <v>250</v>
       </c>
       <c r="F16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2668,16 +2882,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
       <c r="F17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2688,16 +2899,13 @@
         <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>249</v>
+        <v>181</v>
       </c>
       <c r="F18" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2708,16 +2916,13 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>113</v>
+        <v>251</v>
       </c>
       <c r="F19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2730,11 +2935,14 @@
       <c r="D20" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="E20" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="F20" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2742,19 +2950,19 @@
         <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F21" t="s">
         <v>223</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2762,19 +2970,19 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>177</v>
+        <v>113</v>
       </c>
       <c r="F22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -2782,16 +2990,13 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>159</v>
+        <v>256</v>
       </c>
       <c r="F23" t="s">
-        <v>155</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2802,19 +3007,16 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>160</v>
+        <v>257</v>
       </c>
       <c r="F24" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2825,16 +3027,16 @@
         <v>103</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>170</v>
+        <v>260</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="F25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2845,13 +3047,16 @@
         <v>103</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>171</v>
+        <v>189</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="F26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2862,13 +3067,13 @@
         <v>103</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>231</v>
+        <v>152</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>232</v>
+        <v>154</v>
       </c>
       <c r="F27" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2882,10 +3087,13 @@
         <v>103</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>230</v>
+        <v>190</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="F28" t="s">
-        <v>226</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2899,16 +3107,16 @@
         <v>103</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>228</v>
+        <v>158</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>250</v>
+        <v>197</v>
       </c>
       <c r="F29" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2919,16 +3127,13 @@
         <v>103</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>251</v>
+        <v>159</v>
       </c>
       <c r="F30" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2939,16 +3144,16 @@
         <v>103</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>222</v>
+        <v>269</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>234</v>
+        <v>196</v>
       </c>
       <c r="F31" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -2959,16 +3164,13 @@
         <v>103</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="F32" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2979,16 +3181,16 @@
         <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>165</v>
+        <v>212</v>
       </c>
       <c r="F33" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2999,16 +3201,16 @@
         <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="F34" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -3019,16 +3221,16 @@
         <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>122</v>
+        <v>259</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="F35" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -3039,13 +3241,13 @@
         <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="F36" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3059,13 +3261,16 @@
         <v>103</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>178</v>
+        <v>267</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="F37" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -3076,10 +3281,16 @@
         <v>103</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F38" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3087,175 +3298,181 @@
         <v>29</v>
       </c>
       <c r="C39" t="s">
-        <v>179</v>
+        <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>182</v>
+        <v>261</v>
       </c>
       <c r="F39" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F40" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F41" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F42" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F43" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F46" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E48" t="s">
+        <v>276</v>
+      </c>
+      <c r="F48" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" t="s">
-        <v>179</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F40" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" t="s">
-        <v>179</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F41" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" t="s">
-        <v>179</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F42" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" t="s">
-        <v>179</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F43" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" t="s">
-        <v>179</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F44" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" t="s">
-        <v>179</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="F45" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" t="s">
-        <v>179</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" t="s">
-        <v>108</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F48" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -3263,16 +3480,16 @@
         <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>197</v>
+        <v>274</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="F49" t="s">
-        <v>155</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3283,157 +3500,510 @@
         <v>29</v>
       </c>
       <c r="C50" t="s">
+        <v>164</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" t="s">
+        <v>164</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F51" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F52" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F53" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F54" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" t="s">
         <v>108</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="D55" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F55" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F56" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F57" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F59" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F60" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" t="s">
+        <v>108</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F61" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" t="s">
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F51" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" t="s">
-        <v>29</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D62" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F62" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F52" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>29</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D63" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F63" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" t="s">
         <v>108</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F53" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54" t="s">
-        <v>265</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="F54" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" t="s">
-        <v>265</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F55" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56" t="s">
-        <v>265</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F56" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" t="s">
-        <v>265</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F57" t="s">
-        <v>267</v>
+      <c r="D64" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F64" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F65" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" t="s">
+        <v>108</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F66" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" t="s">
+        <v>108</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F67" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" t="s">
+        <v>108</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F68" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" t="s">
+        <v>108</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F69" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" t="s">
+        <v>224</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F70" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" t="s">
+        <v>29</v>
+      </c>
+      <c r="C71" t="s">
+        <v>224</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F71" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72" t="s">
+        <v>224</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F72" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73" t="s">
+        <v>224</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F73" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" t="s">
+        <v>224</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F74" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" t="s">
+        <v>224</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F75" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C76" t="s">
+        <v>224</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F76" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F84">
+  <conditionalFormatting sqref="B3:F101">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -3659,7 +4229,7 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3673,7 +4243,7 @@
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3687,7 +4257,7 @@
         <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3737,13 +4307,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>268</v>
+        <v>226</v>
       </c>
       <c r="C9" t="s">
-        <v>269</v>
+        <v>227</v>
       </c>
       <c r="D9" t="s">
-        <v>270</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3806,7 +4376,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Update: several more Greetings and topic lines to cover various scenarios and quest endings
* Update: reducing number of sound emitters
* Update: additional door to entrance to avoid combat starting immediately upon entering
* Fix: Skeleton Archer sounds
* Fix: Aryasi "killed by guardians" update triggering during transfer
* Fix: Aryasi not rewarding PC after clearing tomb
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84300DBF-DADF-46ED-8FEC-DC58B70C00AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C1DA94-A533-4F76-8874-F6A264CD82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="340">
   <si>
     <t>Name</t>
   </si>
@@ -417,9 +417,6 @@
     <t>(Yes, no), (already found, no), (Yes, (Lie) none), (There is none, not yet)</t>
   </si>
   <si>
-    <t>Thank you again for making it safe for me</t>
-  </si>
-  <si>
     <t>Met Othral/attempted to enter tomb, accepted/accepted after initial decline</t>
   </si>
   <si>
@@ -657,9 +654,6 @@
     <t>Any luck with the shrine?</t>
   </si>
   <si>
-    <t>What? That's incredible! Please lead me to her.</t>
-  </si>
-  <si>
     <t>Ah, ok. I'll continue waiting here.</t>
   </si>
   <si>
@@ -936,9 +930,6 @@
     <t>I told Aryasi that I could not find any hidden section in Othral Ancestral Tomb.</t>
   </si>
   <si>
-    <t>if GetJournalIndex == 45: Choice "Not only have I found a hidden section, but your grandmother has been laid to rest there.", 5 ELSE Choice "There isn't anythig special with the shrine.", 9, "Not yet.", 5</t>
-  </si>
-  <si>
     <t>set tlvoat_Estranged_Spirits to 700, Goodbye</t>
   </si>
   <si>
@@ -1030,6 +1021,51 @@
   </si>
   <si>
     <t>No luck so far. I understand why you don't want to help any further, you've done so much for me already.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 35</t>
+  </si>
+  <si>
+    <t>Are you here to help me find a hidden section in this tomb?</t>
+  </si>
+  <si>
+    <t>Thank you again for making it safe for me.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &gt;= 600</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 600</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &gt;= 700</t>
+  </si>
+  <si>
+    <t>I was so sure that shrine had been keeping a secret this whole time.</t>
+  </si>
+  <si>
+    <t>If grandmother wasn't in that section, then that means she's here and she's as silent as the rest of my family.</t>
+  </si>
+  <si>
+    <t>Hello %PCName, I've just been trying to work out where I go from here.</t>
+  </si>
+  <si>
+    <t>if GetJournalIndex == 45: Choice "Not only have I found a hidden section, but your grandmother has been laid to rest there.", 5, "(Lie) There is a hidden section, but your grandmother is not there.", 8, "(Lie) There isn't anything special with the shrine.", 9, "Not yet.", 6 ELSEIF ButtonPressed == 1: Choice "You were correct, the shrine had a switch.", 4, "(Lie) There is a hidden section, but your grandmother is not there.", 7, "(Lie) There isn't anything special with the shrine.", 9, "Not yet.", 6 ELSE Choice "There isn't anything special with the shrine.", 9, "Not yet.", 6</t>
+  </si>
+  <si>
+    <t>You have? That's… please lead me to her.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &lt;= 45, tlvoat_PCMentionSecret == 1</t>
+  </si>
+  <si>
+    <t>I'm happy that I was right about the shrine, but what's in the hidden section %PCName?</t>
+  </si>
+  <si>
+    <t>Hold on %PCName, let me enter my family's tomb first.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 30, PCGetCell "OAT" == 0</t>
   </si>
 </sst>
 </file>
@@ -1691,16 +1727,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1708,16 +1744,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1725,7 +1761,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1734,7 +1770,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1759,16 +1795,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1776,13 +1812,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1790,7 +1826,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1799,7 +1835,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -1893,7 +1929,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1928,7 +1964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
   <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1964,7 +2000,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1975,16 +2011,16 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1995,13 +2031,13 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2012,16 +2048,16 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2032,16 +2068,16 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D7">
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2052,7 +2088,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2066,7 +2102,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2083,7 +2119,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -2097,7 +2133,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2114,7 +2150,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2128,13 +2164,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2145,7 +2181,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -2162,7 +2198,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D15">
         <v>101</v>
@@ -2179,13 +2215,13 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F16" t="s">
         <v>35</v>
@@ -2199,13 +2235,13 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D17">
         <v>300</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
@@ -2219,7 +2255,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D18">
         <v>400</v>
@@ -2239,7 +2275,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D19">
         <v>500</v>
@@ -2256,7 +2292,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D20">
         <v>600</v>
@@ -2273,7 +2309,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D21">
         <v>700</v>
@@ -2290,7 +2326,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D22">
         <v>701</v>
@@ -2300,7 +2336,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F4 F6:F8 F14 F16:F17 F19:F22 B5:E38">
+  <conditionalFormatting sqref="B3:F4 B5:E38 F6:F8 F14 F16:F17 F19:F22">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2592,10 +2628,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F76"/>
+  <dimension ref="A2:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2635,7 +2671,7 @@
         <v>109</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>113</v>
@@ -2655,7 +2691,7 @@
         <v>109</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>113</v>
@@ -2675,10 +2711,10 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2692,10 +2728,10 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2709,10 +2745,10 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2726,10 +2762,10 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2743,10 +2779,10 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2760,10 +2796,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2777,10 +2813,10 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2794,10 +2830,10 @@
         <v>110</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2811,10 +2847,10 @@
         <v>110</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2828,16 +2864,16 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2848,10 +2884,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>165</v>
+        <v>338</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>162</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2865,13 +2904,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>250</v>
+        <v>164</v>
       </c>
       <c r="F16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2882,13 +2921,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>180</v>
+        <v>326</v>
       </c>
       <c r="F17" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2899,10 +2938,10 @@
         <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
       <c r="F18" t="s">
-        <v>314</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2916,13 +2955,13 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>251</v>
+        <v>179</v>
       </c>
       <c r="F19" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2933,16 +2972,13 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>113</v>
+        <v>337</v>
       </c>
       <c r="F20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2953,16 +2989,13 @@
         <v>110</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="F21" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2973,16 +3006,13 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>113</v>
+        <v>249</v>
       </c>
       <c r="F22" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -2993,13 +3023,16 @@
         <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="F23" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -3010,13 +3043,16 @@
         <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="F24" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -3024,19 +3060,19 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="F25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -3044,19 +3080,16 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>163</v>
+        <v>254</v>
       </c>
       <c r="F26" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -3064,16 +3097,13 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>154</v>
+        <v>333</v>
       </c>
       <c r="F27" t="s">
-        <v>150</v>
+        <v>328</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3084,19 +3114,16 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>154</v>
+        <v>255</v>
       </c>
       <c r="F28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3107,16 +3134,16 @@
         <v>103</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>158</v>
+        <v>258</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="F29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3127,13 +3154,16 @@
         <v>103</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>159</v>
+        <v>188</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="F30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -3144,13 +3174,13 @@
         <v>103</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>269</v>
+        <v>151</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>196</v>
+        <v>153</v>
       </c>
       <c r="F31" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3164,10 +3194,13 @@
         <v>103</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="F32" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3181,16 +3214,16 @@
         <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="F33" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -3201,16 +3234,13 @@
         <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="F34" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -3221,16 +3251,16 @@
         <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F35" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -3241,16 +3271,13 @@
         <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F36" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3261,13 +3288,13 @@
         <v>103</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>267</v>
+        <v>192</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>264</v>
+        <v>210</v>
       </c>
       <c r="F37" t="s">
-        <v>315</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3281,16 +3308,16 @@
         <v>103</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>268</v>
+        <v>192</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>265</v>
+        <v>211</v>
       </c>
       <c r="F38" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3301,13 +3328,16 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="F39" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -3318,13 +3348,13 @@
         <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>263</v>
+        <v>119</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>265</v>
+        <v>197</v>
       </c>
       <c r="F40" t="s">
-        <v>317</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3338,13 +3368,13 @@
         <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F41" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3358,13 +3388,13 @@
         <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>319</v>
+        <v>263</v>
       </c>
       <c r="F42" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3378,13 +3408,13 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="F43" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -3395,10 +3425,16 @@
         <v>103</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F44" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -3406,158 +3442,161 @@
         <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>164</v>
+        <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F45" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F46" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F47" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F49" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F50" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F51" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" t="s">
+        <v>163</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E52" t="s">
+        <v>274</v>
+      </c>
+      <c r="F52" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F45" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" t="s">
-        <v>164</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F46" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" t="s">
-        <v>164</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="F47" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" t="s">
-        <v>164</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E48" t="s">
-        <v>276</v>
-      </c>
-      <c r="F48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" t="s">
-        <v>164</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F49" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C50" t="s">
-        <v>164</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F50" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" t="s">
-        <v>164</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F51" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" t="s">
-        <v>29</v>
-      </c>
-      <c r="C52" t="s">
-        <v>164</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="F52" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>29</v>
-      </c>
-      <c r="C53" t="s">
-        <v>164</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="F53" t="s">
-        <v>323</v>
+        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3568,16 +3607,16 @@
         <v>29</v>
       </c>
       <c r="C54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F54" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -3585,16 +3624,13 @@
         <v>29</v>
       </c>
       <c r="C55" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="F55" t="s">
-        <v>146</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3605,19 +3641,16 @@
         <v>29</v>
       </c>
       <c r="C56" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>284</v>
+        <v>322</v>
       </c>
       <c r="F56" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -3625,19 +3658,16 @@
         <v>29</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>179</v>
+        <v>323</v>
       </c>
       <c r="F57" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3645,19 +3675,16 @@
         <v>29</v>
       </c>
       <c r="C58" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F58" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3668,16 +3695,16 @@
         <v>108</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>203</v>
+        <v>288</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
       <c r="F59" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3688,13 +3715,16 @@
         <v>108</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>204</v>
+        <v>169</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>282</v>
       </c>
       <c r="F60" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3705,16 +3735,16 @@
         <v>108</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>294</v>
+        <v>173</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>297</v>
+        <v>178</v>
       </c>
       <c r="F61" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3725,13 +3755,13 @@
         <v>108</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="F62" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3745,16 +3775,16 @@
         <v>108</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>294</v>
+        <v>335</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>299</v>
+        <v>203</v>
       </c>
       <c r="F63" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -3765,16 +3795,13 @@
         <v>108</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>281</v>
+        <v>202</v>
       </c>
       <c r="F64" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -3785,16 +3812,16 @@
         <v>108</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="F65" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3805,16 +3832,16 @@
         <v>108</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="F66" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -3825,16 +3852,16 @@
         <v>108</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>202</v>
+        <v>292</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>296</v>
       </c>
       <c r="F67" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -3845,13 +3872,16 @@
         <v>108</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>327</v>
+        <v>278</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>279</v>
       </c>
       <c r="F68" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3862,13 +3892,16 @@
         <v>108</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>300</v>
+        <v>285</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>284</v>
       </c>
       <c r="F69" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -3876,19 +3909,19 @@
         <v>29</v>
       </c>
       <c r="C70" t="s">
-        <v>224</v>
+        <v>108</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>230</v>
+        <v>286</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="F70" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -3896,16 +3929,16 @@
         <v>29</v>
       </c>
       <c r="C71" t="s">
-        <v>224</v>
+        <v>108</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>234</v>
+        <v>334</v>
       </c>
       <c r="F71" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3916,16 +3949,13 @@
         <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>224</v>
+        <v>108</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>234</v>
+        <v>324</v>
       </c>
       <c r="F72" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -3936,19 +3966,16 @@
         <v>29</v>
       </c>
       <c r="C73" t="s">
-        <v>224</v>
+        <v>108</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>234</v>
+        <v>331</v>
       </c>
       <c r="F73" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -3956,16 +3983,13 @@
         <v>29</v>
       </c>
       <c r="C74" t="s">
-        <v>224</v>
+        <v>108</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>229</v>
+        <v>332</v>
       </c>
       <c r="F74" t="s">
-        <v>225</v>
+        <v>330</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -3976,34 +4000,151 @@
         <v>29</v>
       </c>
       <c r="C75" t="s">
-        <v>224</v>
+        <v>108</v>
       </c>
       <c r="D75" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F75" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C76" t="s">
+        <v>222</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F76" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" t="s">
+        <v>29</v>
+      </c>
+      <c r="C77" t="s">
+        <v>222</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F77" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" t="s">
+        <v>222</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F78" t="s">
         <v>305</v>
       </c>
-      <c r="F75" t="s">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79" t="s">
+        <v>222</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F79" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80" t="s">
+        <v>222</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F80" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81" t="s">
+        <v>29</v>
+      </c>
+      <c r="C81" t="s">
+        <v>222</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F81" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82" t="s">
+        <v>29</v>
+      </c>
+      <c r="C82" t="s">
+        <v>222</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>14</v>
-      </c>
-      <c r="B76" t="s">
-        <v>29</v>
-      </c>
-      <c r="C76" t="s">
-        <v>224</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F76" t="s">
-        <v>306</v>
+      <c r="F82" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F101">
+  <conditionalFormatting sqref="B3:F107">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -4229,7 +4370,7 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4243,7 +4384,7 @@
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4257,7 +4398,7 @@
         <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -4307,13 +4448,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" t="s">
         <v>226</v>
-      </c>
-      <c r="C9" t="s">
-        <v>227</v>
-      </c>
-      <c r="D9" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -4376,7 +4517,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Update: PC can demand higher gold reward
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C1DA94-A533-4F76-8874-F6A264CD82B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E642070-4B1F-431D-A163-D5724F4B848C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="352">
   <si>
     <t>Name</t>
   </si>
@@ -405,9 +405,6 @@
     <t>escorting, completed escort</t>
   </si>
   <si>
-    <t>Have you changed your mind?</t>
-  </si>
-  <si>
     <t>brief overview of family history, joyous she can reconnect</t>
   </si>
   <si>
@@ -489,9 +486,6 @@
     <t>tlvoat_estranged_spirits.Journal &lt;= 0</t>
   </si>
   <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 10</t>
-  </si>
-  <si>
     <t>Choice = 2</t>
   </si>
   <si>
@@ -534,9 +528,6 @@
     <t>tlvoat_estranged_spirits.Journal == 30</t>
   </si>
   <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 10, set tlvoat_hasPCSaidInTemple to 1</t>
-  </si>
-  <si>
     <t>spirits of my family</t>
   </si>
   <si>
@@ -639,9 +630,6 @@
     <t>Choice "[Let her enter]", 9, "[Stop her] Wait, I think I may have missed a section.", 8</t>
   </si>
   <si>
-    <t>if PCRank Temple &gt;= 0: Choice "Yes, I can clear your family's tomb.", 1, "As a priest of the Temple I'd be happy to.", 2, "I'm too busy right now.", 3, "No I will not.", 4 ELSE Choice "Yes, I can clear your family's tomb.", 1, "I'm too busy right now.", 3, "No I will not.", 4</t>
-  </si>
-  <si>
     <t>tlvoat_PCMentionInTemple = 1</t>
   </si>
   <si>
@@ -1066,6 +1054,54 @@
   </si>
   <si>
     <t>tlvoat_estranged_spirits.Journal == 30, PCGetCell "OAT" == 0</t>
+  </si>
+  <si>
+    <t>Choice = 11</t>
+  </si>
+  <si>
+    <t>Choice = 12</t>
+  </si>
+  <si>
+    <t>Choice = 11, PCLevel &lt;= 2</t>
+  </si>
+  <si>
+    <t>Have you changed your mind? 50 gold is yours if you do it.</t>
+  </si>
+  <si>
+    <t>if PCRank Temple &gt;= 0: Choice "Yes, I can clear your family's tomb.", 1, "As a priest of the Temple I'd be happy to.", 2, "Up the gold and I'll do it.", 11, "I'm too busy right now.", 3, "No I will not.", 4 ELSE Choice "Yes, I can clear your family's tomb.", 1, "Up the gold and I'll do it.", 11, "I'm too busy right now.", 3, "No I will not.", 4</t>
+  </si>
+  <si>
+    <t>No I'm only offering the 50 gold as that's all I can spare. Are you going to do it or not?</t>
+  </si>
+  <si>
+    <t>Fine, I'll make it 70 gold. Any higher and I'll really struggle to feed myself. If you want more then you can take the offerings left by grievers, as well as the family heirlooms. All I ask is to just leave their remains alone.</t>
+  </si>
+  <si>
+    <t>ModDisposition -10, Choice "Fine, I'll do it.", 12, "No I won't.", 4</t>
+  </si>
+  <si>
+    <t>Good. I do appreciate this %PCClass, as I'm very much aware that I'm putting you in a lot of danger. There's offerings and the family heirlooms that you can take, as well as anything the guardians have. Just please leave my family's remains alone.</t>
+  </si>
+  <si>
+    <t>Oh right I had forgotten. It was 70 right? Well here, you've earned it.</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits &gt;= 30, tlvoat_hasPCReceivedReward1 = 0, tlvoat_hasHighReward1 = 1</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 10,set "tlvoat_ex_othral_door_unique".controlState to 1</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 10, set tlvoat_hasPCSaidInTemple to 1, set "tlvoat_ex_othral_door_unique".controlState to 1</t>
+  </si>
+  <si>
+    <t>ModDisposition -10, set tlvoat_hasHighReward1 to 1, Journal "tlvoat_Estranged_Spirits", 10, set "tlvoat_ex_othral_door_unique".controlState to 1</t>
+  </si>
+  <si>
+    <t>ModDisposition 2,  Journal "tlvoat_Estranged_Spirits", 10, set "tlvoat_ex_othral_door_unique".controlState to 1</t>
   </si>
 </sst>
 </file>
@@ -1727,16 +1763,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1744,16 +1780,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1761,7 +1797,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1770,7 +1806,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1795,16 +1831,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1812,13 +1848,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1826,7 +1862,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1835,7 +1871,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1929,7 +1965,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1964,8 +2000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
   <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2000,7 +2036,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2011,16 +2047,16 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2031,13 +2067,13 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2048,16 +2084,16 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D6">
         <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2068,16 +2104,16 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D7">
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2088,7 +2124,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2102,7 +2138,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2119,7 +2155,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -2133,7 +2169,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2150,7 +2186,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2164,13 +2200,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2181,7 +2217,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -2198,7 +2234,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D15">
         <v>101</v>
@@ -2215,13 +2251,13 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F16" t="s">
         <v>35</v>
@@ -2235,13 +2271,13 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D17">
         <v>300</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
@@ -2255,7 +2291,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D18">
         <v>400</v>
@@ -2275,7 +2311,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D19">
         <v>500</v>
@@ -2292,7 +2328,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D20">
         <v>600</v>
@@ -2309,7 +2345,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D21">
         <v>700</v>
@@ -2326,7 +2362,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D22">
         <v>701</v>
@@ -2597,7 +2633,7 @@
         <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -2610,7 +2646,7 @@
         <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -2618,7 +2654,7 @@
         <v>104</v>
       </c>
       <c r="D28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2628,10 +2664,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F82"/>
+  <dimension ref="A2:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2671,7 +2707,7 @@
         <v>109</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>113</v>
@@ -2691,7 +2727,7 @@
         <v>109</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>113</v>
@@ -2711,10 +2747,10 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2728,10 +2764,10 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2745,10 +2781,10 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2762,10 +2798,10 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2779,10 +2815,10 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2796,10 +2832,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F10" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2813,10 +2849,10 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2830,10 +2866,10 @@
         <v>110</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2847,10 +2883,10 @@
         <v>110</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2864,13 +2900,13 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2884,13 +2920,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2904,10 +2940,10 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2921,10 +2957,10 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F17" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2938,10 +2974,10 @@
         <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F18" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2955,10 +2991,10 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F19" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2972,10 +3008,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F20" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2989,10 +3025,10 @@
         <v>110</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F21" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3006,10 +3042,10 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F22" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3023,13 +3059,13 @@
         <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3043,13 +3079,13 @@
         <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F24" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3063,13 +3099,13 @@
         <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3083,10 +3119,10 @@
         <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F26" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3100,10 +3136,10 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F27" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3117,10 +3153,10 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F28" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3134,16 +3170,16 @@
         <v>103</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>147</v>
+        <v>348</v>
       </c>
       <c r="F29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3154,13 +3190,13 @@
         <v>103</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>162</v>
+        <v>349</v>
       </c>
       <c r="F30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3174,13 +3210,13 @@
         <v>103</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="F31" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3194,13 +3230,13 @@
         <v>103</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3214,13 +3250,13 @@
         <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3234,10 +3270,10 @@
         <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3251,13 +3287,13 @@
         <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -3271,10 +3307,10 @@
         <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F36" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3288,13 +3324,13 @@
         <v>103</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F37" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3308,16 +3344,16 @@
         <v>103</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F38" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3328,16 +3364,16 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>257</v>
+        <v>341</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>197</v>
+        <v>343</v>
       </c>
       <c r="F39" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -3348,16 +3384,16 @@
         <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>119</v>
+        <v>342</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>197</v>
+        <v>350</v>
       </c>
       <c r="F40" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3368,16 +3404,16 @@
         <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>265</v>
+        <v>344</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>262</v>
+        <v>351</v>
       </c>
       <c r="F41" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -3388,16 +3424,16 @@
         <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>263</v>
+        <v>340</v>
       </c>
       <c r="F42" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -3408,13 +3444,16 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>259</v>
+        <v>339</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>340</v>
       </c>
       <c r="F43" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -3428,13 +3467,13 @@
         <v>261</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="F44" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -3445,16 +3484,16 @@
         <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F45" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -3465,16 +3504,13 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>316</v>
+        <v>255</v>
       </c>
       <c r="F46" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3485,13 +3521,16 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>268</v>
+        <v>257</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="F47" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -3502,10 +3541,16 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F48" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -3513,144 +3558,144 @@
         <v>29</v>
       </c>
       <c r="C49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F49" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F50" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F51" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" t="s">
+        <v>160</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F49" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C50" t="s">
-        <v>163</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="F53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" t="s">
+        <v>160</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F54" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" t="s">
+        <v>160</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F55" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" t="s">
+        <v>160</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E56" t="s">
+        <v>270</v>
+      </c>
+      <c r="F56" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" t="s">
-        <v>163</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F51" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" t="s">
-        <v>29</v>
-      </c>
-      <c r="C52" t="s">
-        <v>163</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="E52" t="s">
-        <v>274</v>
-      </c>
-      <c r="F52" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>29</v>
-      </c>
-      <c r="C53" t="s">
-        <v>163</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F53" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54" t="s">
-        <v>163</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="F54" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" t="s">
-        <v>163</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F55" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56" t="s">
-        <v>163</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="F56" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -3658,13 +3703,16 @@
         <v>29</v>
       </c>
       <c r="C57" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>323</v>
+        <v>268</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="F57" t="s">
-        <v>320</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3675,16 +3723,16 @@
         <v>29</v>
       </c>
       <c r="C58" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F58" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3692,16 +3740,13 @@
         <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="F59" t="s">
-        <v>145</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3712,19 +3757,16 @@
         <v>29</v>
       </c>
       <c r="C60" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>282</v>
+        <v>318</v>
       </c>
       <c r="F60" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3732,19 +3774,16 @@
         <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>178</v>
+        <v>319</v>
       </c>
       <c r="F61" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3752,19 +3791,16 @@
         <v>29</v>
       </c>
       <c r="C62" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F62" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3775,16 +3811,16 @@
         <v>108</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>335</v>
+        <v>284</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="F63" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -3795,13 +3831,16 @@
         <v>108</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>202</v>
+        <v>166</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="F64" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -3812,16 +3851,16 @@
         <v>108</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>292</v>
+        <v>170</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>294</v>
+        <v>175</v>
       </c>
       <c r="F65" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3832,13 +3871,13 @@
         <v>108</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="F66" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3852,16 +3891,16 @@
         <v>108</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>292</v>
+        <v>331</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>296</v>
+        <v>199</v>
       </c>
       <c r="F67" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -3872,16 +3911,13 @@
         <v>108</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>279</v>
+        <v>198</v>
       </c>
       <c r="F68" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3892,16 +3928,16 @@
         <v>108</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="F69" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -3912,16 +3948,16 @@
         <v>108</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>291</v>
       </c>
       <c r="F70" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -3932,16 +3968,16 @@
         <v>108</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>201</v>
+        <v>288</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="F71" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -3952,13 +3988,16 @@
         <v>108</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>324</v>
+        <v>274</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="F72" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -3969,13 +4008,16 @@
         <v>108</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>331</v>
+        <v>281</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="F73" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -3986,13 +4028,16 @@
         <v>108</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>332</v>
+        <v>282</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>287</v>
       </c>
       <c r="F74" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4003,13 +4048,16 @@
         <v>108</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>297</v>
+        <v>197</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="F75" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4017,19 +4065,16 @@
         <v>29</v>
       </c>
       <c r="C76" t="s">
-        <v>222</v>
+        <v>108</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="F76" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4037,16 +4082,13 @@
         <v>29</v>
       </c>
       <c r="C77" t="s">
-        <v>222</v>
+        <v>108</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>232</v>
+        <v>327</v>
       </c>
       <c r="F77" t="s">
-        <v>229</v>
+        <v>325</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4057,16 +4099,13 @@
         <v>29</v>
       </c>
       <c r="C78" t="s">
-        <v>222</v>
+        <v>108</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>232</v>
+        <v>328</v>
       </c>
       <c r="F78" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -4077,19 +4116,16 @@
         <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>222</v>
+        <v>108</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>232</v>
+        <v>293</v>
       </c>
       <c r="F79" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4097,19 +4133,19 @@
         <v>29</v>
       </c>
       <c r="C80" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>299</v>
+        <v>224</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>227</v>
+        <v>296</v>
       </c>
       <c r="F80" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4117,16 +4153,19 @@
         <v>29</v>
       </c>
       <c r="C81" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>302</v>
+        <v>226</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="F81" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4134,17 +4173,94 @@
         <v>29</v>
       </c>
       <c r="C82" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>304</v>
       </c>
+      <c r="E82" s="2" t="s">
+        <v>228</v>
+      </c>
       <c r="F82" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" t="s">
+        <v>218</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>303</v>
       </c>
+      <c r="E83" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F83" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" t="s">
+        <v>218</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F84" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85" t="s">
+        <v>29</v>
+      </c>
+      <c r="C85" t="s">
+        <v>218</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F85" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86" t="s">
+        <v>29</v>
+      </c>
+      <c r="C86" t="s">
+        <v>218</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F86" t="s">
+        <v>299</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F107">
+  <conditionalFormatting sqref="B3:F111">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -4370,7 +4486,7 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4384,7 +4500,7 @@
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4398,7 +4514,7 @@
         <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -4448,13 +4564,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -4517,7 +4633,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Update: account for PC picking up all heirlooms
Add: additional line to reflect PC demanding more gold yet declining final reward
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E642070-4B1F-431D-A163-D5724F4B848C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C753F5-B6C7-40EC-BD0B-7B1DC2CEC297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="358">
   <si>
     <t>Name</t>
   </si>
@@ -942,9 +942,6 @@
     <t>tlvoat_Estranged_Spirits.Journal == 100</t>
   </si>
   <si>
-    <t>I hope it's helping you on your adventures.</t>
-  </si>
-  <si>
     <t>tlvoat_Estranged_Spirits.Journal == 101</t>
   </si>
   <si>
@@ -1102,6 +1099,27 @@
   </si>
   <si>
     <t>ModDisposition 2,  Journal "tlvoat_Estranged_Spirits", 10, set "tlvoat_ex_othral_door_unique".controlState to 1</t>
+  </si>
+  <si>
+    <t>Right, your gold. Here's the 70 I promised you. I hope that and the heirlooms satisfy you.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits &gt;= 30, tlvoat_hasPCReceivedReward1 = 0, tlvoat_hasHighReward1 = 1, PC has sword &amp; bracers</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits &gt;= 30, tlvoat_hasPCReceivedReward1 = 0, PC has sword &amp; bracers</t>
+  </si>
+  <si>
+    <t>By the way, here's your gold. I hope that and the heirlooms are enough to satisfy you.</t>
+  </si>
+  <si>
+    <t>Choice = 2, tlvoat_hasHighReward1 = 1</t>
+  </si>
+  <si>
+    <t>I hope that it's of some use to you on your adventures.</t>
+  </si>
+  <si>
+    <t>After demanding for more gold earlier I thought you'd accept the ring. You confuse me %PCName. Well, regardless, I hope that we meet again someday.</t>
   </si>
 </sst>
 </file>
@@ -2124,7 +2142,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2664,10 +2682,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F86"/>
+  <dimension ref="A2:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B89" sqref="B3:B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2906,7 +2924,7 @@
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2920,13 +2938,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2957,10 +2975,10 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2994,7 +3012,7 @@
         <v>176</v>
       </c>
       <c r="F19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3008,10 +3026,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3028,7 +3046,7 @@
         <v>177</v>
       </c>
       <c r="F21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3136,10 +3154,10 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -3173,7 +3191,7 @@
         <v>254</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F29" t="s">
         <v>144</v>
@@ -3193,7 +3211,7 @@
         <v>185</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F30" t="s">
         <v>146</v>
@@ -3364,13 +3382,13 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F39" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3384,13 +3402,13 @@
         <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3404,13 +3422,13 @@
         <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F41" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3427,7 +3445,7 @@
         <v>253</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F42" t="s">
         <v>145</v>
@@ -3444,10 +3462,10 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>340</v>
       </c>
       <c r="F43" t="s">
         <v>150</v>
@@ -3470,7 +3488,7 @@
         <v>258</v>
       </c>
       <c r="F44" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3490,7 +3508,7 @@
         <v>259</v>
       </c>
       <c r="F45" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3527,7 +3545,7 @@
         <v>259</v>
       </c>
       <c r="F47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3547,7 +3565,7 @@
         <v>258</v>
       </c>
       <c r="F48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3561,13 +3579,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>346</v>
-      </c>
       <c r="F49" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3581,16 +3599,16 @@
         <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>266</v>
+        <v>344</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>312</v>
+        <v>345</v>
       </c>
       <c r="F50" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -3601,13 +3619,16 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>264</v>
+        <v>354</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="F51" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -3618,10 +3639,16 @@
         <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -3629,19 +3656,16 @@
         <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>163</v>
+        <v>264</v>
       </c>
       <c r="F53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -3649,16 +3673,13 @@
         <v>29</v>
       </c>
       <c r="C54" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="F54" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -3669,10 +3690,13 @@
         <v>160</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>269</v>
+        <v>162</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="F55" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -3686,16 +3710,13 @@
         <v>160</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E56" t="s">
-        <v>270</v>
+        <v>312</v>
       </c>
       <c r="F56" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -3706,16 +3727,13 @@
         <v>160</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>164</v>
+        <v>269</v>
       </c>
       <c r="F57" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3726,13 +3744,16 @@
         <v>160</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>271</v>
+        <v>313</v>
+      </c>
+      <c r="E58" t="s">
+        <v>270</v>
       </c>
       <c r="F58" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3743,10 +3764,13 @@
         <v>160</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>196</v>
+        <v>268</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="F59" t="s">
-        <v>195</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3760,10 +3784,10 @@
         <v>160</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>318</v>
+        <v>271</v>
       </c>
       <c r="F60" t="s">
-        <v>317</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3777,10 +3801,10 @@
         <v>160</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>319</v>
+        <v>196</v>
       </c>
       <c r="F61" t="s">
-        <v>316</v>
+        <v>195</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3794,13 +3818,13 @@
         <v>160</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>273</v>
+        <v>317</v>
       </c>
       <c r="F62" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3808,16 +3832,13 @@
         <v>29</v>
       </c>
       <c r="C63" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>171</v>
+        <v>318</v>
       </c>
       <c r="F63" t="s">
-        <v>144</v>
+        <v>315</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3828,19 +3849,16 @@
         <v>29</v>
       </c>
       <c r="C64" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F64" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -3851,16 +3869,16 @@
         <v>108</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>170</v>
+        <v>284</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F65" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3871,16 +3889,16 @@
         <v>108</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>283</v>
+        <v>166</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F66" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -3891,16 +3909,16 @@
         <v>108</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>331</v>
+        <v>170</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="F67" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -3911,10 +3929,13 @@
         <v>108</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>198</v>
+        <v>283</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="F68" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3928,16 +3949,16 @@
         <v>108</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>288</v>
+        <v>330</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>290</v>
+        <v>199</v>
       </c>
       <c r="F69" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -3948,13 +3969,10 @@
         <v>108</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>291</v>
+        <v>198</v>
       </c>
       <c r="F70" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3971,13 +3989,13 @@
         <v>288</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F71" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -3988,16 +4006,16 @@
         <v>108</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="F72" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -4008,16 +4026,16 @@
         <v>108</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="F73" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4028,16 +4046,16 @@
         <v>108</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="F74" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4048,16 +4066,16 @@
         <v>108</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>197</v>
+        <v>281</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="F75" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4068,13 +4086,16 @@
         <v>108</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>320</v>
+        <v>282</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>287</v>
       </c>
       <c r="F76" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4085,10 +4106,13 @@
         <v>108</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>327</v>
+        <v>197</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="F77" t="s">
-        <v>325</v>
+        <v>247</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4102,10 +4126,10 @@
         <v>108</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="F78" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -4119,53 +4143,47 @@
         <v>108</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F79" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80" t="s">
+        <v>108</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F80" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81" t="s">
+        <v>29</v>
+      </c>
+      <c r="C81" t="s">
+        <v>108</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F81" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>14</v>
-      </c>
-      <c r="B80" t="s">
-        <v>29</v>
-      </c>
-      <c r="C80" t="s">
-        <v>218</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F80" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>14</v>
-      </c>
-      <c r="B81" t="s">
-        <v>29</v>
-      </c>
-      <c r="C81" t="s">
-        <v>218</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F81" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4176,16 +4194,16 @@
         <v>218</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>304</v>
+        <v>224</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>228</v>
+        <v>296</v>
       </c>
       <c r="F82" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4196,16 +4214,16 @@
         <v>218</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>303</v>
+        <v>226</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>228</v>
       </c>
       <c r="F83" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4216,16 +4234,16 @@
         <v>218</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>295</v>
+        <v>357</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="F84" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4236,13 +4254,16 @@
         <v>218</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>298</v>
+        <v>303</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="F85" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -4253,14 +4274,71 @@
         <v>218</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="F86" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>14</v>
+      </c>
+      <c r="B87" t="s">
+        <v>29</v>
+      </c>
+      <c r="C87" t="s">
+        <v>218</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F87" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" t="s">
+        <v>29</v>
+      </c>
+      <c r="C88" t="s">
+        <v>218</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F88" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>14</v>
+      </c>
+      <c r="B89" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" t="s">
+        <v>218</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>299</v>
       </c>
+      <c r="F89" t="s">
+        <v>298</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F111">
+  <conditionalFormatting sqref="B3:F114">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add: Aryasi reacting to the PC disturbing family remains, ending the quest
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C753F5-B6C7-40EC-BD0B-7B1DC2CEC297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF75AF7A-C226-4A5A-9B16-ED8364030CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="368">
   <si>
     <t>Name</t>
   </si>
@@ -1120,6 +1120,36 @@
   </si>
   <si>
     <t>After demanding for more gold earlier I thought you'd accept the ring. You confuse me %PCName. Well, regardless, I hope that we meet again someday.</t>
+  </si>
+  <si>
+    <t>Aryasi is upset that I disturbed her relatives remains, and she is no longer speaking to me.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estarnged_Spirits.Journal == 30, tlvoat_Othral_Disturb1_State == 1</t>
+  </si>
+  <si>
+    <t>I spent a lot of effort trying to reach out to my family's spirits, but they are silent to me. I can't tell if they are still pushing me away, or that they are silent because you did the ONE thing I told you NOT to do! Was not disturbing the remains of my family really too much for you? Get out of my sight. I wish that we had never met.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estarnged_Spirits.Journal == 30, tlvoat_Othral_Disturb1_State == 1, tlvoat_hasPCSaidInTemple == 1</t>
+  </si>
+  <si>
+    <t>Who are you %PCName? You couldn't possibly be a priest from the Temple, given that you disturbed my family's remains. What priest would do that? You need to leave.</t>
+  </si>
+  <si>
+    <t>SetDisposition 0, Journal "tlvoat_Estranged_Spirits", 150, Goodbye</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 150</t>
+  </si>
+  <si>
+    <t>Go away.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 70, tlvoat_Othral_Disturb1_State == 1</t>
+  </si>
+  <si>
+    <t>I hate you %PCName. From the depths of my heart I curse you. Why would you disturb my grandmother's remains? Why? Right at the point when I felt hopeful and happy to find a connection with my past and you took it away. You are a cruel and disturbing person. I never want to see you ever again. Leave me.</t>
   </si>
 </sst>
 </file>
@@ -2016,10 +2046,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
-  <dimension ref="A2:F22"/>
+  <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2269,19 +2299,16 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>169</v>
+        <v>358</v>
       </c>
       <c r="D16">
-        <v>200</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="F16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2289,19 +2316,19 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>128</v>
+        <v>169</v>
       </c>
       <c r="D17">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2309,19 +2336,19 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="D18">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>36</v>
+        <v>167</v>
       </c>
       <c r="F18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2329,10 +2356,13 @@
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>237</v>
+        <v>173</v>
       </c>
       <c r="D19">
-        <v>500</v>
+        <v>400</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F19" t="s">
         <v>35</v>
@@ -2346,16 +2376,16 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>289</v>
+        <v>237</v>
       </c>
       <c r="D20">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="F20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2363,10 +2393,10 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D21">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="F21" t="s">
         <v>35</v>
@@ -2380,17 +2410,34 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D22">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F22" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23">
+        <v>701</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F4 B5:E38 F6:F8 F14 F16:F17 F19:F22">
+  <conditionalFormatting sqref="B3:F4 F6:F8 F14 F20:F23 B5:E39 F16:F18">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2682,10 +2729,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F89"/>
+  <dimension ref="A2:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B89" sqref="B3:B89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2947,7 +2994,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2958,13 +3005,16 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>161</v>
+        <v>362</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="F16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2975,10 +3025,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>321</v>
+        <v>360</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="F17" t="s">
-        <v>320</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2992,13 +3045,13 @@
         <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>244</v>
+        <v>161</v>
       </c>
       <c r="F18" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -3009,10 +3062,10 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>176</v>
+        <v>321</v>
       </c>
       <c r="F19" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3026,13 +3079,13 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>332</v>
+        <v>244</v>
       </c>
       <c r="F20" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -3043,10 +3096,10 @@
         <v>110</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3060,10 +3113,10 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>245</v>
+        <v>332</v>
       </c>
       <c r="F22" t="s">
-        <v>247</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3077,13 +3130,10 @@
         <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="F23" t="s">
-        <v>182</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3097,13 +3147,10 @@
         <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="F24" t="s">
-        <v>217</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3117,16 +3164,16 @@
         <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F25" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -3137,10 +3184,13 @@
         <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="F26" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3154,13 +3204,16 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>328</v>
+        <v>249</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -3171,10 +3224,13 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>251</v>
+        <v>367</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="F28" t="s">
-        <v>252</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3185,19 +3241,16 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>347</v>
+        <v>250</v>
       </c>
       <c r="F29" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3205,19 +3258,16 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="F30" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -3225,16 +3275,16 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>149</v>
+        <v>365</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>147</v>
+        <v>364</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3245,19 +3295,16 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>151</v>
+        <v>251</v>
       </c>
       <c r="F32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -3268,16 +3315,16 @@
         <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>155</v>
+        <v>254</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>193</v>
+        <v>347</v>
       </c>
       <c r="F33" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -3288,13 +3335,16 @@
         <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>156</v>
+        <v>185</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="F34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -3305,13 +3355,13 @@
         <v>103</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>263</v>
+        <v>149</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
       <c r="F35" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -3325,10 +3375,13 @@
         <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F36" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3342,16 +3395,16 @@
         <v>103</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="F37" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -3362,16 +3415,13 @@
         <v>103</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>207</v>
+        <v>156</v>
       </c>
       <c r="F38" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3382,16 +3432,16 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>340</v>
+        <v>263</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>342</v>
+        <v>192</v>
       </c>
       <c r="F39" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -3402,16 +3452,13 @@
         <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>349</v>
+        <v>191</v>
       </c>
       <c r="F40" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3422,16 +3469,16 @@
         <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>343</v>
+        <v>189</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>350</v>
+        <v>206</v>
       </c>
       <c r="F41" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -3442,16 +3489,16 @@
         <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>253</v>
+        <v>189</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>339</v>
+        <v>207</v>
       </c>
       <c r="F42" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -3462,16 +3509,16 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="F43" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -3482,16 +3529,16 @@
         <v>103</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>261</v>
+        <v>341</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>258</v>
+        <v>349</v>
       </c>
       <c r="F44" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -3502,16 +3549,16 @@
         <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>262</v>
+        <v>343</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>259</v>
+        <v>350</v>
       </c>
       <c r="F45" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -3522,13 +3569,16 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="F46" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3539,13 +3589,13 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>257</v>
+        <v>338</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>259</v>
+        <v>339</v>
       </c>
       <c r="F47" t="s">
-        <v>309</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3559,13 +3609,13 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>258</v>
       </c>
       <c r="F48" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3579,16 +3629,16 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>351</v>
+        <v>262</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>345</v>
+        <v>259</v>
       </c>
       <c r="F49" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3599,13 +3649,10 @@
         <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>345</v>
+        <v>255</v>
       </c>
       <c r="F50" t="s">
-        <v>346</v>
+        <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3619,16 +3666,16 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>354</v>
+        <v>257</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>311</v>
+        <v>259</v>
       </c>
       <c r="F51" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -3639,16 +3686,16 @@
         <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>311</v>
+        <v>258</v>
       </c>
       <c r="F52" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -3659,13 +3706,16 @@
         <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>264</v>
+        <v>351</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="F53" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -3676,84 +3726,87 @@
         <v>103</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F54" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F55" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" t="s">
+        <v>103</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F56" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F57" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" t="s">
+        <v>103</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" t="s">
-        <v>160</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F55" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56" t="s">
-        <v>160</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="F56" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" t="s">
-        <v>160</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="F57" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58" t="s">
-        <v>160</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E58" t="s">
-        <v>270</v>
-      </c>
-      <c r="F58" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3764,16 +3817,16 @@
         <v>160</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>268</v>
+        <v>162</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F59" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3784,13 +3837,13 @@
         <v>160</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>271</v>
+        <v>312</v>
       </c>
       <c r="F60" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3801,13 +3854,13 @@
         <v>160</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>196</v>
+        <v>269</v>
       </c>
       <c r="F61" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3818,13 +3871,16 @@
         <v>160</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
+      </c>
+      <c r="E62" t="s">
+        <v>270</v>
       </c>
       <c r="F62" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3835,10 +3891,13 @@
         <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>318</v>
+        <v>268</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="F63" t="s">
-        <v>315</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3852,13 +3911,13 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F64" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -3866,16 +3925,13 @@
         <v>29</v>
       </c>
       <c r="C65" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="F65" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3886,19 +3942,16 @@
         <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>278</v>
+        <v>317</v>
       </c>
       <c r="F66" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -3906,19 +3959,16 @@
         <v>29</v>
       </c>
       <c r="C67" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>175</v>
+        <v>318</v>
       </c>
       <c r="F67" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -3926,19 +3976,16 @@
         <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F68" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3949,16 +3996,16 @@
         <v>108</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>330</v>
+        <v>284</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="F69" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -3969,13 +4016,16 @@
         <v>108</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>198</v>
+        <v>166</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="F70" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -3986,16 +4036,16 @@
         <v>108</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>288</v>
+        <v>170</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>290</v>
+        <v>175</v>
       </c>
       <c r="F71" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4006,13 +4056,13 @@
         <v>108</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="F72" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4026,16 +4076,16 @@
         <v>108</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>288</v>
+        <v>330</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>292</v>
+        <v>199</v>
       </c>
       <c r="F73" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4046,16 +4096,13 @@
         <v>108</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>275</v>
+        <v>198</v>
       </c>
       <c r="F74" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4066,16 +4113,16 @@
         <v>108</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="F75" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4086,16 +4133,16 @@
         <v>108</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="F76" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4106,16 +4153,16 @@
         <v>108</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>197</v>
+        <v>288</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>329</v>
+        <v>292</v>
       </c>
       <c r="F77" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -4126,13 +4173,16 @@
         <v>108</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>319</v>
+        <v>274</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="F78" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4143,13 +4193,16 @@
         <v>108</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>326</v>
+        <v>281</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="F79" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4160,13 +4213,16 @@
         <v>108</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>327</v>
+        <v>282</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>287</v>
       </c>
       <c r="F80" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4177,13 +4233,16 @@
         <v>108</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>293</v>
+        <v>197</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="F81" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4191,19 +4250,16 @@
         <v>29</v>
       </c>
       <c r="C82" t="s">
-        <v>218</v>
+        <v>108</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
       <c r="F82" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4211,16 +4267,13 @@
         <v>29</v>
       </c>
       <c r="C83" t="s">
-        <v>218</v>
+        <v>108</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>228</v>
+        <v>326</v>
       </c>
       <c r="F83" t="s">
-        <v>225</v>
+        <v>324</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4231,19 +4284,16 @@
         <v>29</v>
       </c>
       <c r="C84" t="s">
-        <v>218</v>
+        <v>108</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>228</v>
+        <v>327</v>
       </c>
       <c r="F84" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4251,19 +4301,16 @@
         <v>29</v>
       </c>
       <c r="C85" t="s">
-        <v>218</v>
+        <v>108</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>228</v>
+        <v>293</v>
       </c>
       <c r="F85" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -4274,16 +4321,16 @@
         <v>218</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>302</v>
+        <v>224</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>228</v>
+        <v>296</v>
       </c>
       <c r="F86" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4294,16 +4341,16 @@
         <v>218</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>295</v>
+        <v>226</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="F87" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -4314,13 +4361,16 @@
         <v>218</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="F88" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -4331,14 +4381,91 @@
         <v>218</v>
       </c>
       <c r="D89" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F89" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" t="s">
+        <v>29</v>
+      </c>
+      <c r="C90" t="s">
+        <v>218</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F90" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" t="s">
+        <v>29</v>
+      </c>
+      <c r="C91" t="s">
+        <v>218</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F91" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" t="s">
+        <v>218</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F92" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>14</v>
+      </c>
+      <c r="B93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" t="s">
+        <v>218</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F93" t="s">
         <v>298</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F114">
+  <conditionalFormatting sqref="B3:F118">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -4533,7 +4660,7 @@
   <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4555,7 +4682,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -4569,7 +4696,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
@@ -4583,7 +4710,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Add: additional dialogue disposition changes
Update: replace final two urns in secret area with loot
Update: reduce ring enchant and ring value
Add: message when PC presses shrine switch
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF75AF7A-C226-4A5A-9B16-ED8364030CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFF58DF-6FD5-4994-BE1C-BF848A204645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="369">
   <si>
     <t>Name</t>
   </si>
@@ -663,9 +663,6 @@
     <t>Handles timer &amp; Aryasi PositionCell</t>
   </si>
   <si>
-    <t>StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
-  </si>
-  <si>
     <t>Journal "tlvoat_Estranged_Spirits", 30, ModDisposition 5, StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
   </si>
   <si>
@@ -732,9 +729,6 @@
     <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. She gave me a ring that was her grandmother's.</t>
   </si>
   <si>
-    <t>Journal "tlvoat_Estranged_Spirits", 101</t>
-  </si>
-  <si>
     <t>tlvoat_urn_uravasa_uni_script</t>
   </si>
   <si>
@@ -1137,9 +1131,6 @@
     <t>Who are you %PCName? You couldn't possibly be a priest from the Temple, given that you disturbed my family's remains. What priest would do that? You need to leave.</t>
   </si>
   <si>
-    <t>SetDisposition 0, Journal "tlvoat_Estranged_Spirits", 150, Goodbye</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal == 150</t>
   </si>
   <si>
@@ -1150,6 +1141,18 @@
   </si>
   <si>
     <t>I hate you %PCName. From the depths of my heart I curse you. Why would you disturb my grandmother's remains? Why? Right at the point when I felt hopeful and happy to find a connection with my past and you took it away. You are a cruel and disturbing person. I never want to see you ever again. Leave me.</t>
+  </si>
+  <si>
+    <t>ModDisposition -100, Journal "tlvoat_Estranged_Spirits", 150, Goodbye</t>
+  </si>
+  <si>
+    <t>ModDisposition 5, Journal "tlvoat_Estranged_Spirits", 101</t>
+  </si>
+  <si>
+    <t>ModDisposition 7, Journal "tlvoat_Estranged_Spirits", 101</t>
+  </si>
+  <si>
+    <t>ModDisposition 10, StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
   </si>
 </sst>
 </file>
@@ -1910,7 +1913,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1919,7 +1922,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2132,7 +2135,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -2152,7 +2155,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D7">
         <v>31</v>
@@ -2172,7 +2175,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2186,7 +2189,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2203,7 +2206,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -2217,7 +2220,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2234,7 +2237,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2248,13 +2251,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2265,7 +2268,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -2299,7 +2302,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D16">
         <v>150</v>
@@ -2376,7 +2379,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D20">
         <v>500</v>
@@ -2393,7 +2396,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D21">
         <v>600</v>
@@ -2410,7 +2413,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D22">
         <v>700</v>
@@ -2427,7 +2430,7 @@
         <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D23">
         <v>701</v>
@@ -2437,7 +2440,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F4 F6:F8 F14 F20:F23 B5:E39 F16:F18">
+  <conditionalFormatting sqref="B3:F4 B5:E39 F6:F8 F14 F16:F18 F20:F23">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2731,8 +2734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
   <dimension ref="A2:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2812,7 +2815,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F5" t="s">
         <v>140</v>
@@ -2829,7 +2832,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F6" t="s">
         <v>141</v>
@@ -2846,7 +2849,7 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F7" t="s">
         <v>142</v>
@@ -2863,7 +2866,7 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F8" t="s">
         <v>143</v>
@@ -2880,7 +2883,7 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F9" t="s">
         <v>150</v>
@@ -2897,10 +2900,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2914,10 +2917,10 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2965,13 +2968,13 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2985,13 +2988,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3005,13 +3008,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="F16" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3025,13 +3028,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="F17" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3062,10 +3065,10 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F19" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3079,10 +3082,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3099,7 +3102,7 @@
         <v>176</v>
       </c>
       <c r="F21" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3113,10 +3116,10 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F22" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3133,7 +3136,7 @@
         <v>177</v>
       </c>
       <c r="F23" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3147,10 +3150,10 @@
         <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F24" t="s">
         <v>245</v>
-      </c>
-      <c r="F24" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3164,7 +3167,7 @@
         <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>113</v>
@@ -3184,13 +3187,13 @@
         <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>205</v>
+        <v>368</v>
       </c>
       <c r="F26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3204,13 +3207,13 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3224,13 +3227,13 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F28" t="s">
         <v>363</v>
-      </c>
-      <c r="F28" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3244,10 +3247,10 @@
         <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3261,10 +3264,10 @@
         <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F30" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3278,13 +3281,13 @@
         <v>110</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3298,10 +3301,10 @@
         <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F32" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3315,10 +3318,10 @@
         <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F33" t="s">
         <v>144</v>
@@ -3338,7 +3341,7 @@
         <v>185</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F34" t="s">
         <v>146</v>
@@ -3432,7 +3435,7 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>192</v>
@@ -3472,7 +3475,7 @@
         <v>189</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F41" t="s">
         <v>188</v>
@@ -3492,7 +3495,7 @@
         <v>189</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F42" t="s">
         <v>190</v>
@@ -3509,13 +3512,13 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>342</v>
-      </c>
       <c r="F43" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3529,13 +3532,13 @@
         <v>103</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F44" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3549,13 +3552,13 @@
         <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F45" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3569,10 +3572,10 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F46" t="s">
         <v>145</v>
@@ -3589,10 +3592,10 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F47" t="s">
         <v>150</v>
@@ -3609,13 +3612,13 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F48" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3629,13 +3632,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F49" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3649,10 +3652,10 @@
         <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3666,13 +3669,13 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="F51" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3686,13 +3689,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F52" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3706,13 +3709,13 @@
         <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F53" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3726,13 +3729,13 @@
         <v>103</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="F54" t="s">
         <v>344</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="F54" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3746,13 +3749,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F55" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3766,13 +3769,13 @@
         <v>103</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F56" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3786,7 +3789,7 @@
         <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F57" t="s">
         <v>194</v>
@@ -3803,7 +3806,7 @@
         <v>103</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
@@ -3837,7 +3840,7 @@
         <v>160</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F60" t="s">
         <v>146</v>
@@ -3854,7 +3857,7 @@
         <v>160</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F61" t="s">
         <v>147</v>
@@ -3871,10 +3874,10 @@
         <v>160</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E62" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F62" t="s">
         <v>148</v>
@@ -3891,13 +3894,13 @@
         <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>164</v>
       </c>
       <c r="F63" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3911,7 +3914,7 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F64" t="s">
         <v>165</v>
@@ -3945,10 +3948,10 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F66" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3962,10 +3965,10 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F67" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3979,10 +3982,10 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F68" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3996,7 +3999,7 @@
         <v>108</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>171</v>
@@ -4019,7 +4022,7 @@
         <v>166</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F70" t="s">
         <v>146</v>
@@ -4056,10 +4059,10 @@
         <v>108</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F72" t="s">
         <v>148</v>
@@ -4076,7 +4079,7 @@
         <v>108</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>199</v>
@@ -4113,10 +4116,10 @@
         <v>108</v>
       </c>
       <c r="D75" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="F75" t="s">
         <v>153</v>
@@ -4133,10 +4136,10 @@
         <v>108</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F76" t="s">
         <v>187</v>
@@ -4153,10 +4156,10 @@
         <v>108</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F77" t="s">
         <v>188</v>
@@ -4173,10 +4176,10 @@
         <v>108</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F78" t="s">
         <v>172</v>
@@ -4193,13 +4196,13 @@
         <v>108</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F79" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4213,13 +4216,13 @@
         <v>108</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F80" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="216" x14ac:dyDescent="0.3">
@@ -4236,10 +4239,10 @@
         <v>197</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F81" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4253,10 +4256,10 @@
         <v>108</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F82" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -4270,10 +4273,10 @@
         <v>108</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F83" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4287,10 +4290,10 @@
         <v>108</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F84" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -4304,10 +4307,10 @@
         <v>108</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F85" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -4318,13 +4321,13 @@
         <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F86" t="s">
         <v>144</v>
@@ -4338,16 +4341,16 @@
         <v>29</v>
       </c>
       <c r="C87" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>228</v>
+        <v>366</v>
       </c>
       <c r="F87" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4358,16 +4361,16 @@
         <v>29</v>
       </c>
       <c r="C88" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>228</v>
+        <v>366</v>
       </c>
       <c r="F88" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4378,36 +4381,36 @@
         <v>29</v>
       </c>
       <c r="C89" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>228</v>
+        <v>367</v>
       </c>
       <c r="F89" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" t="s">
+        <v>29</v>
+      </c>
+      <c r="C90" t="s">
+        <v>217</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>14</v>
-      </c>
-      <c r="B90" t="s">
-        <v>29</v>
-      </c>
-      <c r="C90" t="s">
-        <v>218</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="E90" s="2" t="s">
-        <v>228</v>
+        <v>366</v>
       </c>
       <c r="F90" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4418,16 +4421,16 @@
         <v>29</v>
       </c>
       <c r="C91" t="s">
+        <v>217</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F91" t="s">
         <v>218</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F91" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -4438,13 +4441,13 @@
         <v>29</v>
       </c>
       <c r="C92" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F92" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4455,13 +4458,13 @@
         <v>29</v>
       </c>
       <c r="C93" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F93" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -4769,13 +4772,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" t="s">
         <v>220</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>221</v>
-      </c>
-      <c r="D9" t="s">
-        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: additional lines to allow PC to interrupt Aryasi during "speech"
Add: fire and cheap food sack by Aryasi's bedroll
Add: Veloth fresco to main room
Fix: typo in README
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFF58DF-6FD5-4994-BE1C-BF848A204645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DE5F9B-EFEA-45DF-A436-740F36535319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="380">
   <si>
     <t>Name</t>
   </si>
@@ -540,9 +540,6 @@
     <t>if PC in Temple: Choice "I'm sorry to hear that your family pushed you away.", 2, "Was there anyone in your family who you had a good relationship with?", 3, "Just as Ghostfence is a monument to Dunmer pride in overcoming our enemies, so too should you in standing up for yourself against a family that should know better.", 4 ELSE Choice "I'm sorry to hear that your family pushed you away.", 2, "Was there anyone in your family who you had a good relationship with?", 3</t>
   </si>
   <si>
-    <t>Choice "Continue", 1, set tlvoat_hasAskedAboutSpirits to 1</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal == 30, tlvoat_hasAskedAboutSpirits = 1</t>
   </si>
   <si>
@@ -1153,6 +1150,42 @@
   </si>
   <si>
     <t>ModDisposition 10, StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
+  </si>
+  <si>
+    <t>Choice = 20</t>
+  </si>
+  <si>
+    <t>Choice = 20, tlvoat_hasHighReward1 = 1</t>
+  </si>
+  <si>
+    <t>Choice = 21</t>
+  </si>
+  <si>
+    <t>IF tlvoat_hasPCReceivedReward1 = 0: Choice "[Let her continue.]", 1, "[Interrupt] Hey! They're dead, you're alive. And I'd like to get paid.", 20, "[Interrupt] Easy now, take a deep breath.", 21 ELSE Choice "[Let her continue.]", 1, "[Interrupt] Easy now, take a deep breath.", 21; set tlvoat_hasAskedAboutSpirits to 1</t>
+  </si>
+  <si>
+    <t>Your pay, right, I had forgotten. Here's your 70 gold. I don't suppose you could help me out again by looking for a hidden section of the tomb?</t>
+  </si>
+  <si>
+    <t>It was 50 gold I promised right? Here. While you're here could I ask you to help me again by looking for a hidden section of the tomb?</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1; set tlvoat_hasPCInterruptSpeech to 1</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 50; Player-&gt;AddItem Gold_001, 50; set tlvoat_hasPCReceivedReward1; set tlvoat_hasPCInterruptSpeech to 1</t>
+  </si>
+  <si>
+    <t>set tlvoat_hasPCInterruptSpeech to 1</t>
+  </si>
+  <si>
+    <t>I'm sorry about that. Being here and trying to speak with them again has brought up a lot of old feelings, made worse because I can't hear my grandmother's spirit. I used to suspect that she was laid to rest in a hidden section of the tomb, and if that's true, then maybe that's why I can't hear her.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 30; tlvoat_hasPCInterruptSpeech == 1</t>
+  </si>
+  <si>
+    <t>I once saw my mother do something to the shrine when she was going through one of her moments of deeply missing grandmother. I checked it out a few times, but I couldn't find anything. Perhaps your more capable hands and eyes might pick something out?</t>
   </si>
 </sst>
 </file>
@@ -1814,16 +1847,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1831,7 +1864,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -1840,7 +1873,7 @@
         <v>135</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1899,13 +1932,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1913,7 +1946,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1922,7 +1955,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2087,7 +2120,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2098,7 +2131,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -2118,7 +2151,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -2135,7 +2168,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -2155,7 +2188,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D7">
         <v>31</v>
@@ -2175,7 +2208,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2189,7 +2222,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2206,7 +2239,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -2220,7 +2253,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2237,7 +2270,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2251,13 +2284,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2268,7 +2301,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -2285,7 +2318,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D15">
         <v>101</v>
@@ -2302,7 +2335,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D16">
         <v>150</v>
@@ -2319,13 +2352,13 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D17">
         <v>200</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
@@ -2345,7 +2378,7 @@
         <v>300</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F18" t="s">
         <v>35</v>
@@ -2359,7 +2392,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D19">
         <v>400</v>
@@ -2379,7 +2412,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D20">
         <v>500</v>
@@ -2396,7 +2429,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D21">
         <v>600</v>
@@ -2413,7 +2446,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D22">
         <v>700</v>
@@ -2430,7 +2463,7 @@
         <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D23">
         <v>701</v>
@@ -2732,10 +2765,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F93"/>
+  <dimension ref="A2:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2815,7 +2848,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F5" t="s">
         <v>140</v>
@@ -2832,7 +2865,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F6" t="s">
         <v>141</v>
@@ -2849,7 +2882,7 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F7" t="s">
         <v>142</v>
@@ -2866,7 +2899,7 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F8" t="s">
         <v>143</v>
@@ -2883,7 +2916,7 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F9" t="s">
         <v>150</v>
@@ -2900,10 +2933,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2917,10 +2950,10 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F11" t="s">
         <v>236</v>
-      </c>
-      <c r="F11" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2937,7 +2970,7 @@
         <v>138</v>
       </c>
       <c r="F12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2968,13 +3001,13 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2988,13 +3021,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3008,13 +3041,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3028,13 +3061,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3065,10 +3098,10 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3082,10 +3115,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3099,10 +3132,10 @@
         <v>110</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3116,10 +3149,10 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3133,10 +3166,10 @@
         <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3150,10 +3183,10 @@
         <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3167,13 +3200,13 @@
         <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3187,13 +3220,13 @@
         <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3207,13 +3240,13 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3227,13 +3260,13 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>365</v>
-      </c>
       <c r="F28" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3247,10 +3280,10 @@
         <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3264,10 +3297,10 @@
         <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3281,13 +3314,13 @@
         <v>110</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3301,10 +3334,10 @@
         <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F32" t="s">
         <v>249</v>
-      </c>
-      <c r="F32" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3318,10 +3351,10 @@
         <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F33" t="s">
         <v>144</v>
@@ -3338,10 +3371,10 @@
         <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F34" t="s">
         <v>146</v>
@@ -3378,7 +3411,7 @@
         <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>151</v>
@@ -3401,7 +3434,7 @@
         <v>155</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F37" t="s">
         <v>152</v>
@@ -3435,10 +3468,10 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F39" t="s">
         <v>153</v>
@@ -3455,10 +3488,10 @@
         <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3472,13 +3505,13 @@
         <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3492,13 +3525,13 @@
         <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F42" t="s">
         <v>189</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F42" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3512,13 +3545,13 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F43" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3532,13 +3565,13 @@
         <v>103</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3552,13 +3585,13 @@
         <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F45" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3572,10 +3605,10 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F46" t="s">
         <v>145</v>
@@ -3592,10 +3625,10 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="F47" t="s">
         <v>150</v>
@@ -3612,13 +3645,13 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3632,13 +3665,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F49" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3652,10 +3685,10 @@
         <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F50" t="s">
         <v>253</v>
-      </c>
-      <c r="F50" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3669,13 +3702,13 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F51" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3689,13 +3722,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F52" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3709,13 +3742,13 @@
         <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="F53" t="s">
         <v>349</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="F53" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3729,13 +3762,13 @@
         <v>103</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" t="s">
         <v>343</v>
-      </c>
-      <c r="F54" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3749,13 +3782,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F55" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3769,13 +3802,13 @@
         <v>103</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F56" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3789,10 +3822,10 @@
         <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F57" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -3806,7 +3839,7 @@
         <v>103</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
@@ -3840,7 +3873,7 @@
         <v>160</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F60" t="s">
         <v>146</v>
@@ -3857,7 +3890,7 @@
         <v>160</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F61" t="s">
         <v>147</v>
@@ -3874,16 +3907,16 @@
         <v>160</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E62" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F62" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3894,16 +3927,16 @@
         <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>266</v>
+        <v>372</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>164</v>
+        <v>374</v>
       </c>
       <c r="F63" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -3914,13 +3947,16 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>269</v>
+        <v>373</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="F64" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -3931,13 +3967,16 @@
         <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>196</v>
+        <v>377</v>
+      </c>
+      <c r="E65" t="s">
+        <v>376</v>
       </c>
       <c r="F65" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3948,10 +3987,13 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>315</v>
+        <v>265</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>371</v>
       </c>
       <c r="F66" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3965,10 +4007,10 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>316</v>
+        <v>268</v>
       </c>
       <c r="F67" t="s">
-        <v>313</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3982,13 +4024,13 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>271</v>
+        <v>195</v>
       </c>
       <c r="F68" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3996,16 +4038,13 @@
         <v>29</v>
       </c>
       <c r="C69" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>171</v>
+        <v>314</v>
       </c>
       <c r="F69" t="s">
-        <v>144</v>
+        <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4016,19 +4055,16 @@
         <v>29</v>
       </c>
       <c r="C70" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>276</v>
+        <v>315</v>
       </c>
       <c r="F70" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -4036,19 +4072,16 @@
         <v>29</v>
       </c>
       <c r="C71" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>175</v>
+        <v>270</v>
       </c>
       <c r="F71" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4062,10 +4095,10 @@
         <v>281</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>274</v>
+        <v>170</v>
       </c>
       <c r="F72" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4079,16 +4112,16 @@
         <v>108</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>328</v>
+        <v>165</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>199</v>
+        <v>275</v>
       </c>
       <c r="F73" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4099,13 +4132,16 @@
         <v>108</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>198</v>
+        <v>169</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="F74" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4116,13 +4152,13 @@
         <v>108</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="F75" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4136,16 +4172,16 @@
         <v>108</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>286</v>
+        <v>327</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>289</v>
+        <v>198</v>
       </c>
       <c r="F76" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4156,16 +4192,13 @@
         <v>108</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>290</v>
+        <v>197</v>
       </c>
       <c r="F77" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -4176,16 +4209,16 @@
         <v>108</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="F78" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4196,16 +4229,16 @@
         <v>108</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="F79" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4216,16 +4249,16 @@
         <v>108</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="F80" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4236,16 +4269,16 @@
         <v>108</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>197</v>
+        <v>379</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>327</v>
+        <v>272</v>
       </c>
       <c r="F81" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4256,13 +4289,16 @@
         <v>108</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>317</v>
+        <v>271</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="F82" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4273,13 +4309,16 @@
         <v>108</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>324</v>
+        <v>278</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="F83" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4290,13 +4329,16 @@
         <v>108</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>325</v>
+        <v>279</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>284</v>
       </c>
       <c r="F84" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4307,13 +4349,16 @@
         <v>108</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>291</v>
+        <v>196</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="F85" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -4321,19 +4366,16 @@
         <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>294</v>
+        <v>316</v>
       </c>
       <c r="F86" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4341,16 +4383,13 @@
         <v>29</v>
       </c>
       <c r="C87" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>366</v>
+        <v>323</v>
       </c>
       <c r="F87" t="s">
-        <v>224</v>
+        <v>321</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4361,19 +4400,16 @@
         <v>29</v>
       </c>
       <c r="C88" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>366</v>
+        <v>324</v>
       </c>
       <c r="F88" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -4381,19 +4417,16 @@
         <v>29</v>
       </c>
       <c r="C89" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>367</v>
+        <v>290</v>
       </c>
       <c r="F89" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4401,19 +4434,19 @@
         <v>29</v>
       </c>
       <c r="C90" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>300</v>
+        <v>222</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>366</v>
+        <v>293</v>
       </c>
       <c r="F90" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4421,19 +4454,19 @@
         <v>29</v>
       </c>
       <c r="C91" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>293</v>
+        <v>224</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>222</v>
+        <v>365</v>
       </c>
       <c r="F91" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -4441,34 +4474,114 @@
         <v>29</v>
       </c>
       <c r="C92" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>354</v>
       </c>
+      <c r="E92" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="F92" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>14</v>
+      </c>
+      <c r="B93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" t="s">
+        <v>216</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F93" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" t="s">
+        <v>216</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F94" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>14</v>
+      </c>
+      <c r="B95" t="s">
+        <v>29</v>
+      </c>
+      <c r="C95" t="s">
+        <v>216</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F95" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>14</v>
+      </c>
+      <c r="B96" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" t="s">
+        <v>216</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="F96" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>14</v>
+      </c>
+      <c r="B97" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" t="s">
+        <v>216</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F97" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>14</v>
-      </c>
-      <c r="B93" t="s">
-        <v>29</v>
-      </c>
-      <c r="C93" t="s">
-        <v>217</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="F93" t="s">
-        <v>296</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F118">
+  <conditionalFormatting sqref="B3:F122">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -4772,13 +4885,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" t="s">
         <v>219</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>220</v>
-      </c>
-      <c r="D9" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Full review of dialogue, applying adjustments where needed.
Add: northmarker
Add: ability for PC to report being unable to clear the tomb
Fix: PC killing Aryasi after quest triggering a journal update
Update: slight buff to health and attack 1 for melee skeletons
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DE5F9B-EFEA-45DF-A436-740F36535319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5713783C-1FA1-47AE-B527-C2CC911FBABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="386">
   <si>
     <t>Name</t>
   </si>
@@ -633,9 +633,6 @@
     <t>tlvoat_Estranged_Spirits.journal &lt;= 50</t>
   </si>
   <si>
-    <t>While most of my family continue to push me away, I hope my grandmother does not react in the same way.</t>
-  </si>
-  <si>
     <t>Any luck with the shrine?</t>
   </si>
   <si>
@@ -744,9 +741,6 @@
     <t>%PCName it's good to see you again. Have you found some time to help me clear the tomb?</t>
   </si>
   <si>
-    <t>Hey, excuse me, are you going in? I need to clear the tomb, would you be willing to help me out? Though if you don't want to I can't stop a powerful %PCClass such as yourself from going in anyway.</t>
-  </si>
-  <si>
     <t>I saw that you went in. Did you happen to clear the tomb so that it's safe even for me?</t>
   </si>
   <si>
@@ -783,9 +777,6 @@
     <t>tlvoat_Estranged_Spirits.Journal &lt;= 45</t>
   </si>
   <si>
-    <t>Oh my! This really is her urn! Thank you so much for taking me to my grandmother. Please, leave me for an hour so that I can have some time to speak with her spirit.</t>
-  </si>
-  <si>
     <t>Please come back to me in an hour.</t>
   </si>
   <si>
@@ -813,12 +804,6 @@
     <t>Is it safe to go in?</t>
   </si>
   <si>
-    <t>Choice "Yes, the tomb is now safe.", 5, "No, it's not yet safe for you to enter.", 6</t>
-  </si>
-  <si>
-    <t>Choice "(Lie) Yes, the tomb is now safe.", 7, "No, it's not yet safe for you to enter.", 6</t>
-  </si>
-  <si>
     <t>Is it safe to go in? You do look like you've seen some scrapes.</t>
   </si>
   <si>
@@ -831,9 +816,6 @@
     <t>It is? You seem rather untouched after dealing with the tomb's guardians. Well, I trust you %PCName, thank you for putting yourself in danger for me. Give me a little while so that I may converse with my family's spirits.</t>
   </si>
   <si>
-    <t>Thank you again sera %PCName for making my family's tomb safe enough for me to speak with my family. I've never met a priest like you before.</t>
-  </si>
-  <si>
     <t>tlvoat_Estranged_Spirits &gt;= 30, tlvoat_hasPCReceivedReward1 = 0</t>
   </si>
   <si>
@@ -858,9 +840,6 @@
     <t>tlvoat_Estranged_Spirits.journal &gt;= 70</t>
   </si>
   <si>
-    <t>I'm so happy that I've been able to reconnect with my grandmother. Thank you %PCName.</t>
-  </si>
-  <si>
     <t>Whenever I asked my parents they always denied it, but every time my mother expressed missing grandmother she would come to the tomb. Once, I followed her and watched as she prayed at the shrine, then after a while, she reached out to it and I heard something heavy move elsewhere in the tomb. But that was when she caught me and dragged me out. I investigated the shrine a few other times when I was alone, but found nothing. Maybe some fresh hands and eyes could reveal something?</t>
   </si>
   <si>
@@ -891,9 +870,6 @@
     <t>So I was right! I really don't want to get my hopes up too much, but please take a look. You're looking for an urn labelled "Uravasa Othral". There might also be more guardians in there so be careful.</t>
   </si>
   <si>
-    <t>You will? Thank you! I honestly wasn't expecting you to offer to help again. I recommend investigating the shrine first, but the switch might actually be elsewhere. If there is a hidden area then you're looking for an urn labelled "Uravasa Othral".</t>
-  </si>
-  <si>
     <t>I told Aryasi that I could not find her grandmother's resting place in the hidden section of Othral Ancestral Tomb.</t>
   </si>
   <si>
@@ -1038,12 +1014,6 @@
     <t>I'm happy that I was right about the shrine, but what's in the hidden section %PCName?</t>
   </si>
   <si>
-    <t>Hold on %PCName, let me enter my family's tomb first.</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal == 30, PCGetCell "OAT" == 0</t>
-  </si>
-  <si>
     <t>Choice = 11</t>
   </si>
   <si>
@@ -1059,18 +1029,12 @@
     <t>if PCRank Temple &gt;= 0: Choice "Yes, I can clear your family's tomb.", 1, "As a priest of the Temple I'd be happy to.", 2, "Up the gold and I'll do it.", 11, "I'm too busy right now.", 3, "No I will not.", 4 ELSE Choice "Yes, I can clear your family's tomb.", 1, "Up the gold and I'll do it.", 11, "I'm too busy right now.", 3, "No I will not.", 4</t>
   </si>
   <si>
-    <t>No I'm only offering the 50 gold as that's all I can spare. Are you going to do it or not?</t>
-  </si>
-  <si>
     <t>Fine, I'll make it 70 gold. Any higher and I'll really struggle to feed myself. If you want more then you can take the offerings left by grievers, as well as the family heirlooms. All I ask is to just leave their remains alone.</t>
   </si>
   <si>
     <t>ModDisposition -10, Choice "Fine, I'll do it.", 12, "No I won't.", 4</t>
   </si>
   <si>
-    <t>Good. I do appreciate this %PCClass, as I'm very much aware that I'm putting you in a lot of danger. There's offerings and the family heirlooms that you can take, as well as anything the guardians have. Just please leave my family's remains alone.</t>
-  </si>
-  <si>
     <t>Oh right I had forgotten. It was 70 right? Well here, you've earned it.</t>
   </si>
   <si>
@@ -1186,6 +1150,60 @@
   </si>
   <si>
     <t>I once saw my mother do something to the shrine when she was going through one of her moments of deeply missing grandmother. I checked it out a few times, but I couldn't find anything. Perhaps your more capable hands and eyes might pick something out?</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &gt;= 30, tlvoat_Estranged_Spirits.Journal &lt;= 31, PCGetCell "OAT" == 0</t>
+  </si>
+  <si>
+    <t>Hold on %PCName, allow me enter my family's tomb first.</t>
+  </si>
+  <si>
+    <t>Oh my! This really is her urn! Thank you so much for taking me to my grandmother. Please, leave me for an hour so that I can have some time to attempt to reach out to her spirit.</t>
+  </si>
+  <si>
+    <t>No I'm only offering the 50 gold as that's all I can spare. If you want more then you are free to take the offerings and family heirlooms. Are you going to do it or not?</t>
+  </si>
+  <si>
+    <t>Good. I do appreciate this %PCClass, as I'm very much aware that I'm putting you in a lot of danger. Like I said, there's offerings and the family heirlooms that you can take, as well as anything the guardians have. Just please leave my family's remains alone.</t>
+  </si>
+  <si>
+    <t>Thank you again sera %PCName for making my family's tomb safe enough for me to speak with my family.</t>
+  </si>
+  <si>
+    <t>I hope that my grandmother isn't as silent.</t>
+  </si>
+  <si>
+    <t>I'm so happy that I've been able to reconnect with my grandmother's spirit. Thank you %PCName.</t>
+  </si>
+  <si>
+    <t>You will? Thank you! I honestly wasn't expecting you to accept to help again. I recommend investigating the shrine first, but the switch might actually be elsewhere. If there is a hidden area then you're looking for an urn labelled "Uravasa Othral".</t>
+  </si>
+  <si>
+    <t>Choice = 3, tlvoat_hasPCInterruptSpeech = 1</t>
+  </si>
+  <si>
+    <t>I understand %PCName, as you have already put yourself in danger for me, a stranger. Thank you.</t>
+  </si>
+  <si>
+    <t>Oh, I… thank you for looking. Then I must not be any granddaughter of hers. Please, leave me. I need to be alone.</t>
+  </si>
+  <si>
+    <t>Hey, excuse me, are you going in? I need to clear the tomb, but I'm not enough of a mage to be able to do it. Would you be willing to help me out? Though if you don't want to I can't stop a powerful %PCClass such as yourself from going in anyway.</t>
+  </si>
+  <si>
+    <t>Choice = 13</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 500; Goodbye</t>
+  </si>
+  <si>
+    <t>Really? Oh, well, thank you for trying. It was worth a shot.</t>
+  </si>
+  <si>
+    <t>Choice "Yes, the tomb is now safe.", 5, "No, it's not yet safe for you to enter.", 6, "(Lie) I couldn't clear it.", 13</t>
+  </si>
+  <si>
+    <t>Choice "(Lie) Yes, the tomb is now safe.", 7, "No, it's not yet safe for you to enter.", 6, "I couldn't clear it.", 13</t>
   </si>
 </sst>
 </file>
@@ -1932,13 +1950,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1946,7 +1964,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1955,7 +1973,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2131,7 +2149,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -2151,7 +2169,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -2168,7 +2186,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -2188,7 +2206,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D7">
         <v>31</v>
@@ -2208,7 +2226,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2222,7 +2240,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2239,7 +2257,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -2253,7 +2271,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2270,7 +2288,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2284,13 +2302,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2301,7 +2319,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -2318,7 +2336,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D15">
         <v>101</v>
@@ -2335,7 +2353,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="D16">
         <v>150</v>
@@ -2412,7 +2430,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D20">
         <v>500</v>
@@ -2429,7 +2447,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D21">
         <v>600</v>
@@ -2446,7 +2464,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D22">
         <v>700</v>
@@ -2463,7 +2481,7 @@
         <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D23">
         <v>701</v>
@@ -2765,10 +2783,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F97"/>
+  <dimension ref="A2:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2848,7 +2866,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F5" t="s">
         <v>140</v>
@@ -2865,7 +2883,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>232</v>
+        <v>380</v>
       </c>
       <c r="F6" t="s">
         <v>141</v>
@@ -2882,7 +2900,7 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F7" t="s">
         <v>142</v>
@@ -2899,7 +2917,7 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F8" t="s">
         <v>143</v>
@@ -2916,7 +2934,7 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F9" t="s">
         <v>150</v>
@@ -2933,10 +2951,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2950,10 +2968,10 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3001,13 +3019,13 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -3021,13 +3039,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>330</v>
+        <v>369</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>331</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3041,13 +3059,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="F16" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3061,13 +3079,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="F17" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3098,10 +3116,10 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="F19" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3115,10 +3133,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F20" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3135,7 +3153,7 @@
         <v>175</v>
       </c>
       <c r="F21" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3149,10 +3167,10 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="F22" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3169,7 +3187,7 @@
         <v>176</v>
       </c>
       <c r="F23" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3183,10 +3201,10 @@
         <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F24" t="s">
         <v>242</v>
-      </c>
-      <c r="F24" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3200,7 +3218,7 @@
         <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>113</v>
@@ -3209,7 +3227,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -3220,13 +3238,13 @@
         <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>245</v>
+        <v>370</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="F26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3240,13 +3258,13 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3260,13 +3278,13 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="F28" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3280,10 +3298,10 @@
         <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3297,10 +3315,10 @@
         <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="F30" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3314,13 +3332,13 @@
         <v>110</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3334,10 +3352,10 @@
         <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F32" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3351,10 +3369,10 @@
         <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="F33" t="s">
         <v>144</v>
@@ -3374,7 +3392,7 @@
         <v>184</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="F34" t="s">
         <v>146</v>
@@ -3468,7 +3486,7 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>191</v>
@@ -3508,7 +3526,7 @@
         <v>188</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F41" t="s">
         <v>187</v>
@@ -3528,7 +3546,7 @@
         <v>188</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F42" t="s">
         <v>189</v>
@@ -3545,13 +3563,13 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>337</v>
+        <v>371</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="F43" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3565,13 +3583,13 @@
         <v>103</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="F44" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3585,16 +3603,16 @@
         <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>340</v>
+        <v>372</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="F45" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -3605,13 +3623,13 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>250</v>
+        <v>383</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>336</v>
+        <v>382</v>
       </c>
       <c r="F46" t="s">
-        <v>145</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3625,16 +3643,16 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>335</v>
+        <v>247</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="F47" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -3645,13 +3663,13 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>258</v>
+        <v>325</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>255</v>
+        <v>326</v>
       </c>
       <c r="F48" t="s">
-        <v>304</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3665,16 +3683,16 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>256</v>
+        <v>384</v>
       </c>
       <c r="F49" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3685,13 +3703,16 @@
         <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>385</v>
       </c>
       <c r="F50" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -3702,16 +3723,13 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F51" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -3722,13 +3740,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>255</v>
+        <v>385</v>
       </c>
       <c r="F52" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3742,13 +3760,13 @@
         <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>348</v>
+        <v>252</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>342</v>
+        <v>384</v>
       </c>
       <c r="F53" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3762,13 +3780,13 @@
         <v>103</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="F54" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3782,13 +3800,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="F55" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3802,16 +3820,16 @@
         <v>103</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>263</v>
+        <v>339</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="F56" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -3822,13 +3840,16 @@
         <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="F57" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3839,10 +3860,13 @@
         <v>103</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+      <c r="F58" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3850,19 +3874,13 @@
         <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F59" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3873,13 +3891,16 @@
         <v>160</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>309</v>
+        <v>162</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="F60" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3890,13 +3911,13 @@
         <v>160</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>266</v>
+        <v>301</v>
       </c>
       <c r="F61" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3907,16 +3928,13 @@
         <v>160</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E62" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="F62" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3927,13 +3945,13 @@
         <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>374</v>
+        <v>302</v>
+      </c>
+      <c r="E63" t="s">
+        <v>261</v>
       </c>
       <c r="F63" t="s">
-        <v>369</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3947,13 +3965,13 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="F64" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3967,16 +3985,16 @@
         <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="E65" t="s">
-        <v>376</v>
+        <v>361</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="F65" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3987,16 +4005,16 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
+      </c>
+      <c r="E66" t="s">
+        <v>364</v>
       </c>
       <c r="F66" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -4007,10 +4025,13 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>268</v>
+        <v>259</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>359</v>
       </c>
       <c r="F67" t="s">
-        <v>164</v>
+        <v>258</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4024,13 +4045,13 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>195</v>
+        <v>262</v>
       </c>
       <c r="F68" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -4041,10 +4062,10 @@
         <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>314</v>
+        <v>374</v>
       </c>
       <c r="F69" t="s">
-        <v>313</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4058,10 +4079,10 @@
         <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="F70" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4075,13 +4096,13 @@
         <v>160</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="F71" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4089,19 +4110,16 @@
         <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>170</v>
+        <v>375</v>
       </c>
       <c r="F72" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -4112,16 +4130,16 @@
         <v>108</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>165</v>
+        <v>376</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>275</v>
+        <v>170</v>
       </c>
       <c r="F73" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4132,16 +4150,16 @@
         <v>108</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>174</v>
+        <v>268</v>
       </c>
       <c r="F74" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4152,16 +4170,16 @@
         <v>108</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>280</v>
+        <v>378</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>273</v>
+        <v>174</v>
       </c>
       <c r="F75" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4172,16 +4190,16 @@
         <v>108</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>327</v>
+        <v>169</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="F76" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4192,10 +4210,13 @@
         <v>108</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>197</v>
+        <v>273</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>266</v>
       </c>
       <c r="F77" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4209,16 +4230,16 @@
         <v>108</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>285</v>
+        <v>319</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>287</v>
+        <v>197</v>
       </c>
       <c r="F78" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4229,13 +4250,10 @@
         <v>108</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>288</v>
+        <v>196</v>
       </c>
       <c r="F79" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4249,16 +4267,16 @@
         <v>108</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>285</v>
+        <v>379</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F80" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4272,13 +4290,13 @@
         <v>379</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="F81" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4289,13 +4307,13 @@
         <v>108</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="F82" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -4309,16 +4327,16 @@
         <v>108</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>278</v>
+        <v>367</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="F83" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4329,16 +4347,16 @@
         <v>108</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="F84" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4349,16 +4367,16 @@
         <v>108</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>196</v>
+        <v>271</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>326</v>
+        <v>270</v>
       </c>
       <c r="F85" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -4369,13 +4387,16 @@
         <v>108</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>316</v>
+        <v>272</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="F86" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4386,10 +4407,13 @@
         <v>108</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>323</v>
+        <v>195</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="F87" t="s">
-        <v>321</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4403,10 +4427,10 @@
         <v>108</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="F88" t="s">
-        <v>322</v>
+        <v>294</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -4420,13 +4444,13 @@
         <v>108</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="F89" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4434,56 +4458,50 @@
         <v>29</v>
       </c>
       <c r="C90" t="s">
-        <v>216</v>
+        <v>108</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="F90" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" t="s">
+        <v>29</v>
+      </c>
+      <c r="C91" t="s">
+        <v>108</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F91" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" t="s">
+        <v>215</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F92" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>14</v>
-      </c>
-      <c r="B91" t="s">
-        <v>29</v>
-      </c>
-      <c r="C91" t="s">
-        <v>216</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="F91" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>14</v>
-      </c>
-      <c r="B92" t="s">
-        <v>29</v>
-      </c>
-      <c r="C92" t="s">
-        <v>216</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="F92" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4494,16 +4512,16 @@
         <v>29</v>
       </c>
       <c r="C93" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>300</v>
+        <v>223</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="F93" t="s">
-        <v>297</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4514,19 +4532,19 @@
         <v>29</v>
       </c>
       <c r="C94" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>299</v>
+        <v>342</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="F94" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -4534,19 +4552,19 @@
         <v>29</v>
       </c>
       <c r="C95" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>292</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>221</v>
+        <v>354</v>
       </c>
       <c r="F95" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -4554,13 +4572,16 @@
         <v>29</v>
       </c>
       <c r="C96" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D96" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E96" s="2" t="s">
         <v>353</v>
       </c>
       <c r="F96" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4571,17 +4592,54 @@
         <v>29</v>
       </c>
       <c r="C97" t="s">
+        <v>215</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F97" t="s">
         <v>216</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F97" t="s">
-        <v>295</v>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>14</v>
+      </c>
+      <c r="B98" t="s">
+        <v>29</v>
+      </c>
+      <c r="C98" t="s">
+        <v>215</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="F98" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B99" t="s">
+        <v>29</v>
+      </c>
+      <c r="C99" t="s">
+        <v>215</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F99" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F122">
+  <conditionalFormatting sqref="B3:F124">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -4885,13 +4943,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" t="s">
         <v>218</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>219</v>
-      </c>
-      <c r="D9" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: flowchart for dialogue changes
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5713783C-1FA1-47AE-B527-C2CC911FBABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712A963F-89BE-4C90-8ED9-13BC4528C596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -2785,8 +2785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
   <dimension ref="A2:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update: rework of flow of dialogue during "speech"
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712A963F-89BE-4C90-8ED9-13BC4528C596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00E5D16-A8EF-43A7-81D0-3D6D4E0F4638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="400">
   <si>
     <t>Name</t>
   </si>
@@ -534,12 +534,6 @@
     <t>It feels… colder in here than I remember. I spent some time reaching out, but the spirits of my family are silent to me.</t>
   </si>
   <si>
-    <t>Ever since I… better understood who I am they pressured me to be who they wanted me to be. When that didn't work they turned to shame and mockery. Then it was denying what was promised to me as the firstborn, giving to my younger brothers Lletho and Jathys the family blade and armor. Eventually I took what I could and ran away. That was many years ago, and it was only recently that I received a letter from an old friend letting me know the fate of my family.</t>
-  </si>
-  <si>
-    <t>if PC in Temple: Choice "I'm sorry to hear that your family pushed you away.", 2, "Was there anyone in your family who you had a good relationship with?", 3, "Just as Ghostfence is a monument to Dunmer pride in overcoming our enemies, so too should you in standing up for yourself against a family that should know better.", 4 ELSE Choice "I'm sorry to hear that your family pushed you away.", 2, "Was there anyone in your family who you had a good relationship with?", 3</t>
-  </si>
-  <si>
     <t>tlvoat_estranged_spirits.Journal == 30, tlvoat_hasAskedAboutSpirits = 1</t>
   </si>
   <si>
@@ -831,9 +825,6 @@
     <t>Yes, there was: my grandmother. I can't hear her either, which makes everything hurt all the more. I find myself hoping that there's a hidden section of the tomb, just as I once did, and that she's there. And that's why I can't hear her, but I'm probably just letting myself be fooled by hope once again.</t>
   </si>
   <si>
-    <t>set tlvoat_PCMentionInTemple to 1</t>
-  </si>
-  <si>
     <t>They are remaining silent. I can't help but hope that my grandmother is in some hidden section.</t>
   </si>
   <si>
@@ -1119,33 +1110,12 @@
     <t>Choice = 20</t>
   </si>
   <si>
-    <t>Choice = 20, tlvoat_hasHighReward1 = 1</t>
-  </si>
-  <si>
     <t>Choice = 21</t>
   </si>
   <si>
-    <t>IF tlvoat_hasPCReceivedReward1 = 0: Choice "[Let her continue.]", 1, "[Interrupt] Hey! They're dead, you're alive. And I'd like to get paid.", 20, "[Interrupt] Easy now, take a deep breath.", 21 ELSE Choice "[Let her continue.]", 1, "[Interrupt] Easy now, take a deep breath.", 21; set tlvoat_hasAskedAboutSpirits to 1</t>
-  </si>
-  <si>
-    <t>Your pay, right, I had forgotten. Here's your 70 gold. I don't suppose you could help me out again by looking for a hidden section of the tomb?</t>
-  </si>
-  <si>
-    <t>It was 50 gold I promised right? Here. While you're here could I ask you to help me again by looking for a hidden section of the tomb?</t>
-  </si>
-  <si>
-    <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1; set tlvoat_hasPCInterruptSpeech to 1</t>
-  </si>
-  <si>
-    <t>RemoveItem Gold_001, 50; Player-&gt;AddItem Gold_001, 50; set tlvoat_hasPCReceivedReward1; set tlvoat_hasPCInterruptSpeech to 1</t>
-  </si>
-  <si>
     <t>set tlvoat_hasPCInterruptSpeech to 1</t>
   </si>
   <si>
-    <t>I'm sorry about that. Being here and trying to speak with them again has brought up a lot of old feelings, made worse because I can't hear my grandmother's spirit. I used to suspect that she was laid to rest in a hidden section of the tomb, and if that's true, then maybe that's why I can't hear her.</t>
-  </si>
-  <si>
     <t>tlvoat_Estranged_Spirits.Journal == 30; tlvoat_hasPCInterruptSpeech == 1</t>
   </si>
   <si>
@@ -1204,6 +1174,80 @@
   </si>
   <si>
     <t>Choice "(Lie) Yes, the tomb is now safe.", 7, "No, it's not yet safe for you to enter.", 6, "I couldn't clear it.", 13</t>
+  </si>
+  <si>
+    <t>They are here, as I can... sense their presence. No, they are choosing to keep me out. I am not family to them, and I haven't been for a long time.</t>
+  </si>
+  <si>
+    <t>IF tlvoat_hasPCReceivedReward1 = 0: Choice "You've been disowned?", 1, "I'm sorry to hear that, but I would like my gold before we continue.", 2 ELSE Choice "You've been disowned?", 1, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4; set tlvoat_hasAskedAboutSpirits to 1</t>
+  </si>
+  <si>
+    <t>Choice "[Let her continue.]", 10, "I wouldn't know. I didn't know my parents.", 11</t>
+  </si>
+  <si>
+    <t>Your pay, right, I had forgotten. Here's your 70 gold.</t>
+  </si>
+  <si>
+    <t>Of course! You were here to help, not listen to me. It was 50 gold I promised right? Here you go.</t>
+  </si>
+  <si>
+    <t>Well, while I can sense my family's spirits I can't work out who's who until they speak. I want to speak with my grandmother, but I don't know if she's here or in another part of the tomb. She should be in this room, and if she isn't then I can't help but wonder if there's a hidden section. Just as I once did many years ago.</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1; Choice "So, your family. They don't like you very much?", 5, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 50; Player-&gt;AddItem Gold_001, 50; set tlvoat_hasPCReceivedReward1; Choice "So, your family. They don't like you very much?", 5, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
+  </si>
+  <si>
+    <t>Good luck on your adventures too %PCClass. Thank you again for making my family's tomb safe for me.</t>
+  </si>
+  <si>
+    <t>Aryasi Othral paid me for making her family's tomb safe.</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 105; Goodbye</t>
+  </si>
+  <si>
+    <t>It started when I… better understood who I am. They really didn't like that and so pressured me to be who they wanted me to be. When that didn't work they turned to shame and mockery. Then it was denying what was promised to me as the firstborn, giving to my younger brothers Lletho and Jathys the family blade and armor. Eventually I took what I could and ran away. That was many years ago, and it was only recently that I received a letter from an old friend letting me know the fate of my family.</t>
+  </si>
+  <si>
+    <t>Honestly that sounds like a blessing from the Tribunal. No one to judge you, no one to control you. You're free from the burden of lingering pain of what could, should, have been.</t>
+  </si>
+  <si>
+    <t>if PC in Temple: Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21, "Just as Ghostfence is a monument to Dunmer pride in overcoming our enemies, so too should you in standing up for yourself against a family that should know better.", 22 ELSE Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21</t>
+  </si>
+  <si>
+    <t>Choice "What happened?", 10, "No one to love you. No happy memories.", 12, "That sounds like, despite the pain, you have some happy memories?", 13</t>
+  </si>
+  <si>
+    <t>Well, that's... true. I'm sorry %PCName, that was insensitive of me. [She's quiet for a minute.] My childhood happy memories are all of the times I was with grandmother. I loved how she could do so much with her magic. It's why I'm learning I suppose. It hurts all the more because I can't hear her. She's silent. Yet I can't help but drag up an old hope that she's actually in a hidden section of the tomb.</t>
+  </si>
+  <si>
+    <t>I do, and all of them are of my grandmother. I loved how she could do so much with her magic, how she could turn invisible or make someone like her more. Though she died before... I changed. I've often wondered whether she'd accept me, but this silence says not. Yet I can't help but drag up an old hope that she's actually in a hidden section of the tomb.</t>
+  </si>
+  <si>
+    <t>Choice = 22</t>
+  </si>
+  <si>
+    <t>Choice = 23</t>
+  </si>
+  <si>
+    <t>Choice = 24</t>
+  </si>
+  <si>
+    <t>Choice "You are not weak. After all, you came back here to face the spirits of your family,
+so that you can lay to rest your pain.", 23, "Correct, you're weak. Only because you've had to expend your strength in carrying the burdens your family placed upon your shoulders.
+From today you'll grow into the woman you're meant to be.", 24; set tlvoat_PCMentionInTemple to 1</t>
+  </si>
+  <si>
+    <t>ModDisposition 10</t>
+  </si>
+  <si>
+    <t>I hadn't thought about it like that. [A look of contemplation passes over her face, before easing into a lighter expression.] Thank you sera %PCName for being patient with me and hearing me out.</t>
+  </si>
+  <si>
+    <t>Thank you sera %PCName, I hope that's true. There's so much more that I want to do, but never felt like I could stick with it.</t>
   </si>
 </sst>
 </file>
@@ -1865,16 +1909,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1882,7 +1926,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -1891,7 +1935,7 @@
         <v>135</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1950,13 +1994,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1964,7 +2008,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -1973,7 +2017,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2100,10 +2144,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
-  <dimension ref="A2:F23"/>
+  <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2138,7 +2182,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2149,7 +2193,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -2169,7 +2213,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -2186,7 +2230,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -2206,7 +2250,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D7">
         <v>31</v>
@@ -2226,7 +2270,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2240,7 +2284,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2257,7 +2301,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -2271,7 +2315,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2288,7 +2332,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2302,13 +2346,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2319,7 +2363,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -2336,7 +2380,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D15">
         <v>101</v>
@@ -2345,21 +2389,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>343</v>
+        <v>385</v>
       </c>
       <c r="D16">
-        <v>150</v>
-      </c>
-      <c r="F16" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2370,19 +2411,16 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>168</v>
+        <v>340</v>
       </c>
       <c r="D17">
-        <v>200</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2390,19 +2428,19 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="D18">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2410,19 +2448,19 @@
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="D19">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>36</v>
+        <v>164</v>
       </c>
       <c r="F19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2430,10 +2468,13 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>232</v>
+        <v>170</v>
       </c>
       <c r="D20">
-        <v>500</v>
+        <v>400</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F20" t="s">
         <v>35</v>
@@ -2447,16 +2488,16 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>278</v>
+        <v>230</v>
       </c>
       <c r="D21">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="F21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2464,10 +2505,10 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D22">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="F22" t="s">
         <v>35</v>
@@ -2481,17 +2522,34 @@
         <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D23">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F23" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D24">
+        <v>701</v>
+      </c>
+      <c r="F24" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F4 B5:E39 F6:F8 F14 F16:F18 F20:F23">
+  <conditionalFormatting sqref="B3:F4 B5:E40 F6:F8 F14 F17:F19 F21:F24">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2783,10 +2841,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F99"/>
+  <dimension ref="A2:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2866,7 +2924,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F5" t="s">
         <v>140</v>
@@ -2883,7 +2941,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="F6" t="s">
         <v>141</v>
@@ -2900,7 +2958,7 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F7" t="s">
         <v>142</v>
@@ -2917,7 +2975,7 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F8" t="s">
         <v>143</v>
@@ -2934,7 +2992,7 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F9" t="s">
         <v>150</v>
@@ -2951,10 +3009,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2968,10 +3026,10 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2988,7 +3046,7 @@
         <v>138</v>
       </c>
       <c r="F12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -3019,13 +3077,13 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -3039,13 +3097,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3059,13 +3117,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F16" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3079,13 +3137,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F17" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3116,10 +3174,10 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F19" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3133,10 +3191,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3150,10 +3208,10 @@
         <v>110</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F21" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3167,10 +3225,10 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F22" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3184,10 +3242,10 @@
         <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F23" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3201,10 +3259,10 @@
         <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F24" t="s">
         <v>240</v>
-      </c>
-      <c r="F24" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -3218,13 +3276,13 @@
         <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3238,13 +3296,13 @@
         <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F26" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3258,13 +3316,13 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3278,13 +3336,13 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F28" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3298,10 +3356,10 @@
         <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3315,10 +3373,10 @@
         <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F30" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -3332,13 +3390,13 @@
         <v>110</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -3352,10 +3410,10 @@
         <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F32" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3369,10 +3427,10 @@
         <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F33" t="s">
         <v>144</v>
@@ -3389,10 +3447,10 @@
         <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F34" t="s">
         <v>146</v>
@@ -3429,7 +3487,7 @@
         <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>151</v>
@@ -3452,7 +3510,7 @@
         <v>155</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F37" t="s">
         <v>152</v>
@@ -3486,10 +3544,10 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F39" t="s">
         <v>153</v>
@@ -3506,10 +3564,10 @@
         <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F40" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3523,13 +3581,13 @@
         <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F41" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3543,13 +3601,13 @@
         <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F42" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3563,13 +3621,13 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F43" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3583,13 +3641,13 @@
         <v>103</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F44" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3603,13 +3661,13 @@
         <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F45" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3623,13 +3681,13 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="F46" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3643,10 +3701,10 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F47" t="s">
         <v>145</v>
@@ -3663,10 +3721,10 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F48" t="s">
         <v>150</v>
@@ -3683,13 +3741,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="F49" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3703,13 +3761,13 @@
         <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="F50" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3723,10 +3781,10 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F51" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3740,13 +3798,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="F52" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3760,13 +3818,13 @@
         <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="F53" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3780,13 +3838,13 @@
         <v>103</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F54" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3800,13 +3858,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F55" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3820,13 +3878,13 @@
         <v>103</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F56" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3840,13 +3898,13 @@
         <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F57" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3860,10 +3918,10 @@
         <v>103</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="F58" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -3877,12 +3935,12 @@
         <v>103</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60" t="s">
         <v>29</v>
@@ -3891,18 +3949,18 @@
         <v>160</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>162</v>
+        <v>257</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>163</v>
+        <v>378</v>
       </c>
       <c r="F60" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
         <v>29</v>
@@ -3911,15 +3969,18 @@
         <v>160</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>301</v>
+        <v>379</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>382</v>
       </c>
       <c r="F61" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B62" t="s">
         <v>29</v>
@@ -3928,15 +3989,18 @@
         <v>160</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>260</v>
+        <v>380</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="F62" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B63" t="s">
         <v>29</v>
@@ -3945,18 +4009,18 @@
         <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E63" t="s">
-        <v>261</v>
+        <v>381</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>355</v>
       </c>
       <c r="F63" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B64" t="s">
         <v>29</v>
@@ -3965,18 +4029,18 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>360</v>
+        <v>384</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>362</v>
+        <v>386</v>
       </c>
       <c r="F64" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B65" t="s">
         <v>29</v>
@@ -3985,18 +4049,18 @@
         <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>361</v>
+        <v>387</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>363</v>
+        <v>389</v>
       </c>
       <c r="F65" t="s">
-        <v>356</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B66" t="s">
         <v>29</v>
@@ -4005,18 +4069,18 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="E66" t="s">
-        <v>364</v>
+        <v>388</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>390</v>
       </c>
       <c r="F66" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B67" t="s">
         <v>29</v>
@@ -4025,18 +4089,15 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>359</v>
+        <v>391</v>
       </c>
       <c r="F67" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B68" t="s">
         <v>29</v>
@@ -4045,15 +4106,15 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>262</v>
+        <v>392</v>
       </c>
       <c r="F68" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B69" t="s">
         <v>29</v>
@@ -4062,15 +4123,15 @@
         <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>374</v>
+        <v>298</v>
       </c>
       <c r="F69" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B70" t="s">
         <v>29</v>
@@ -4079,15 +4140,15 @@
         <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>306</v>
+        <v>258</v>
       </c>
       <c r="F70" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
         <v>29</v>
@@ -4096,15 +4157,18 @@
         <v>160</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>396</v>
       </c>
       <c r="F71" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B72" t="s">
         <v>29</v>
@@ -4113,50 +4177,53 @@
         <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>375</v>
+        <v>398</v>
+      </c>
+      <c r="E72" t="s">
+        <v>397</v>
       </c>
       <c r="F72" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B73" t="s">
         <v>29</v>
       </c>
       <c r="C73" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E73" t="s">
+        <v>397</v>
+      </c>
+      <c r="F73" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" t="s">
+        <v>160</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F73" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" t="s">
-        <v>29</v>
-      </c>
-      <c r="C74" t="s">
-        <v>108</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="E74" s="2" t="s">
-        <v>268</v>
+        <v>377</v>
       </c>
       <c r="F74" t="s">
-        <v>146</v>
+        <v>256</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4167,19 +4234,16 @@
         <v>29</v>
       </c>
       <c r="C75" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>174</v>
+        <v>259</v>
       </c>
       <c r="F75" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4187,19 +4251,16 @@
         <v>29</v>
       </c>
       <c r="C76" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>174</v>
+        <v>364</v>
       </c>
       <c r="F76" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4207,16 +4268,13 @@
         <v>29</v>
       </c>
       <c r="C77" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>266</v>
+        <v>303</v>
       </c>
       <c r="F77" t="s">
-        <v>148</v>
+        <v>302</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4227,19 +4285,16 @@
         <v>29</v>
       </c>
       <c r="C78" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>197</v>
+        <v>304</v>
       </c>
       <c r="F78" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4247,16 +4302,16 @@
         <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>196</v>
+        <v>365</v>
       </c>
       <c r="F79" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4267,13 +4322,13 @@
         <v>108</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>279</v>
+        <v>168</v>
       </c>
       <c r="F80" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4287,13 +4342,13 @@
         <v>108</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>379</v>
+        <v>163</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="F81" t="s">
-        <v>186</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4307,16 +4362,16 @@
         <v>108</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>277</v>
+        <v>368</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>281</v>
+        <v>172</v>
       </c>
       <c r="F82" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4327,16 +4382,16 @@
         <v>108</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>367</v>
+        <v>167</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>265</v>
+        <v>172</v>
       </c>
       <c r="F83" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4347,16 +4402,16 @@
         <v>108</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F84" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4367,16 +4422,16 @@
         <v>108</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>271</v>
+        <v>316</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>270</v>
+        <v>195</v>
       </c>
       <c r="F85" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -4387,16 +4442,13 @@
         <v>108</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="F86" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4407,13 +4459,13 @@
         <v>108</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>195</v>
+        <v>369</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>318</v>
+        <v>276</v>
       </c>
       <c r="F87" t="s">
-        <v>242</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4427,13 +4479,16 @@
         <v>108</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>308</v>
+        <v>369</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="F88" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -4444,13 +4499,16 @@
         <v>108</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>315</v>
+        <v>274</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="F89" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4461,13 +4519,16 @@
         <v>108</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>316</v>
+        <v>357</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="F90" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4478,13 +4539,16 @@
         <v>108</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>282</v>
+        <v>261</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="F91" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -4492,19 +4556,19 @@
         <v>29</v>
       </c>
       <c r="C92" t="s">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>221</v>
+        <v>268</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="F92" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -4512,19 +4576,19 @@
         <v>29</v>
       </c>
       <c r="C93" t="s">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>353</v>
+        <v>273</v>
       </c>
       <c r="F93" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -4532,16 +4596,16 @@
         <v>29</v>
       </c>
       <c r="C94" t="s">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>342</v>
+        <v>193</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>353</v>
+        <v>315</v>
       </c>
       <c r="F94" t="s">
-        <v>340</v>
+        <v>240</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4552,19 +4616,16 @@
         <v>29</v>
       </c>
       <c r="C95" t="s">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>354</v>
+        <v>305</v>
       </c>
       <c r="F95" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -4572,19 +4633,16 @@
         <v>29</v>
       </c>
       <c r="C96" t="s">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>353</v>
+        <v>312</v>
       </c>
       <c r="F96" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -4592,16 +4650,13 @@
         <v>29</v>
       </c>
       <c r="C97" t="s">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>220</v>
+        <v>313</v>
       </c>
       <c r="F97" t="s">
-        <v>216</v>
+        <v>311</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -4612,34 +4667,171 @@
         <v>29</v>
       </c>
       <c r="C98" t="s">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>341</v>
+        <v>279</v>
       </c>
       <c r="F98" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B99" t="s">
+        <v>29</v>
+      </c>
+      <c r="C99" t="s">
+        <v>213</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F99" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>14</v>
+      </c>
+      <c r="B100" t="s">
+        <v>29</v>
+      </c>
+      <c r="C100" t="s">
+        <v>213</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="F100" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>14</v>
+      </c>
+      <c r="B101" t="s">
+        <v>29</v>
+      </c>
+      <c r="C101" t="s">
+        <v>213</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="F101" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>14</v>
+      </c>
+      <c r="B102" t="s">
+        <v>29</v>
+      </c>
+      <c r="C102" t="s">
+        <v>213</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F102" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>14</v>
-      </c>
-      <c r="B99" t="s">
-        <v>29</v>
-      </c>
-      <c r="C99" t="s">
-        <v>215</v>
-      </c>
-      <c r="D99" s="2" t="s">
+    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>14</v>
+      </c>
+      <c r="B103" t="s">
+        <v>29</v>
+      </c>
+      <c r="C103" t="s">
+        <v>213</v>
+      </c>
+      <c r="D103" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F99" t="s">
+      <c r="E103" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="F103" t="s">
         <v>287</v>
       </c>
     </row>
+    <row r="104" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>14</v>
+      </c>
+      <c r="B104" t="s">
+        <v>29</v>
+      </c>
+      <c r="C104" t="s">
+        <v>213</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F104" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>14</v>
+      </c>
+      <c r="B105" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" t="s">
+        <v>213</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F105" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>14</v>
+      </c>
+      <c r="B106" t="s">
+        <v>29</v>
+      </c>
+      <c r="C106" t="s">
+        <v>213</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F106" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F124">
+  <conditionalFormatting sqref="B3:F131">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -4943,13 +5135,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D9" t="s">
         <v>217</v>
-      </c>
-      <c r="C9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D9" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: expanded Aryasi's "speech" so that it doesn't feel as sudden
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00E5D16-A8EF-43A7-81D0-3D6D4E0F4638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2086C7EB-1F29-43B6-A183-4F37B38B7551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="402">
   <si>
     <t>Name</t>
   </si>
@@ -1192,12 +1192,6 @@
   </si>
   <si>
     <t>Well, while I can sense my family's spirits I can't work out who's who until they speak. I want to speak with my grandmother, but I don't know if she's here or in another part of the tomb. She should be in this room, and if she isn't then I can't help but wonder if there's a hidden section. Just as I once did many years ago.</t>
-  </si>
-  <si>
-    <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1; Choice "So, your family. They don't like you very much?", 5, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
-  </si>
-  <si>
-    <t>RemoveItem Gold_001, 50; Player-&gt;AddItem Gold_001, 50; set tlvoat_hasPCReceivedReward1; Choice "So, your family. They don't like you very much?", 5, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
   </si>
   <si>
     <t>Good luck on your adventures too %PCClass. Thank you again for making my family's tomb safe for me.</t>
@@ -1248,6 +1242,18 @@
   </si>
   <si>
     <t>Thank you sera %PCName, I hope that's true. There's so much more that I want to do, but never felt like I could stick with it.</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1; Choice "So, your family. They don't like you very much?", 1, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 50; Player-&gt;AddItem Gold_001, 50; set tlvoat_hasPCReceivedReward1; Choice "So, your family. They don't like you very much?", 1, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
+  </si>
+  <si>
+    <t>Same as before, they continue to keep me out.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.journal == 105</t>
   </si>
 </sst>
 </file>
@@ -2147,7 +2153,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2391,13 +2397,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D16">
         <v>105</v>
@@ -2841,10 +2847,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F106"/>
+  <dimension ref="A2:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3940,7 +3946,7 @@
     </row>
     <row r="60" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B60" t="s">
         <v>29</v>
@@ -3960,7 +3966,7 @@
     </row>
     <row r="61" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B61" t="s">
         <v>29</v>
@@ -3972,7 +3978,7 @@
         <v>379</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>382</v>
+        <v>398</v>
       </c>
       <c r="F61" t="s">
         <v>337</v>
@@ -3980,7 +3986,7 @@
     </row>
     <row r="62" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
         <v>29</v>
@@ -3992,7 +3998,7 @@
         <v>380</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>383</v>
+        <v>399</v>
       </c>
       <c r="F62" t="s">
         <v>146</v>
@@ -4000,7 +4006,7 @@
     </row>
     <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B63" t="s">
         <v>29</v>
@@ -4020,7 +4026,7 @@
     </row>
     <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
         <v>29</v>
@@ -4029,10 +4035,10 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>386</v>
       </c>
       <c r="F64" t="s">
         <v>148</v>
@@ -4040,7 +4046,7 @@
     </row>
     <row r="65" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B65" t="s">
         <v>29</v>
@@ -4049,10 +4055,10 @@
         <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>389</v>
       </c>
       <c r="F65" t="s">
         <v>187</v>
@@ -4060,7 +4066,7 @@
     </row>
     <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
         <v>29</v>
@@ -4069,10 +4075,10 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="F66" t="s">
         <v>319</v>
@@ -4080,7 +4086,7 @@
     </row>
     <row r="67" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
         <v>29</v>
@@ -4089,7 +4095,7 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F67" t="s">
         <v>320</v>
@@ -4097,7 +4103,7 @@
     </row>
     <row r="68" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B68" t="s">
         <v>29</v>
@@ -4106,7 +4112,7 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F68" t="s">
         <v>371</v>
@@ -4114,7 +4120,7 @@
     </row>
     <row r="69" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
         <v>29</v>
@@ -4131,7 +4137,7 @@
     </row>
     <row r="70" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B70" t="s">
         <v>29</v>
@@ -4148,7 +4154,7 @@
     </row>
     <row r="71" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
         <v>29</v>
@@ -4160,15 +4166,15 @@
         <v>299</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F71" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B72" t="s">
         <v>29</v>
@@ -4177,18 +4183,18 @@
         <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E72" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F72" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B73" t="s">
         <v>29</v>
@@ -4197,18 +4203,18 @@
         <v>160</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E73" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F73" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B74" t="s">
         <v>29</v>
@@ -4260,7 +4266,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4271,10 +4277,10 @@
         <v>160</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>303</v>
+        <v>400</v>
       </c>
       <c r="F77" t="s">
-        <v>302</v>
+        <v>401</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4288,10 +4294,10 @@
         <v>160</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F78" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4305,33 +4311,30 @@
         <v>160</v>
       </c>
       <c r="D79" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F79" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F80" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>14</v>
-      </c>
-      <c r="B80" t="s">
-        <v>29</v>
-      </c>
-      <c r="C80" t="s">
-        <v>108</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F80" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4342,13 +4345,13 @@
         <v>108</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>163</v>
+        <v>366</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>265</v>
+        <v>168</v>
       </c>
       <c r="F81" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4362,16 +4365,16 @@
         <v>108</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>368</v>
+        <v>163</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>172</v>
+        <v>265</v>
       </c>
       <c r="F82" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4382,13 +4385,13 @@
         <v>108</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>167</v>
+        <v>368</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>172</v>
       </c>
       <c r="F83" t="s">
-        <v>147</v>
+        <v>367</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4402,16 +4405,16 @@
         <v>108</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>270</v>
+        <v>167</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>263</v>
+        <v>172</v>
       </c>
       <c r="F84" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4422,16 +4425,16 @@
         <v>108</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>316</v>
+        <v>270</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="F85" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -4442,13 +4445,16 @@
         <v>108</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>194</v>
+        <v>316</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="F86" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4459,13 +4465,10 @@
         <v>108</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="F87" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4482,10 +4485,10 @@
         <v>369</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F88" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4499,16 +4502,16 @@
         <v>108</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>274</v>
+        <v>369</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F89" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4519,13 +4522,13 @@
         <v>108</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>357</v>
+        <v>274</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="F90" t="s">
-        <v>356</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -4539,13 +4542,13 @@
         <v>108</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>261</v>
+        <v>357</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>262</v>
       </c>
       <c r="F91" t="s">
-        <v>169</v>
+        <v>356</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -4559,16 +4562,16 @@
         <v>108</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F92" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -4579,16 +4582,16 @@
         <v>108</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F93" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -4599,16 +4602,16 @@
         <v>108</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>193</v>
+        <v>269</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>315</v>
+        <v>273</v>
       </c>
       <c r="F94" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -4619,13 +4622,16 @@
         <v>108</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>305</v>
+        <v>193</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>315</v>
       </c>
       <c r="F95" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -4636,13 +4642,13 @@
         <v>108</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="F96" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -4653,13 +4659,13 @@
         <v>108</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F97" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -4670,33 +4676,30 @@
         <v>108</v>
       </c>
       <c r="D98" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F98" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B99" t="s">
+        <v>29</v>
+      </c>
+      <c r="C99" t="s">
+        <v>108</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F99" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>14</v>
-      </c>
-      <c r="B99" t="s">
-        <v>29</v>
-      </c>
-      <c r="C99" t="s">
-        <v>213</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F99" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -4707,13 +4710,13 @@
         <v>213</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>350</v>
+        <v>282</v>
       </c>
       <c r="F100" t="s">
-        <v>220</v>
+        <v>144</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4727,13 +4730,13 @@
         <v>213</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>339</v>
+        <v>221</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>350</v>
       </c>
       <c r="F101" t="s">
-        <v>337</v>
+        <v>220</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4747,13 +4750,13 @@
         <v>213</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>289</v>
+        <v>339</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F102" t="s">
-        <v>286</v>
+        <v>337</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4767,16 +4770,16 @@
         <v>213</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F103" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>14</v>
       </c>
@@ -4787,16 +4790,16 @@
         <v>213</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>218</v>
+        <v>350</v>
       </c>
       <c r="F104" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>14</v>
       </c>
@@ -4807,13 +4810,16 @@
         <v>213</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>338</v>
+        <v>281</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="F105" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>14</v>
       </c>
@@ -4824,14 +4830,31 @@
         <v>213</v>
       </c>
       <c r="D106" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F106" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" t="s">
+        <v>29</v>
+      </c>
+      <c r="C107" t="s">
+        <v>213</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F107" t="s">
         <v>284</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F131">
+  <conditionalFormatting sqref="B3:F132">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated: added fail for disturbing remains when PC does it in front of Aryasi
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2086C7EB-1F29-43B6-A183-4F37B38B7551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE59A2B9-1E1D-452B-9B69-5B49A1D61F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="408">
   <si>
     <t>Name</t>
   </si>
@@ -655,9 +655,6 @@
   </si>
   <si>
     <t>Journal "tlvoat_Estranged_Spirits", 31, ModDisposition 5, StartScript tlvoat_othral_quest_glb_script, Goodbye</t>
-  </si>
-  <si>
-    <t>tlvoat_estranged_spirits.Journal == 70</t>
   </si>
   <si>
     <t>I should speak with Aryasi now that she's had time to speak to her grandmother's spirit.</t>
@@ -1254,6 +1251,27 @@
   </si>
   <si>
     <t>tlvoat_Estranged_Spirits.journal == 105</t>
+  </si>
+  <si>
+    <t>tlvoat_Estarnged_Spirits.Journal &gt;= 30, tlvoat_Estarnged_Spirits.Journal &lt;= 45, tlvoat_Othral_Disturb1_State == 1</t>
+  </si>
+  <si>
+    <t>What are you DOING? Just because my family has pushed me away does NOT mean that I'm fine with having their remains disturbed. I need you to leave. NOW!</t>
+  </si>
+  <si>
+    <t>ModDisposition -100, Journal "tlvoat_Estranged_Spirits", 150; StopScript "tlvoat_othral_quest_glb_script"; Goodbye</t>
+  </si>
+  <si>
+    <t>Why would you do that? What is wrong with you? You need to leave.</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal == 60, tlvoat_Othral_Disturb2_State == 1</t>
+  </si>
+  <si>
+    <t>tlvoat_estranged_spirits.Journal &gt; 70</t>
+  </si>
+  <si>
+    <t>Did you lead me here just to make me watch as you disturbed my grandmother's remains? You are a sick and cruel person %PCName. Leave this place.</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1887,7 @@
   <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2014,7 +2032,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -2023,7 +2041,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2236,7 +2254,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -2256,7 +2274,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7">
         <v>31</v>
@@ -2276,7 +2294,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2290,7 +2308,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2307,7 +2325,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -2321,7 +2339,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2338,7 +2356,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2352,13 +2370,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2369,7 +2387,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -2403,7 +2421,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D16">
         <v>105</v>
@@ -2417,7 +2435,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D17">
         <v>150</v>
@@ -2494,7 +2512,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D21">
         <v>500</v>
@@ -2511,7 +2529,7 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D22">
         <v>600</v>
@@ -2528,7 +2546,7 @@
         <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D23">
         <v>700</v>
@@ -2545,7 +2563,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D24">
         <v>701</v>
@@ -2847,10 +2865,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F107"/>
+  <dimension ref="A2:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2930,7 +2948,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F5" t="s">
         <v>140</v>
@@ -2947,7 +2965,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F6" t="s">
         <v>141</v>
@@ -2964,7 +2982,7 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F7" t="s">
         <v>142</v>
@@ -2981,7 +2999,7 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F8" t="s">
         <v>143</v>
@@ -2998,7 +3016,7 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F9" t="s">
         <v>150</v>
@@ -3015,10 +3033,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3032,10 +3050,10 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F11" t="s">
         <v>231</v>
-      </c>
-      <c r="F11" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3083,13 +3101,13 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -3103,13 +3121,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3123,13 +3141,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3143,13 +3161,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F17" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3163,13 +3181,16 @@
         <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>161</v>
+        <v>402</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="F18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -3180,13 +3201,13 @@
         <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>307</v>
+        <v>161</v>
       </c>
       <c r="F19" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -3197,10 +3218,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>237</v>
+        <v>306</v>
       </c>
       <c r="F20" t="s">
-        <v>236</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3214,10 +3235,10 @@
         <v>110</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>173</v>
+        <v>236</v>
       </c>
       <c r="F21" t="s">
-        <v>291</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3231,13 +3252,13 @@
         <v>110</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>318</v>
+        <v>173</v>
       </c>
       <c r="F22" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -3248,13 +3269,13 @@
         <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>174</v>
+        <v>317</v>
       </c>
       <c r="F23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -3265,13 +3286,13 @@
         <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>238</v>
+        <v>174</v>
       </c>
       <c r="F24" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -3282,16 +3303,13 @@
         <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F25" t="s">
         <v>239</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -3302,16 +3320,16 @@
         <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>360</v>
+        <v>238</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>352</v>
+        <v>113</v>
       </c>
       <c r="F26" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -3322,16 +3340,16 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>241</v>
+        <v>407</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>113</v>
+        <v>403</v>
       </c>
       <c r="F27" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -3342,16 +3360,16 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F28" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3362,13 +3380,16 @@
         <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="F29" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -3379,13 +3400,16 @@
         <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>314</v>
+        <v>347</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="F30" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -3396,16 +3420,13 @@
         <v>110</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F31" t="s">
         <v>346</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F31" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -3416,73 +3437,70 @@
         <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="F32" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F33" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F35" t="s">
         <v>243</v>
       </c>
-      <c r="F32" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="F33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="F34" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F35" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -3493,16 +3511,16 @@
         <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>183</v>
+        <v>245</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>151</v>
+        <v>328</v>
       </c>
       <c r="F36" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3513,16 +3531,16 @@
         <v>103</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>190</v>
+        <v>329</v>
       </c>
       <c r="F37" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -3533,13 +3551,16 @@
         <v>103</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="F38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3550,16 +3571,16 @@
         <v>103</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>253</v>
+        <v>183</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="F39" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -3570,13 +3591,16 @@
         <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>188</v>
+        <v>155</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="F40" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3587,13 +3611,10 @@
         <v>103</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>201</v>
+        <v>156</v>
       </c>
       <c r="F41" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3607,16 +3628,16 @@
         <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>186</v>
+        <v>252</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="F42" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -3627,16 +3648,13 @@
         <v>103</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>325</v>
+        <v>188</v>
       </c>
       <c r="F43" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -3647,16 +3665,16 @@
         <v>103</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>324</v>
+        <v>186</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>331</v>
+        <v>201</v>
       </c>
       <c r="F44" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -3667,13 +3685,13 @@
         <v>103</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>362</v>
+        <v>186</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>332</v>
+        <v>202</v>
       </c>
       <c r="F45" t="s">
-        <v>320</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3687,16 +3705,16 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>372</v>
+        <v>324</v>
       </c>
       <c r="F46" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -3707,16 +3725,16 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>245</v>
+        <v>323</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="F47" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -3727,16 +3745,16 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>322</v>
+        <v>361</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="F48" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -3747,16 +3765,16 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>251</v>
+        <v>372</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F49" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3767,16 +3785,16 @@
         <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>375</v>
+        <v>322</v>
       </c>
       <c r="F50" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -3787,10 +3805,13 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>247</v>
+        <v>321</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="F51" t="s">
-        <v>248</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3804,13 +3825,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F52" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3824,16 +3845,16 @@
         <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>374</v>
       </c>
       <c r="F53" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -3844,13 +3865,10 @@
         <v>103</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>327</v>
+        <v>246</v>
       </c>
       <c r="F54" t="s">
-        <v>334</v>
+        <v>247</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3864,13 +3882,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>326</v>
+        <v>248</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
       <c r="F55" t="s">
-        <v>328</v>
+        <v>294</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3884,13 +3902,13 @@
         <v>103</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>336</v>
+        <v>249</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>297</v>
+        <v>373</v>
       </c>
       <c r="F56" t="s">
-        <v>335</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3904,16 +3922,16 @@
         <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>255</v>
+        <v>332</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>297</v>
+        <v>326</v>
       </c>
       <c r="F57" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3924,13 +3942,16 @@
         <v>103</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>363</v>
+        <v>325</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="F58" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -3941,10 +3962,16 @@
         <v>103</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F59" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3952,19 +3979,19 @@
         <v>29</v>
       </c>
       <c r="C60" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>378</v>
+        <v>296</v>
       </c>
       <c r="F60" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -3972,19 +3999,16 @@
         <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>398</v>
+        <v>362</v>
       </c>
       <c r="F61" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3992,19 +4016,13 @@
         <v>29</v>
       </c>
       <c r="C62" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="F62" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -4015,16 +4033,16 @@
         <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>381</v>
+        <v>256</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>355</v>
+        <v>377</v>
       </c>
       <c r="F63" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -4035,16 +4053,16 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="F64" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -4055,13 +4073,13 @@
         <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="F65" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -4075,16 +4093,16 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>388</v>
+        <v>354</v>
       </c>
       <c r="F66" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -4095,13 +4113,16 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>389</v>
+        <v>381</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="F67" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -4112,13 +4133,16 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>390</v>
+        <v>384</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>386</v>
       </c>
       <c r="F68" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -4129,13 +4153,16 @@
         <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>298</v>
+        <v>385</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>387</v>
       </c>
       <c r="F69" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -4146,13 +4173,13 @@
         <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>258</v>
+        <v>388</v>
       </c>
       <c r="F70" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -4163,16 +4190,13 @@
         <v>160</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F71" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4183,16 +4207,13 @@
         <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E72" t="s">
-        <v>395</v>
+        <v>297</v>
       </c>
       <c r="F72" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -4203,16 +4224,13 @@
         <v>160</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="E73" t="s">
-        <v>395</v>
+        <v>257</v>
       </c>
       <c r="F73" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4223,16 +4241,16 @@
         <v>160</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>376</v>
+        <v>298</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>377</v>
+        <v>393</v>
       </c>
       <c r="F74" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4243,13 +4261,16 @@
         <v>160</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>259</v>
+        <v>395</v>
+      </c>
+      <c r="E75" t="s">
+        <v>394</v>
       </c>
       <c r="F75" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4260,13 +4281,16 @@
         <v>160</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>364</v>
+        <v>396</v>
+      </c>
+      <c r="E76" t="s">
+        <v>394</v>
       </c>
       <c r="F76" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4277,10 +4301,13 @@
         <v>160</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>400</v>
+        <v>375</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="F77" t="s">
-        <v>401</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4294,13 +4321,13 @@
         <v>160</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="F78" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4311,13 +4338,13 @@
         <v>160</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>304</v>
+        <v>363</v>
       </c>
       <c r="F79" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4328,13 +4355,13 @@
         <v>160</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>365</v>
+        <v>399</v>
       </c>
       <c r="F80" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4342,16 +4369,13 @@
         <v>29</v>
       </c>
       <c r="C81" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>168</v>
+        <v>302</v>
       </c>
       <c r="F81" t="s">
-        <v>144</v>
+        <v>301</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4362,16 +4386,13 @@
         <v>29</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>265</v>
+        <v>303</v>
       </c>
       <c r="F82" t="s">
-        <v>146</v>
+        <v>300</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4382,19 +4403,16 @@
         <v>29</v>
       </c>
       <c r="C83" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>172</v>
+        <v>364</v>
       </c>
       <c r="F83" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4405,16 +4423,16 @@
         <v>108</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>167</v>
+        <v>365</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F84" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4425,13 +4443,13 @@
         <v>108</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>270</v>
+        <v>163</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F85" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4445,16 +4463,16 @@
         <v>108</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>316</v>
+        <v>367</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="F86" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4465,13 +4483,16 @@
         <v>108</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>194</v>
+        <v>167</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="F87" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -4482,13 +4503,13 @@
         <v>108</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>369</v>
+        <v>269</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="F88" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4502,16 +4523,16 @@
         <v>108</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>369</v>
+        <v>315</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
       <c r="F89" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4522,16 +4543,13 @@
         <v>108</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>278</v>
+        <v>194</v>
       </c>
       <c r="F90" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4542,16 +4560,16 @@
         <v>108</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="F91" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -4562,16 +4580,16 @@
         <v>108</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>261</v>
+        <v>368</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="F92" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -4582,16 +4600,16 @@
         <v>108</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="F93" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -4602,16 +4620,16 @@
         <v>108</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>269</v>
+        <v>356</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="F94" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -4622,16 +4640,16 @@
         <v>108</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>193</v>
+        <v>260</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>315</v>
+        <v>261</v>
       </c>
       <c r="F95" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -4642,13 +4660,16 @@
         <v>108</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>305</v>
+        <v>267</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>266</v>
       </c>
       <c r="F96" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -4659,13 +4680,16 @@
         <v>108</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>312</v>
+        <v>268</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="F97" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -4676,13 +4700,16 @@
         <v>108</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>313</v>
+        <v>193</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>314</v>
       </c>
       <c r="F98" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -4693,13 +4720,13 @@
         <v>108</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
       <c r="F99" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -4707,16 +4734,13 @@
         <v>29</v>
       </c>
       <c r="C100" t="s">
-        <v>213</v>
+        <v>108</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>282</v>
+        <v>311</v>
       </c>
       <c r="F100" t="s">
-        <v>144</v>
+        <v>309</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4727,19 +4751,16 @@
         <v>29</v>
       </c>
       <c r="C101" t="s">
-        <v>213</v>
+        <v>108</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="F101" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>14</v>
       </c>
@@ -4747,19 +4768,16 @@
         <v>29</v>
       </c>
       <c r="C102" t="s">
-        <v>213</v>
+        <v>108</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>350</v>
+        <v>278</v>
       </c>
       <c r="F102" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>14</v>
       </c>
@@ -4767,16 +4785,16 @@
         <v>29</v>
       </c>
       <c r="C103" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>289</v>
+        <v>218</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>351</v>
+        <v>281</v>
       </c>
       <c r="F103" t="s">
-        <v>286</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4787,74 +4805,134 @@
         <v>29</v>
       </c>
       <c r="C104" t="s">
+        <v>212</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F104" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>14</v>
+      </c>
+      <c r="B105" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F105" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>14</v>
+      </c>
+      <c r="B106" t="s">
+        <v>29</v>
+      </c>
+      <c r="C106" t="s">
+        <v>212</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="F106" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" t="s">
+        <v>29</v>
+      </c>
+      <c r="C107" t="s">
+        <v>212</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F107" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>14</v>
+      </c>
+      <c r="B108" t="s">
+        <v>29</v>
+      </c>
+      <c r="C108" t="s">
+        <v>212</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F108" t="s">
         <v>213</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F104" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>14</v>
-      </c>
-      <c r="B105" t="s">
-        <v>29</v>
-      </c>
-      <c r="C105" t="s">
-        <v>213</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F105" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>14</v>
-      </c>
-      <c r="B106" t="s">
-        <v>29</v>
-      </c>
-      <c r="C106" t="s">
-        <v>213</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="F106" t="s">
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>14</v>
+      </c>
+      <c r="B109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C109" t="s">
+        <v>212</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F109" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110" t="s">
+        <v>29</v>
+      </c>
+      <c r="C110" t="s">
+        <v>212</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F110" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>14</v>
-      </c>
-      <c r="B107" t="s">
-        <v>29</v>
-      </c>
-      <c r="C107" t="s">
-        <v>213</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="F107" t="s">
-        <v>284</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F132">
+  <conditionalFormatting sqref="B3:F135">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -5158,13 +5236,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" t="s">
         <v>215</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>216</v>
-      </c>
-      <c r="D9" t="s">
-        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: alt good ends
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE59A2B9-1E1D-452B-9B69-5B49A1D61F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F366F1DF-D092-4899-A68C-AD69834F01C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="2" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="422">
   <si>
     <t>Name</t>
   </si>
@@ -642,9 +642,6 @@
     <t>I have met a woman named Aryasi Othral who wants to enter her family's tomb, but cant't as it's unsafe even for her as the tomb's guardians will kill her. She wants me to clear the tomb so that it's safe for her.</t>
   </si>
   <si>
-    <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. I turned down her reward.</t>
-  </si>
-  <si>
     <t>tlvoat_othral_quest_glb_script</t>
   </si>
   <si>
@@ -711,9 +708,6 @@
     <t>My apologies sera %PCName, I forgot that priests do not usually accept gifts and rewards for acts of service. Well, I hope that we can meet again someday.</t>
   </si>
   <si>
-    <t>Aryasi Othral is grateful that I've lead her to her grandmother's spirit and that because of this she's had an opportunity to reconnect. She gave me a ring that was her grandmother's.</t>
-  </si>
-  <si>
     <t>tlvoat_urn_uravasa_uni_script</t>
   </si>
   <si>
@@ -888,9 +882,6 @@
     <t>tlvoat_Estranged_Spirits.Journal &gt;= 50</t>
   </si>
   <si>
-    <t>It was one of the things that I took when I ran away. Something to remember her by. I thought my grandmother would be angry when I spoke to her, but it turns out she always wanted me to have it. Another thing my parents denied to me.</t>
-  </si>
-  <si>
     <t>RemoveItem "tlvoat_ring_matriarch_unique", 1; Player-&gt;AddItem "tlvoat_ring_matriarch_unique", 1; Journal "tlvoat_Estranged_Spirits", 100</t>
   </si>
   <si>
@@ -1206,16 +1197,10 @@
     <t>Honestly that sounds like a blessing from the Tribunal. No one to judge you, no one to control you. You're free from the burden of lingering pain of what could, should, have been.</t>
   </si>
   <si>
-    <t>if PC in Temple: Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21, "Just as Ghostfence is a monument to Dunmer pride in overcoming our enemies, so too should you in standing up for yourself against a family that should know better.", 22 ELSE Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21</t>
-  </si>
-  <si>
     <t>Choice "What happened?", 10, "No one to love you. No happy memories.", 12, "That sounds like, despite the pain, you have some happy memories?", 13</t>
   </si>
   <si>
     <t>Well, that's... true. I'm sorry %PCName, that was insensitive of me. [She's quiet for a minute.] My childhood happy memories are all of the times I was with grandmother. I loved how she could do so much with her magic. It's why I'm learning I suppose. It hurts all the more because I can't hear her. She's silent. Yet I can't help but drag up an old hope that she's actually in a hidden section of the tomb.</t>
-  </si>
-  <si>
-    <t>I do, and all of them are of my grandmother. I loved how she could do so much with her magic, how she could turn invisible or make someone like her more. Though she died before... I changed. I've often wondered whether she'd accept me, but this silence says not. Yet I can't help but drag up an old hope that she's actually in a hidden section of the tomb.</t>
   </si>
   <si>
     <t>Choice = 22</t>
@@ -1238,9 +1223,6 @@
     <t>I hadn't thought about it like that. [A look of contemplation passes over her face, before easing into a lighter expression.] Thank you sera %PCName for being patient with me and hearing me out.</t>
   </si>
   <si>
-    <t>Thank you sera %PCName, I hope that's true. There's so much more that I want to do, but never felt like I could stick with it.</t>
-  </si>
-  <si>
     <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1; Choice "So, your family. They don't like you very much?", 1, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
   </si>
   <si>
@@ -1272,6 +1254,66 @@
   </si>
   <si>
     <t>Did you lead me here just to make me watch as you disturbed my grandmother's remains? You are a sick and cruel person %PCName. Leave this place.</t>
+  </si>
+  <si>
+    <t>if PC in Temple: Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21, "Just as Ghostfence is a monument to Dunmer pride in overcoming our enemies, so too should you in staying true to yourself and doing what you must.", 22 ELSE Choice "I'm sorry to hear that your family pushed you away.", 20, "Was there anyone in your family who you had a good relationship with?", 21</t>
+  </si>
+  <si>
+    <t>Yes, and almost all of them are of my grandmother. I loved how she could do so much with her magic, how she could turn invisible or make someone like her with a flick of her hand. Though she died just before I... changed. I've often wondered whether she'd accept and be proud of me? I don't think so, not with how I've ran away from everything, and yet I can't help but drag up an old hope that she's actually in a hidden section of the tomb. If that exists, should I even attempt to speak with her?</t>
+  </si>
+  <si>
+    <t>Choice "Make a promise to yourself to live your life to make her proud. Then return when you're ready.", 30, "Do it, or regret not doing it.", 31</t>
+  </si>
+  <si>
+    <t>Thank you sera %PCName, I hope that's true. There's so much more that I want to do, but never felt like I could stick with it. Because right now, I'm a bit of a failure. Even if my family's spirits spoke to me they'd be disappointed that I haven't dedicated myself to anything. When the going gets tough I move to a new town, or guild, or job. Not staying long enough to even leave behind any friends or lovers. I want to speak to grandmother, but I'm scared of what she'd think of me. Of what she'd say.</t>
+  </si>
+  <si>
+    <t>Choice = 30</t>
+  </si>
+  <si>
+    <t>Choice = 31</t>
+  </si>
+  <si>
+    <t>Then, %PCName, bear witness to this promise that I, Aryasi Othral, will make something of my life. To make settle in one place, make friends, and return here with happiness in my heart. So that I can make grandmother proud of me! I will try the Mages Guild and work from there I think. Hey, %PCName, I want to thank you. All I have left is my grandmother's ring, and I want you to have it.</t>
+  </si>
+  <si>
+    <t>You're right %PCName. I need to not continue my life with regrets. If it's that she isn't here, then let's begin with the shrine as I remember once watching my mother do something to it, but I could never find anything. Your fresh eyes and hands might reveal something.</t>
+  </si>
+  <si>
+    <t>Journal "tlvoat_Estranged_Spirits", 40</t>
+  </si>
+  <si>
+    <t>After speaking with Aryasi she is going to live her life in a way to make her grandmother's spirit proud.</t>
+  </si>
+  <si>
+    <t>Aryasi Othral is grateful for my help. She gave me a ring that was her grandmother's.</t>
+  </si>
+  <si>
+    <t>set tlvoat_isEarlyFinish to 1; Journal "tlvoat_Estranged_Spirits", 71</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.journal &gt;= 70, tlvoat_isEarlyFinish == 1</t>
+  </si>
+  <si>
+    <t>Don't worry, %PCName. I'm going to keep my promise to make my grandmother proud.</t>
+  </si>
+  <si>
+    <t>Maybe one day I'll see if it exists, but for now I have a life to live.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 71</t>
+  </si>
+  <si>
+    <t>It was one of the things that I took when I ran away just to have something to remember her by. I don't think I need it anymore, and I think you'll be able to put it to better use.</t>
+  </si>
+  <si>
+    <t>It was one of the things that I took when I ran away just to have something to remember her by. I thought my grandmother would be angry when I spoke to her, but it turns out she always wanted me to have it. Another thing my parents denied to me.</t>
+  </si>
+  <si>
+    <t>ModDisposition 10; Choice "You don't have to reach out to her now. Go out into the world with the promise that'll you'll make her proud held deep within your heart. Then return when you're ready.", 30, "The unknown meeting is always the scariest, because we cannot anticipate it's contents. You mentioned their might be a hidden section? Then let's find it so that you can make the unknown known.", 31</t>
+  </si>
+  <si>
+    <t>Aryasi Othral is grateful for my help. I turned down her reward.</t>
   </si>
 </sst>
 </file>
@@ -2018,13 +2060,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -2032,7 +2074,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -2041,7 +2083,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2168,10 +2210,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
-  <dimension ref="A2:F24"/>
+  <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2254,7 +2296,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -2274,7 +2316,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D7">
         <v>31</v>
@@ -2294,7 +2336,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2308,7 +2350,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -2325,7 +2367,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D10">
         <v>45</v>
@@ -2339,7 +2381,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -2356,7 +2398,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2370,16 +2412,16 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2387,13 +2429,10 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>221</v>
+        <v>411</v>
       </c>
       <c r="D14">
-        <v>100</v>
-      </c>
-      <c r="F14" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2404,10 +2443,10 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>198</v>
+        <v>412</v>
       </c>
       <c r="D15">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" t="s">
         <v>35</v>
@@ -2421,13 +2460,16 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>382</v>
+        <v>421</v>
       </c>
       <c r="D16">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2435,13 +2477,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>339</v>
+        <v>379</v>
       </c>
       <c r="D17">
-        <v>150</v>
-      </c>
-      <c r="F17" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2452,19 +2491,16 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="D18">
-        <v>200</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="F18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2472,19 +2508,19 @@
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="D19">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2492,19 +2528,19 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="D20">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>36</v>
+        <v>164</v>
       </c>
       <c r="F20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -2512,10 +2548,13 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>229</v>
+        <v>170</v>
       </c>
       <c r="D21">
-        <v>500</v>
+        <v>400</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F21" t="s">
         <v>35</v>
@@ -2529,16 +2568,16 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>274</v>
+        <v>227</v>
       </c>
       <c r="D22">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="F22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -2546,10 +2585,10 @@
         <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D23">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="F23" t="s">
         <v>35</v>
@@ -2563,17 +2602,34 @@
         <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D24">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F24" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D25">
+        <v>701</v>
+      </c>
+      <c r="F25" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F4 B5:E40 F6:F8 F14 F17:F19 F21:F24">
+  <conditionalFormatting sqref="B3:F4 F6:F8 F15 F18:F20 F22:F25 B5:E41">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2865,10 +2921,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F110"/>
+  <dimension ref="A2:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2948,7 +3004,7 @@
         <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F5" t="s">
         <v>140</v>
@@ -2965,7 +3021,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F6" t="s">
         <v>141</v>
@@ -2982,7 +3038,7 @@
         <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F7" t="s">
         <v>142</v>
@@ -2999,7 +3055,7 @@
         <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F8" t="s">
         <v>143</v>
@@ -3016,7 +3072,7 @@
         <v>110</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F9" t="s">
         <v>150</v>
@@ -3033,10 +3089,10 @@
         <v>110</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3050,10 +3106,10 @@
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3101,13 +3157,13 @@
         <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -3121,13 +3177,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3141,13 +3197,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F16" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3161,13 +3217,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F17" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3181,13 +3237,13 @@
         <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F18" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3218,10 +3274,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F20" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3235,10 +3291,10 @@
         <v>110</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3255,7 +3311,7 @@
         <v>173</v>
       </c>
       <c r="F22" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3269,10 +3325,10 @@
         <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F23" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3289,7 +3345,7 @@
         <v>174</v>
       </c>
       <c r="F24" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3303,10 +3359,10 @@
         <v>110</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F25" t="s">
         <v>237</v>
-      </c>
-      <c r="F25" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3320,7 +3376,7 @@
         <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>113</v>
@@ -3340,13 +3396,13 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="F27" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3360,13 +3416,13 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3380,13 +3436,13 @@
         <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3400,13 +3456,13 @@
         <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F30" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3420,10 +3476,10 @@
         <v>110</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F31" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3437,13 +3493,13 @@
         <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F32" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3457,10 +3513,10 @@
         <v>110</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F33" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3474,13 +3530,13 @@
         <v>110</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F34" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -3494,10 +3550,10 @@
         <v>110</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F35" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3511,10 +3567,10 @@
         <v>103</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F36" t="s">
         <v>144</v>
@@ -3534,7 +3590,7 @@
         <v>182</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F37" t="s">
         <v>146</v>
@@ -3628,7 +3684,7 @@
         <v>103</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>189</v>
@@ -3668,7 +3724,7 @@
         <v>186</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F44" t="s">
         <v>185</v>
@@ -3688,7 +3744,7 @@
         <v>186</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F45" t="s">
         <v>187</v>
@@ -3705,13 +3761,13 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F46" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3725,13 +3781,13 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F47" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3745,13 +3801,13 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F48" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3765,13 +3821,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F49" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3785,10 +3841,10 @@
         <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F50" t="s">
         <v>145</v>
@@ -3805,10 +3861,10 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F51" t="s">
         <v>150</v>
@@ -3825,13 +3881,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F52" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3845,13 +3901,13 @@
         <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F53" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3865,10 +3921,10 @@
         <v>103</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F54" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3882,13 +3938,13 @@
         <v>103</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F55" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3902,13 +3958,13 @@
         <v>103</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F56" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3922,13 +3978,13 @@
         <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F57" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3942,13 +3998,13 @@
         <v>103</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F58" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3962,13 +4018,13 @@
         <v>103</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F59" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3982,13 +4038,13 @@
         <v>103</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F60" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4002,7 +4058,7 @@
         <v>103</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F61" t="s">
         <v>191</v>
@@ -4019,7 +4075,7 @@
         <v>103</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -4033,10 +4089,10 @@
         <v>160</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F63" t="s">
         <v>144</v>
@@ -4053,13 +4109,13 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="F64" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4073,10 +4129,10 @@
         <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="F65" t="s">
         <v>146</v>
@@ -4093,10 +4149,10 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F66" t="s">
         <v>147</v>
@@ -4113,10 +4169,10 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F67" t="s">
         <v>148</v>
@@ -4133,10 +4189,10 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>386</v>
+        <v>402</v>
       </c>
       <c r="F68" t="s">
         <v>187</v>
@@ -4153,13 +4209,13 @@
         <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F69" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -4173,13 +4229,13 @@
         <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F70" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
@@ -4190,10 +4246,13 @@
         <v>160</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>389</v>
+        <v>403</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="F71" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -4207,10 +4266,10 @@
         <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F72" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -4224,10 +4283,10 @@
         <v>160</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F73" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
@@ -4241,13 +4300,13 @@
         <v>160</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F74" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4261,16 +4320,16 @@
         <v>160</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E75" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F75" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4281,16 +4340,16 @@
         <v>160</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E76" t="s">
-        <v>394</v>
+        <v>405</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>420</v>
       </c>
       <c r="F76" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4301,16 +4360,16 @@
         <v>160</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>375</v>
+        <v>408</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>376</v>
+        <v>413</v>
       </c>
       <c r="F77" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -4321,13 +4380,16 @@
         <v>160</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>258</v>
+        <v>409</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>410</v>
       </c>
       <c r="F78" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4338,13 +4400,16 @@
         <v>160</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>363</v>
+        <v>372</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="F79" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4355,13 +4420,13 @@
         <v>160</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>399</v>
+        <v>256</v>
       </c>
       <c r="F80" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4372,13 +4437,13 @@
         <v>160</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>302</v>
+        <v>360</v>
       </c>
       <c r="F81" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4389,10 +4454,10 @@
         <v>160</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>303</v>
+        <v>393</v>
       </c>
       <c r="F82" t="s">
-        <v>300</v>
+        <v>394</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4406,13 +4471,13 @@
         <v>160</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>364</v>
+        <v>299</v>
       </c>
       <c r="F83" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4420,16 +4485,13 @@
         <v>29</v>
       </c>
       <c r="C84" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>168</v>
+        <v>300</v>
       </c>
       <c r="F84" t="s">
-        <v>144</v>
+        <v>297</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4440,16 +4502,13 @@
         <v>29</v>
       </c>
       <c r="C85" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>264</v>
+        <v>415</v>
       </c>
       <c r="F85" t="s">
-        <v>146</v>
+        <v>414</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4460,19 +4519,16 @@
         <v>29</v>
       </c>
       <c r="C86" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>172</v>
+        <v>361</v>
       </c>
       <c r="F86" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4483,16 +4539,16 @@
         <v>108</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>167</v>
+        <v>362</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F87" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -4503,13 +4559,13 @@
         <v>108</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>269</v>
+        <v>163</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>262</v>
       </c>
       <c r="F88" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4523,16 +4579,16 @@
         <v>108</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>315</v>
+        <v>364</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="F89" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4543,13 +4599,16 @@
         <v>108</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>194</v>
+        <v>167</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="F90" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4560,13 +4619,13 @@
         <v>108</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>368</v>
+        <v>267</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="F91" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4580,16 +4639,16 @@
         <v>108</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>368</v>
+        <v>312</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>276</v>
+        <v>195</v>
       </c>
       <c r="F92" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -4600,16 +4659,13 @@
         <v>108</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>277</v>
+        <v>194</v>
       </c>
       <c r="F93" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -4620,16 +4676,16 @@
         <v>108</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="F94" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -4640,16 +4696,16 @@
         <v>108</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>260</v>
+        <v>365</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="F95" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -4660,16 +4716,16 @@
         <v>108</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="F96" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -4680,16 +4736,16 @@
         <v>108</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>268</v>
+        <v>353</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="F97" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -4700,16 +4756,16 @@
         <v>108</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>193</v>
+        <v>258</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>314</v>
+        <v>259</v>
       </c>
       <c r="F98" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -4720,13 +4776,16 @@
         <v>108</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>304</v>
+        <v>265</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="F99" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -4737,13 +4796,16 @@
         <v>108</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>311</v>
+        <v>266</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="F100" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -4754,13 +4816,16 @@
         <v>108</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>312</v>
+        <v>193</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="F101" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>14</v>
       </c>
@@ -4771,13 +4836,13 @@
         <v>108</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="F102" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>14</v>
       </c>
@@ -4785,16 +4850,13 @@
         <v>29</v>
       </c>
       <c r="C103" t="s">
-        <v>212</v>
+        <v>108</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
       <c r="F103" t="s">
-        <v>144</v>
+        <v>306</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4805,134 +4867,225 @@
         <v>29</v>
       </c>
       <c r="C104" t="s">
+        <v>108</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F104" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>14</v>
+      </c>
+      <c r="B105" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" t="s">
+        <v>108</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F105" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>14</v>
+      </c>
+      <c r="B106" t="s">
+        <v>29</v>
+      </c>
+      <c r="C106" t="s">
+        <v>108</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F106" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" t="s">
+        <v>29</v>
+      </c>
+      <c r="C107" t="s">
+        <v>211</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F107" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>14</v>
+      </c>
+      <c r="B108" t="s">
+        <v>29</v>
+      </c>
+      <c r="C108" t="s">
+        <v>211</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F108" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>14</v>
+      </c>
+      <c r="B109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C109" t="s">
+        <v>211</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F109" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110" t="s">
+        <v>29</v>
+      </c>
+      <c r="C110" t="s">
+        <v>211</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F110" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>14</v>
+      </c>
+      <c r="B111" t="s">
+        <v>29</v>
+      </c>
+      <c r="C111" t="s">
+        <v>211</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F111" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>14</v>
+      </c>
+      <c r="B112" t="s">
+        <v>29</v>
+      </c>
+      <c r="C112" t="s">
+        <v>211</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F112" t="s">
         <v>212</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="F104" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>14</v>
-      </c>
-      <c r="B105" t="s">
-        <v>29</v>
-      </c>
-      <c r="C105" t="s">
-        <v>212</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="F105" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>14</v>
-      </c>
-      <c r="B106" t="s">
-        <v>29</v>
-      </c>
-      <c r="C106" t="s">
-        <v>212</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F106" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>14</v>
-      </c>
-      <c r="B107" t="s">
-        <v>29</v>
-      </c>
-      <c r="C107" t="s">
-        <v>212</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="F107" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>14</v>
-      </c>
-      <c r="B108" t="s">
-        <v>29</v>
-      </c>
-      <c r="C108" t="s">
-        <v>212</v>
-      </c>
-      <c r="D108" s="2" t="s">
+    </row>
+    <row r="113" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B113" t="s">
+        <v>29</v>
+      </c>
+      <c r="C113" t="s">
+        <v>211</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F113" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>14</v>
+      </c>
+      <c r="B114" t="s">
+        <v>29</v>
+      </c>
+      <c r="C114" t="s">
+        <v>211</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F114" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>14</v>
+      </c>
+      <c r="B115" t="s">
+        <v>29</v>
+      </c>
+      <c r="C115" t="s">
+        <v>211</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F115" t="s">
         <v>280</v>
       </c>
-      <c r="E108" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F108" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>14</v>
-      </c>
-      <c r="B109" t="s">
-        <v>29</v>
-      </c>
-      <c r="C109" t="s">
-        <v>212</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="F109" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>14</v>
-      </c>
-      <c r="B110" t="s">
-        <v>29</v>
-      </c>
-      <c r="C110" t="s">
-        <v>212</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F110" t="s">
-        <v>283</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F135">
+  <conditionalFormatting sqref="B3:F140">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -5236,13 +5389,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" t="s">
         <v>214</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>215</v>
-      </c>
-      <c r="D9" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: dialogue choice reflecting PC finding urn early
Fix: pressing switch dialogue not progressing quest
Updated: extended distance Aryasi will recognise urn
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F366F1DF-D092-4899-A68C-AD69834F01C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA34276-32C5-4B2F-8A71-81B54B7F5D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="2" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -825,12 +825,6 @@
     <t>Whenever I asked my parents they always denied it, but every time my mother expressed missing grandmother she would come to the tomb. Once, I followed her and watched as she prayed at the shrine, then after a while, she reached out to it and I heard something heavy move elsewhere in the tomb. But that was when she caught me and dragged me out. I investigated the shrine a few other times when I was alone, but found nothing. Maybe some fresh hands and eyes could reveal something?</t>
   </si>
   <si>
-    <t>If PCFoundSecret: Choice "I have already found a switch hidden on the shrine and pressed it.", 4, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3 ELSE Choice "I could take a look for you.", 1, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3</t>
-  </si>
-  <si>
-    <t>set tlvoat_hasPCMentionSecret to 1</t>
-  </si>
-  <si>
     <t>tlvoat_Estranged_Spirits.Journal &lt;= 45, tlvoat_hasPCMentionSecret = 1</t>
   </si>
   <si>
@@ -1314,6 +1308,17 @@
   </si>
   <si>
     <t>Aryasi Othral is grateful for my help. I turned down her reward.</t>
+  </si>
+  <si>
+    <t>if ( GetJournalIndex "tlvoat_Estranged_Spirits" == 30 )
+    Journal "tlvoat_Estranged_Spirits", 40
+endif
+if ( GetJournalIndex "tlvoat_Estranged_Spirits" == 35 )
+    Journal "tlvoat_Estranged_Spirits", 40
+endifset tlvoat_hasPCMentionSecret to 1</t>
+  </si>
+  <si>
+    <t>if tlvoat_hasPCFoundUrn: Choice "The shrine does have a switch, and the hidden section has your grandmother's urn.", 5, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3; ELSEIF PCFoundSecret: Choice "I have already found a switch hidden on the shrine and pressed it.", 4, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3 ELSE Choice "I could take a look for you.", 1, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3</t>
   </si>
 </sst>
 </file>
@@ -2212,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A78730-2022-40E5-AA7E-D04FFF65D365}">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2336,7 +2341,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D8">
         <v>35</v>
@@ -2429,7 +2434,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D14">
         <v>71</v>
@@ -2443,7 +2448,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D15">
         <v>100</v>
@@ -2460,7 +2465,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D16">
         <v>101</v>
@@ -2477,7 +2482,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D17">
         <v>105</v>
@@ -2491,7 +2496,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D18">
         <v>150</v>
@@ -2585,7 +2590,7 @@
         <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D23">
         <v>600</v>
@@ -2602,7 +2607,7 @@
         <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D24">
         <v>700</v>
@@ -2619,7 +2624,7 @@
         <v>27</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D25">
         <v>701</v>
@@ -2629,7 +2634,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F4 F6:F8 F15 F18:F20 F22:F25 B5:E41">
+  <conditionalFormatting sqref="B3:F4 B5:E41 F6:F8 F15 F18:F20 F22:F25">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>
@@ -2923,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
   <dimension ref="A2:F115"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3021,7 +3026,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F6" t="s">
         <v>141</v>
@@ -3163,7 +3168,7 @@
         <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -3177,13 +3182,13 @@
         <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3197,13 +3202,13 @@
         <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3217,13 +3222,13 @@
         <v>110</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F17" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3237,13 +3242,13 @@
         <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F18" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3274,10 +3279,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3311,7 +3316,7 @@
         <v>173</v>
       </c>
       <c r="F22" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3325,10 +3330,10 @@
         <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F23" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3345,7 +3350,7 @@
         <v>174</v>
       </c>
       <c r="F24" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3396,13 +3401,13 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F27" t="s">
         <v>397</v>
-      </c>
-      <c r="F27" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3416,10 +3421,10 @@
         <v>110</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F28" t="s">
         <v>210</v>
@@ -3456,13 +3461,13 @@
         <v>110</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F30" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3479,7 +3484,7 @@
         <v>239</v>
       </c>
       <c r="F31" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3493,13 +3498,13 @@
         <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="F32" t="s">
         <v>398</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="F32" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -3513,10 +3518,10 @@
         <v>110</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F33" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3530,13 +3535,13 @@
         <v>110</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F34" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -3570,7 +3575,7 @@
         <v>243</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F36" t="s">
         <v>144</v>
@@ -3590,7 +3595,7 @@
         <v>182</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F37" t="s">
         <v>146</v>
@@ -3761,13 +3766,13 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F46" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3781,13 +3786,13 @@
         <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3801,13 +3806,13 @@
         <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F48" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3821,13 +3826,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F49" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3844,7 +3849,7 @@
         <v>242</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F50" t="s">
         <v>145</v>
@@ -3861,10 +3866,10 @@
         <v>103</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F51" t="s">
         <v>150</v>
@@ -3884,10 +3889,10 @@
         <v>248</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F52" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3904,10 +3909,10 @@
         <v>249</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F53" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3941,10 +3946,10 @@
         <v>246</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F55" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3961,10 +3966,10 @@
         <v>247</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F56" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3978,13 +3983,13 @@
         <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F57" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3998,13 +4003,13 @@
         <v>103</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F58" t="s">
         <v>322</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="F58" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4018,13 +4023,13 @@
         <v>103</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F59" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4041,7 +4046,7 @@
         <v>252</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F60" t="s">
         <v>251</v>
@@ -4058,7 +4063,7 @@
         <v>103</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F61" t="s">
         <v>191</v>
@@ -4075,7 +4080,7 @@
         <v>103</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -4092,7 +4097,7 @@
         <v>254</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F63" t="s">
         <v>144</v>
@@ -4109,13 +4114,13 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F64" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4129,10 +4134,10 @@
         <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F65" t="s">
         <v>146</v>
@@ -4149,10 +4154,10 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F66" t="s">
         <v>147</v>
@@ -4169,10 +4174,10 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="F67" t="s">
         <v>148</v>
@@ -4189,10 +4194,10 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F68" t="s">
         <v>187</v>
@@ -4209,13 +4214,13 @@
         <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F69" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -4229,10 +4234,10 @@
         <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F70" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4246,13 +4251,13 @@
         <v>160</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F71" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -4266,10 +4271,10 @@
         <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F72" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -4286,7 +4291,7 @@
         <v>255</v>
       </c>
       <c r="F73" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
@@ -4300,13 +4305,13 @@
         <v>160</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F74" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4320,13 +4325,13 @@
         <v>160</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E75" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F75" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
@@ -4340,13 +4345,13 @@
         <v>160</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F76" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -4360,13 +4365,13 @@
         <v>160</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F77" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -4380,13 +4385,13 @@
         <v>160</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F78" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -4400,10 +4405,10 @@
         <v>160</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F79" t="s">
         <v>253</v>
@@ -4437,7 +4442,7 @@
         <v>160</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F81" t="s">
         <v>192</v>
@@ -4454,10 +4459,10 @@
         <v>160</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F82" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4471,10 +4476,10 @@
         <v>160</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F83" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4488,10 +4493,10 @@
         <v>160</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F84" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4505,10 +4510,10 @@
         <v>160</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F85" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4522,7 +4527,7 @@
         <v>160</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F86" t="s">
         <v>257</v>
@@ -4539,7 +4544,7 @@
         <v>108</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>168</v>
@@ -4562,7 +4567,7 @@
         <v>163</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F88" t="s">
         <v>146</v>
@@ -4579,13 +4584,13 @@
         <v>108</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>172</v>
       </c>
       <c r="F89" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4608,7 +4613,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4619,10 +4624,10 @@
         <v>108</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>260</v>
+        <v>420</v>
       </c>
       <c r="F91" t="s">
         <v>148</v>
@@ -4639,7 +4644,7 @@
         <v>108</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>195</v>
@@ -4676,10 +4681,10 @@
         <v>108</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F94" t="s">
         <v>153</v>
@@ -4696,10 +4701,10 @@
         <v>108</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F95" t="s">
         <v>184</v>
@@ -4716,16 +4721,16 @@
         <v>108</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F96" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -4736,16 +4741,16 @@
         <v>108</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>259</v>
+        <v>421</v>
       </c>
       <c r="F97" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -4759,7 +4764,7 @@
         <v>258</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>259</v>
+        <v>421</v>
       </c>
       <c r="F98" t="s">
         <v>169</v>
@@ -4776,13 +4781,13 @@
         <v>108</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F99" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4796,13 +4801,13 @@
         <v>108</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F100" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="216" x14ac:dyDescent="0.3">
@@ -4819,7 +4824,7 @@
         <v>193</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F101" t="s">
         <v>237</v>
@@ -4836,10 +4841,10 @@
         <v>108</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F102" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -4853,10 +4858,10 @@
         <v>108</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F103" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4870,10 +4875,10 @@
         <v>108</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F104" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -4887,10 +4892,10 @@
         <v>108</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F105" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -4904,10 +4909,10 @@
         <v>108</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F106" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -4924,7 +4929,7 @@
         <v>217</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F107" t="s">
         <v>144</v>
@@ -4944,7 +4949,7 @@
         <v>219</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F108" t="s">
         <v>218</v>
@@ -4961,13 +4966,13 @@
         <v>211</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F109" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4981,13 +4986,13 @@
         <v>211</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F110" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5001,13 +5006,13 @@
         <v>211</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F111" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5021,7 +5026,7 @@
         <v>211</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>216</v>
@@ -5041,13 +5046,13 @@
         <v>211</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>216</v>
       </c>
       <c r="F113" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -5061,10 +5066,10 @@
         <v>211</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F114" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5078,10 +5083,10 @@
         <v>211</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F115" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: more lines covering missed scenarios
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA34276-32C5-4B2F-8A71-81B54B7F5D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BB2194-80C7-4E96-AC79-04E7E6BF223E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="436">
   <si>
     <t>Name</t>
   </si>
@@ -1168,9 +1168,6 @@
   </si>
   <si>
     <t>Your pay, right, I had forgotten. Here's your 70 gold.</t>
-  </si>
-  <si>
-    <t>Of course! You were here to help, not listen to me. It was 50 gold I promised right? Here you go.</t>
   </si>
   <si>
     <t>Well, while I can sense my family's spirits I can't work out who's who until they speak. I want to speak with my grandmother, but I don't know if she's here or in another part of the tomb. She should be in this room, and if she isn't then I can't help but wonder if there's a hidden section. Just as I once did many years ago.</t>
@@ -1319,6 +1316,51 @@
   </si>
   <si>
     <t>if tlvoat_hasPCFoundUrn: Choice "The shrine does have a switch, and the hidden section has your grandmother's urn.", 5, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3; ELSEIF PCFoundSecret: Choice "I have already found a switch hidden on the shrine and pressed it.", 4, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3 ELSE Choice "I could take a look for you.", 1, "I don't have the time right now.", 2, "I've helped enough, search for it yourself.", 3</t>
+  </si>
+  <si>
+    <t>Your pay, right, I had forgotten. Here's your 70 gold, and I hope my family's heirlooms cover the rest.</t>
+  </si>
+  <si>
+    <t>Choice = 2, tlvoat_hasHighReward1 = 1, PC has sword &amp; bracers</t>
+  </si>
+  <si>
+    <t>Choice = 2, PC has sword &amp; bracers</t>
+  </si>
+  <si>
+    <t>Choice = 2, tlvoat_hasHighReward1 = 1, PC has sword</t>
+  </si>
+  <si>
+    <t>Choice = 2, PC has sword</t>
+  </si>
+  <si>
+    <t>Choice = 2, PC has bracers</t>
+  </si>
+  <si>
+    <t>Of course! You were here to help, not listen to me. It was 50 gold I promised right? Here you go. That and the heirloom's should be enough.</t>
+  </si>
+  <si>
+    <t>Of course! You were here to help, not listen to me. It was 50 gold I promised right? Here you go. That and the sword should be enough.</t>
+  </si>
+  <si>
+    <t>Of course! You were here to help, not listen to me. It was 50 gold I promised right? Here you go. That and the bracers should be enough.</t>
+  </si>
+  <si>
+    <t>Choice = 2, tlvoat_hasHighReward1 = 1, PC has bracers</t>
+  </si>
+  <si>
+    <t>Your pay, right, I had forgotten. I see that you have the bracers, and so here's your 70 gold.</t>
+  </si>
+  <si>
+    <t>Your pay, right, I had forgotten. I see that you have the sword, and so here's your 70 gold.</t>
+  </si>
+  <si>
+    <t>Of course! You were here to help, not listen to me. It was 50 gold I promised right? Well, here you go, and thank you for not taking the heirlooms.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal == 101, tlvoat_isEarlyFinish == 1</t>
+  </si>
+  <si>
+    <t>Yeah, still got it. It's always been a… reminder of spending time with grandmother. In a way I'm glad that you refused it.</t>
   </si>
 </sst>
 </file>
@@ -2434,7 +2476,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D14">
         <v>71</v>
@@ -2448,7 +2490,7 @@
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D15">
         <v>100</v>
@@ -2465,7 +2507,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D16">
         <v>101</v>
@@ -2482,7 +2524,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D17">
         <v>105</v>
@@ -2926,10 +2968,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F115"/>
+  <dimension ref="A2:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3242,13 +3284,13 @@
         <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>343</v>
       </c>
       <c r="F18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3401,13 +3443,13 @@
         <v>110</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F27" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3498,13 +3540,13 @@
         <v>110</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>343</v>
       </c>
       <c r="F32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -4114,13 +4156,13 @@
         <v>160</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>373</v>
+        <v>421</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F64" t="s">
-        <v>331</v>
+        <v>422</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4134,16 +4176,16 @@
         <v>160</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>374</v>
+        <v>431</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F65" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -4154,16 +4196,16 @@
         <v>160</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>375</v>
+        <v>432</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="F66" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -4174,16 +4216,16 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="F67" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -4194,16 +4236,16 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>379</v>
+        <v>427</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="F68" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -4214,16 +4256,16 @@
         <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>380</v>
+        <v>429</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="F69" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -4234,10 +4276,13 @@
         <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>382</v>
+        <v>428</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>389</v>
       </c>
       <c r="F70" t="s">
-        <v>314</v>
+        <v>425</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4251,16 +4296,16 @@
         <v>160</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>401</v>
+        <v>433</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="F71" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4271,13 +4316,16 @@
         <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>292</v>
+        <v>374</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="F72" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -4288,13 +4336,16 @@
         <v>160</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>255</v>
+        <v>375</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="F73" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4305,16 +4356,16 @@
         <v>160</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>293</v>
+        <v>378</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
       <c r="F74" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4325,16 +4376,16 @@
         <v>160</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="E75" t="s">
-        <v>387</v>
+        <v>379</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>380</v>
       </c>
       <c r="F75" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4345,16 +4396,13 @@
         <v>160</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
       <c r="F76" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4365,16 +4413,16 @@
         <v>160</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="F77" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -4385,16 +4433,13 @@
         <v>160</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>408</v>
+        <v>292</v>
       </c>
       <c r="F78" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>14</v>
       </c>
@@ -4405,16 +4450,13 @@
         <v>160</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>371</v>
+        <v>255</v>
       </c>
       <c r="F79" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4425,13 +4467,16 @@
         <v>160</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>256</v>
+        <v>293</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>385</v>
       </c>
       <c r="F80" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4442,13 +4487,16 @@
         <v>160</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>358</v>
+        <v>387</v>
+      </c>
+      <c r="E81" t="s">
+        <v>386</v>
       </c>
       <c r="F81" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4459,13 +4507,16 @@
         <v>160</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>391</v>
+        <v>402</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>417</v>
       </c>
       <c r="F82" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4476,13 +4527,16 @@
         <v>160</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>297</v>
+        <v>405</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>410</v>
       </c>
       <c r="F83" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4493,13 +4547,16 @@
         <v>160</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>298</v>
+        <v>406</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>407</v>
       </c>
       <c r="F84" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4510,10 +4567,13 @@
         <v>160</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>413</v>
+        <v>370</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>371</v>
       </c>
       <c r="F85" t="s">
-        <v>412</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4527,13 +4587,13 @@
         <v>160</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>359</v>
+        <v>256</v>
       </c>
       <c r="F86" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4541,19 +4601,16 @@
         <v>29</v>
       </c>
       <c r="C87" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>168</v>
+        <v>358</v>
       </c>
       <c r="F87" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -4561,16 +4618,13 @@
         <v>29</v>
       </c>
       <c r="C88" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>260</v>
+        <v>390</v>
       </c>
       <c r="F88" t="s">
-        <v>146</v>
+        <v>391</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4581,19 +4635,16 @@
         <v>29</v>
       </c>
       <c r="C89" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>172</v>
+        <v>297</v>
       </c>
       <c r="F89" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -4601,19 +4652,16 @@
         <v>29</v>
       </c>
       <c r="C90" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>172</v>
+        <v>298</v>
       </c>
       <c r="F90" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4621,16 +4669,13 @@
         <v>29</v>
       </c>
       <c r="C91" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="F91" t="s">
-        <v>148</v>
+        <v>411</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4641,19 +4686,16 @@
         <v>29</v>
       </c>
       <c r="C92" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>195</v>
+        <v>359</v>
       </c>
       <c r="F92" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -4664,10 +4706,13 @@
         <v>108</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>194</v>
+        <v>360</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="F93" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4681,13 +4726,13 @@
         <v>108</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>363</v>
+        <v>163</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="F94" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4701,16 +4746,16 @@
         <v>108</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>272</v>
+        <v>172</v>
       </c>
       <c r="F95" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -4721,16 +4766,16 @@
         <v>108</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>269</v>
+        <v>167</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>273</v>
+        <v>172</v>
       </c>
       <c r="F96" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -4741,16 +4786,16 @@
         <v>108</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>351</v>
+        <v>265</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F97" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>14</v>
       </c>
@@ -4761,16 +4806,16 @@
         <v>108</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>258</v>
+        <v>310</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>421</v>
+        <v>195</v>
       </c>
       <c r="F98" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -4781,16 +4826,13 @@
         <v>108</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>262</v>
+        <v>194</v>
       </c>
       <c r="F99" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -4801,16 +4843,16 @@
         <v>108</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>264</v>
+        <v>363</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F100" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -4821,13 +4863,13 @@
         <v>108</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>193</v>
+        <v>363</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>309</v>
+        <v>272</v>
       </c>
       <c r="F101" t="s">
-        <v>237</v>
+        <v>184</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4841,13 +4883,16 @@
         <v>108</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>299</v>
+        <v>269</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="F102" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>14</v>
       </c>
@@ -4858,13 +4903,16 @@
         <v>108</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>306</v>
+        <v>351</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>420</v>
       </c>
       <c r="F103" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>14</v>
       </c>
@@ -4875,13 +4923,16 @@
         <v>108</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>307</v>
+        <v>258</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>420</v>
       </c>
       <c r="F104" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>14</v>
       </c>
@@ -4892,13 +4943,16 @@
         <v>108</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>414</v>
+        <v>263</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="F105" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>14</v>
       </c>
@@ -4909,13 +4963,16 @@
         <v>108</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>274</v>
+        <v>264</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="F106" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>14</v>
       </c>
@@ -4923,16 +4980,16 @@
         <v>29</v>
       </c>
       <c r="C107" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>276</v>
+        <v>309</v>
       </c>
       <c r="F107" t="s">
-        <v>144</v>
+        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4943,19 +5000,16 @@
         <v>29</v>
       </c>
       <c r="C108" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>344</v>
+        <v>299</v>
       </c>
       <c r="F108" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>14</v>
       </c>
@@ -4963,16 +5017,13 @@
         <v>29</v>
       </c>
       <c r="C109" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
       <c r="F109" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4983,19 +5034,16 @@
         <v>29</v>
       </c>
       <c r="C110" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="F110" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>14</v>
       </c>
@@ -5003,19 +5051,16 @@
         <v>29</v>
       </c>
       <c r="C111" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>344</v>
+        <v>413</v>
       </c>
       <c r="F111" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>14</v>
       </c>
@@ -5023,19 +5068,16 @@
         <v>29</v>
       </c>
       <c r="C112" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>216</v>
+        <v>274</v>
       </c>
       <c r="F112" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>14</v>
       </c>
@@ -5046,16 +5088,16 @@
         <v>211</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>416</v>
+        <v>217</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>216</v>
+        <v>276</v>
       </c>
       <c r="F113" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>14</v>
       </c>
@@ -5066,13 +5108,16 @@
         <v>211</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>332</v>
+        <v>219</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>344</v>
       </c>
       <c r="F114" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>14</v>
       </c>
@@ -5083,14 +5128,148 @@
         <v>211</v>
       </c>
       <c r="D115" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F115" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>14</v>
+      </c>
+      <c r="B116" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" t="s">
+        <v>211</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F116" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>14</v>
+      </c>
+      <c r="B117" t="s">
+        <v>29</v>
+      </c>
+      <c r="C117" t="s">
+        <v>211</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F117" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>14</v>
+      </c>
+      <c r="B118" t="s">
+        <v>29</v>
+      </c>
+      <c r="C118" t="s">
+        <v>211</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F118" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>14</v>
+      </c>
+      <c r="B119" t="s">
+        <v>29</v>
+      </c>
+      <c r="C119" t="s">
+        <v>211</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F119" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>14</v>
+      </c>
+      <c r="B120" t="s">
+        <v>29</v>
+      </c>
+      <c r="C120" t="s">
+        <v>211</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F120" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>14</v>
+      </c>
+      <c r="B121" t="s">
+        <v>29</v>
+      </c>
+      <c r="C121" t="s">
+        <v>211</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="F121" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>14</v>
+      </c>
+      <c r="B122" t="s">
+        <v>29</v>
+      </c>
+      <c r="C122" t="s">
+        <v>211</v>
+      </c>
+      <c r="D122" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F115" t="s">
+      <c r="F122" t="s">
         <v>278</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F140">
+  <conditionalFormatting sqref="B3:F147">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update: finished sword, decal and icon assets
* Update: adjusted sword stats
* Update: fixed dialogue choice missing 'your'
* Update: slightly darkened the tomb
* Update: 4 more lines to Aryasi to cover diff heirloom scenarios
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BB2194-80C7-4E96-AC79-04E7E6BF223E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E3DC6-5D98-4BAF-AD2E-878C0DC9CF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="444">
   <si>
     <t>Name</t>
   </si>
@@ -1361,6 +1361,30 @@
   </si>
   <si>
     <t>Yeah, still got it. It's always been a… reminder of spending time with grandmother. In a way I'm glad that you refused it.</t>
+  </si>
+  <si>
+    <t>Right, your gold. Here's the 70 I promised you. I hope that and the bracers are enough.</t>
+  </si>
+  <si>
+    <t>By the way, here's your gold. I hope that and the bracers are enough to satisfy you.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits &gt;= 30, tlvoat_hasPCReceivedReward1 = 0, PC has bracers</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits &gt;= 30, tlvoat_hasPCReceivedReward1 = 0, PC has sword</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits &gt;= 30, tlvoat_hasPCReceivedReward1 = 0, tlvoat_hasHighReward1 = 1, PC has bracers</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits &gt;= 30, tlvoat_hasPCReceivedReward1 = 0, tlvoat_hasHighReward1 = 1, PC has sword</t>
+  </si>
+  <si>
+    <t>Right, your gold. Here's the 70 I promised you. I hope that and the sword are enough. It's good that it's put to use once more rather than collecting dust in here.</t>
+  </si>
+  <si>
+    <t>By the way, here's your gold. I hope that and the sword are enough to satisfy you. It's good that it's put to use once more rather than collecting dust in here.</t>
   </si>
 </sst>
 </file>
@@ -2968,10 +2992,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F122"/>
+  <dimension ref="A2:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4045,13 +4069,13 @@
         <v>103</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>320</v>
+        <v>436</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>321</v>
       </c>
       <c r="F58" t="s">
-        <v>322</v>
+        <v>440</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4065,13 +4089,13 @@
         <v>103</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>330</v>
+        <v>442</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>291</v>
+        <v>321</v>
       </c>
       <c r="F59" t="s">
-        <v>329</v>
+        <v>441</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4085,16 +4109,16 @@
         <v>103</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>252</v>
+        <v>320</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>291</v>
+        <v>321</v>
       </c>
       <c r="F60" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -4105,13 +4129,16 @@
         <v>103</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>357</v>
+        <v>330</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>291</v>
       </c>
       <c r="F61" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -4122,90 +4149,87 @@
         <v>103</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F62" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F63" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F64" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" t="s">
+        <v>103</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F65" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" t="s">
+        <v>103</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>14</v>
-      </c>
-      <c r="B63" t="s">
-        <v>29</v>
-      </c>
-      <c r="C63" t="s">
-        <v>160</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="F63" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B64" t="s">
-        <v>29</v>
-      </c>
-      <c r="C64" t="s">
-        <v>160</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="F64" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>14</v>
-      </c>
-      <c r="B65" t="s">
-        <v>29</v>
-      </c>
-      <c r="C65" t="s">
-        <v>160</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="F65" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>14</v>
-      </c>
-      <c r="B66" t="s">
-        <v>29</v>
-      </c>
-      <c r="C66" t="s">
-        <v>160</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="F66" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -4216,13 +4240,13 @@
         <v>160</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>373</v>
+        <v>254</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="F67" t="s">
-        <v>331</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4236,13 +4260,13 @@
         <v>160</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F68" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4256,13 +4280,13 @@
         <v>160</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F69" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4276,13 +4300,13 @@
         <v>160</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F70" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -4296,16 +4320,16 @@
         <v>160</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>433</v>
+        <v>373</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F71" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4316,16 +4340,16 @@
         <v>160</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>374</v>
+        <v>427</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>349</v>
+        <v>389</v>
       </c>
       <c r="F72" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -4336,16 +4360,16 @@
         <v>160</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>375</v>
+        <v>429</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="F73" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4356,16 +4380,16 @@
         <v>160</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>378</v>
+        <v>428</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="F74" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -4376,16 +4400,16 @@
         <v>160</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>379</v>
+        <v>433</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="F75" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -4396,13 +4420,16 @@
         <v>160</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>381</v>
+        <v>374</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="F76" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4413,16 +4440,16 @@
         <v>160</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>400</v>
+        <v>375</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>401</v>
+        <v>377</v>
       </c>
       <c r="F77" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -4433,10 +4460,13 @@
         <v>160</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>292</v>
+        <v>378</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>399</v>
       </c>
       <c r="F78" t="s">
-        <v>347</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -4450,13 +4480,16 @@
         <v>160</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>255</v>
+        <v>379</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>380</v>
       </c>
       <c r="F79" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -4467,16 +4500,13 @@
         <v>160</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F80" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4487,16 +4517,16 @@
         <v>160</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E81" t="s">
-        <v>386</v>
+        <v>400</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="F81" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -4507,16 +4537,13 @@
         <v>160</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>417</v>
+        <v>292</v>
       </c>
       <c r="F82" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4527,16 +4554,13 @@
         <v>160</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>410</v>
+        <v>255</v>
       </c>
       <c r="F83" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -4547,16 +4571,16 @@
         <v>160</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>406</v>
+        <v>293</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
       <c r="F84" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -4567,16 +4591,16 @@
         <v>160</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>371</v>
+        <v>387</v>
+      </c>
+      <c r="E85" t="s">
+        <v>386</v>
       </c>
       <c r="F85" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -4587,13 +4611,16 @@
         <v>160</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>256</v>
+        <v>402</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>417</v>
       </c>
       <c r="F86" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -4604,13 +4631,16 @@
         <v>160</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>358</v>
+        <v>405</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>410</v>
       </c>
       <c r="F87" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -4621,13 +4651,16 @@
         <v>160</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>390</v>
+        <v>406</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>407</v>
       </c>
       <c r="F88" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -4638,10 +4671,13 @@
         <v>160</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>297</v>
+        <v>370</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>371</v>
       </c>
       <c r="F89" t="s">
-        <v>296</v>
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4655,13 +4691,13 @@
         <v>160</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>298</v>
+        <v>256</v>
       </c>
       <c r="F90" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -4672,13 +4708,13 @@
         <v>160</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>412</v>
+        <v>358</v>
       </c>
       <c r="F91" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -4689,13 +4725,13 @@
         <v>160</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>359</v>
+        <v>390</v>
       </c>
       <c r="F92" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -4703,16 +4739,13 @@
         <v>29</v>
       </c>
       <c r="C93" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>168</v>
+        <v>297</v>
       </c>
       <c r="F93" t="s">
-        <v>144</v>
+        <v>296</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4723,16 +4756,13 @@
         <v>29</v>
       </c>
       <c r="C94" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>260</v>
+        <v>298</v>
       </c>
       <c r="F94" t="s">
-        <v>146</v>
+        <v>295</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4743,19 +4773,16 @@
         <v>29</v>
       </c>
       <c r="C95" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>172</v>
+        <v>412</v>
       </c>
       <c r="F95" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -4763,19 +4790,16 @@
         <v>29</v>
       </c>
       <c r="C96" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>172</v>
+        <v>359</v>
       </c>
       <c r="F96" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -4786,13 +4810,13 @@
         <v>108</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>265</v>
+        <v>360</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>419</v>
+        <v>168</v>
       </c>
       <c r="F97" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4806,16 +4830,16 @@
         <v>108</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>310</v>
+        <v>163</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>195</v>
+        <v>260</v>
       </c>
       <c r="F98" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -4826,13 +4850,16 @@
         <v>108</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>194</v>
+        <v>362</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="F99" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -4843,16 +4870,16 @@
         <v>108</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>363</v>
+        <v>167</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>271</v>
+        <v>172</v>
       </c>
       <c r="F100" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -4863,13 +4890,13 @@
         <v>108</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>363</v>
+        <v>265</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>272</v>
+        <v>419</v>
       </c>
       <c r="F101" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4883,16 +4910,16 @@
         <v>108</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>269</v>
+        <v>310</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>273</v>
+        <v>195</v>
       </c>
       <c r="F102" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>14</v>
       </c>
@@ -4903,16 +4930,13 @@
         <v>108</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>420</v>
+        <v>194</v>
       </c>
       <c r="F103" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>14</v>
       </c>
@@ -4923,16 +4947,16 @@
         <v>108</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>258</v>
+        <v>363</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>420</v>
+        <v>271</v>
       </c>
       <c r="F104" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>14</v>
       </c>
@@ -4943,16 +4967,16 @@
         <v>108</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>263</v>
+        <v>363</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="F105" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>14</v>
       </c>
@@ -4963,16 +4987,16 @@
         <v>108</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="F106" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>14</v>
       </c>
@@ -4983,16 +5007,16 @@
         <v>108</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>193</v>
+        <v>351</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>309</v>
+        <v>420</v>
       </c>
       <c r="F107" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>14</v>
       </c>
@@ -5003,13 +5027,16 @@
         <v>108</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>299</v>
+        <v>258</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>420</v>
       </c>
       <c r="F108" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>14</v>
       </c>
@@ -5020,13 +5047,16 @@
         <v>108</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>306</v>
+        <v>263</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="F109" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>14</v>
       </c>
@@ -5037,13 +5067,16 @@
         <v>108</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>307</v>
+        <v>264</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="F110" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>14</v>
       </c>
@@ -5054,13 +5087,16 @@
         <v>108</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>413</v>
+        <v>193</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="F111" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>14</v>
       </c>
@@ -5071,13 +5107,13 @@
         <v>108</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
       <c r="F112" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>14</v>
       </c>
@@ -5085,16 +5121,13 @@
         <v>29</v>
       </c>
       <c r="C113" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>276</v>
+        <v>306</v>
       </c>
       <c r="F113" t="s">
-        <v>144</v>
+        <v>304</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5105,19 +5138,16 @@
         <v>29</v>
       </c>
       <c r="C114" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>344</v>
+        <v>307</v>
       </c>
       <c r="F114" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>14</v>
       </c>
@@ -5125,19 +5155,16 @@
         <v>29</v>
       </c>
       <c r="C115" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>344</v>
+        <v>413</v>
       </c>
       <c r="F115" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>14</v>
       </c>
@@ -5145,19 +5172,16 @@
         <v>29</v>
       </c>
       <c r="C116" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>345</v>
+        <v>274</v>
       </c>
       <c r="F116" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>14</v>
       </c>
@@ -5168,16 +5192,16 @@
         <v>211</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>282</v>
+        <v>217</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>344</v>
+        <v>276</v>
       </c>
       <c r="F117" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>14</v>
       </c>
@@ -5188,16 +5212,16 @@
         <v>211</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>416</v>
+        <v>219</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>216</v>
+        <v>344</v>
       </c>
       <c r="F118" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>14</v>
       </c>
@@ -5208,16 +5232,16 @@
         <v>211</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>415</v>
+        <v>333</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>216</v>
+        <v>344</v>
       </c>
       <c r="F119" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>14</v>
       </c>
@@ -5228,10 +5252,13 @@
         <v>211</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>332</v>
+        <v>283</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="F120" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5245,13 +5272,16 @@
         <v>211</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>435</v>
+        <v>282</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>344</v>
       </c>
       <c r="F121" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>14</v>
       </c>
@@ -5262,14 +5292,88 @@
         <v>211</v>
       </c>
       <c r="D122" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F122" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>14</v>
+      </c>
+      <c r="B123" t="s">
+        <v>29</v>
+      </c>
+      <c r="C123" t="s">
+        <v>211</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F123" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>14</v>
+      </c>
+      <c r="B124" t="s">
+        <v>29</v>
+      </c>
+      <c r="C124" t="s">
+        <v>211</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F124" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>14</v>
+      </c>
+      <c r="B125" t="s">
+        <v>29</v>
+      </c>
+      <c r="C125" t="s">
+        <v>211</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="F125" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>14</v>
+      </c>
+      <c r="B126" t="s">
+        <v>29</v>
+      </c>
+      <c r="C126" t="s">
+        <v>211</v>
+      </c>
+      <c r="D126" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F126" t="s">
         <v>278</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:F147">
+  <conditionalFormatting sqref="B3:F151">
     <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3="No"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add: new family blade topic
* Add: new release screenshot
* Update: various readmes and descriptions
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\othral-ancestral-tomb\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E3DC6-5D98-4BAF-AD2E-878C0DC9CF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E1245F-2F1C-4BD1-A8A2-FBB4056FDE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="4" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="455">
   <si>
     <t>Name</t>
   </si>
@@ -1385,6 +1385,39 @@
   </si>
   <si>
     <t>By the way, here's your gold. I hope that and the sword are enough to satisfy you. It's good that it's put to use once more rather than collecting dust in here.</t>
+  </si>
+  <si>
+    <t>family blade</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 50; Player-&gt;AddItem Gold_001, 50; set tlvoat_hasPCReceivedReward1; AddTopic "family blade"</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 50; Player-&gt;AddItem Gold_001, 50; set tlvoat_hasPCReceivedReward1;  AddTopic "family blade"</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1;  AddTopic "family blade"</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 70; Player-&gt;AddItem Gold_001, 70; set tlvoat_hasPCReceivedReward1;  AddTopic "family blade"; Choice "So, your family. They don't like you very much?", 1, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
+  </si>
+  <si>
+    <t>RemoveItem Gold_001, 50; Player-&gt;AddItem Gold_001, 50; set tlvoat_hasPCReceivedReward1;  AddTopic "family blade"; Choice "So, your family. They don't like you very much?", 1, "Before I go, is there anything else I could help with?", 3, "[Leave] Good luck with your family.", 4</t>
+  </si>
+  <si>
+    <t>It has been in the family for as long as anyone could remember, and has been passed down from parent to firstborn every generation. Well, until this one. My younger brother Jathys received it instead due to my… transgressions. It's a fine blade and I hope it serves you as well as it has my family.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &gt;= 30</t>
+  </si>
+  <si>
+    <t>A fine blade and I think it suits you! Every generation has made some change to it. Putting their mark on it I suppose. Grandmother did something a little different given her expertise in magic and enhanced the blade's ability to hold powerful enchantments. She left it up for a future generation to decide what that enchantment should be.</t>
+  </si>
+  <si>
+    <t>tlvoat_Estranged_Spirits.Journal &gt;= 100, PC Enchant &gt;= 50</t>
+  </si>
+  <si>
+    <t>A fine blade and I think it suits you! Every generation has made some change to it. Putting their mark on it I suppose. Grandmother did something a little different given her expertise in magic and enhanced the blade's ability to hold powerful enchantments. She left it up for a future generation to decide what that enchantment should be. Though I suppose that's you now, given your skill as an enchanter.</t>
   </si>
 </sst>
 </file>
@@ -1918,8 +1951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B451BEBD-3E4F-477C-8824-662D4D8A357C}">
   <dimension ref="A2:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1958,7 +1991,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -2992,10 +3025,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FFBF93-1C76-46C0-825C-97FF26B47D4C}">
-  <dimension ref="A2:F126"/>
+  <dimension ref="A2:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4038,7 +4071,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -4052,7 +4085,7 @@
         <v>327</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>321</v>
+        <v>447</v>
       </c>
       <c r="F57" t="s">
         <v>328</v>
@@ -4078,7 +4111,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -4092,7 +4125,7 @@
         <v>442</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>321</v>
+        <v>447</v>
       </c>
       <c r="F59" t="s">
         <v>441</v>
@@ -4118,7 +4151,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -4132,7 +4165,7 @@
         <v>330</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>291</v>
+        <v>445</v>
       </c>
       <c r="F61" t="s">
         <v>329</v>
@@ -4158,7 +4191,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -4172,7 +4205,7 @@
         <v>443</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>291</v>
+        <v>446</v>
       </c>
       <c r="F63" t="s">
         <v>439</v>
@@ -4249,7 +4282,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -4263,7 +4296,7 @@
         <v>421</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>388</v>
+        <v>448</v>
       </c>
       <c r="F68" t="s">
         <v>422</v>
@@ -4289,7 +4322,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -4303,7 +4336,7 @@
         <v>432</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>388</v>
+        <v>448</v>
       </c>
       <c r="F70" t="s">
         <v>424</v>
@@ -4329,7 +4362,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4343,7 +4376,7 @@
         <v>427</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>389</v>
+        <v>449</v>
       </c>
       <c r="F72" t="s">
         <v>423</v>
@@ -4369,7 +4402,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -4383,7 +4416,7 @@
         <v>428</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>389</v>
+        <v>449</v>
       </c>
       <c r="F74" t="s">
         <v>425</v>
@@ -5370,6 +5403,57 @@
       </c>
       <c r="F126" t="s">
         <v>278</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>14</v>
+      </c>
+      <c r="B127" t="s">
+        <v>29</v>
+      </c>
+      <c r="C127" t="s">
+        <v>444</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="F127" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>14</v>
+      </c>
+      <c r="B128" t="s">
+        <v>29</v>
+      </c>
+      <c r="C128" t="s">
+        <v>444</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="F128" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>14</v>
+      </c>
+      <c r="B129" t="s">
+        <v>29</v>
+      </c>
+      <c r="C129" t="s">
+        <v>444</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="F129" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -5382,7 +5466,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D1:D1048576" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Dialogue entries are limited to 512 characters." sqref="D130:D1048576 D1:D129" xr:uid="{9A5A56BD-256F-439B-8B34-4997B504B9BF}">
       <formula1>512</formula1>
     </dataValidation>
   </dataValidations>
@@ -5394,7 +5478,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A1048576</xm:sqref>
+          <xm:sqref>A130:A1048576 A1:A129</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5568,7 +5652,7 @@
   <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>